<commit_message>
recrutiment, fixing (but unfinished) the country problem,
removed data from Spain
</commit_message>
<xml_diff>
--- a/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
+++ b/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
@@ -402,22 +402,22 @@
         <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>58.7912899899249</v>
+        <v>58.4807609927735</v>
       </c>
       <c r="C2" t="n">
-        <v>169.812788264165</v>
+        <v>169.724300119598</v>
       </c>
       <c r="D2" t="n">
-        <v>490.487333463712</v>
+        <v>492.578030143061</v>
       </c>
       <c r="E2" t="n">
-        <v>45.066502798915</v>
+        <v>45.3764559826106</v>
       </c>
       <c r="F2" t="n">
-        <v>207.959663090207</v>
+        <v>207.974661428798</v>
       </c>
       <c r="G2" t="n">
-        <v>959.631184730708</v>
+        <v>953.213706530961</v>
       </c>
     </row>
     <row r="3">
@@ -425,22 +425,22 @@
         <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>74.7651266350414</v>
+        <v>74.2828367059565</v>
       </c>
       <c r="C3" t="n">
-        <v>215.951625164131</v>
+        <v>215.585472158523</v>
       </c>
       <c r="D3" t="n">
-        <v>623.754770572032</v>
+        <v>625.677449419302</v>
       </c>
       <c r="E3" t="n">
-        <v>25.3901430258007</v>
+        <v>25.5638530321481</v>
       </c>
       <c r="F3" t="n">
-        <v>117.162976080425</v>
+        <v>117.167230539424</v>
       </c>
       <c r="G3" t="n">
-        <v>540.649296464109</v>
+        <v>537.014506186314</v>
       </c>
     </row>
     <row r="4">
@@ -448,22 +448,22 @@
         <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>62.2562403294813</v>
+        <v>61.9072142208721</v>
       </c>
       <c r="C4" t="n">
-        <v>179.820952372452</v>
+        <v>179.668636789625</v>
       </c>
       <c r="D4" t="n">
-        <v>519.394919143927</v>
+        <v>521.438728137095</v>
       </c>
       <c r="E4" t="n">
-        <v>38.7983976731105</v>
+        <v>39.063577026526</v>
       </c>
       <c r="F4" t="n">
-        <v>179.035452219164</v>
+        <v>179.040738866934</v>
       </c>
       <c r="G4" t="n">
-        <v>826.160230156507</v>
+        <v>820.6003805604</v>
       </c>
     </row>
     <row r="5">
@@ -471,22 +471,22 @@
         <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>54.7054863129487</v>
+        <v>54.434849178556</v>
       </c>
       <c r="C5" t="n">
-        <v>158.011351098795</v>
+        <v>157.98215553467</v>
       </c>
       <c r="D5" t="n">
-        <v>456.400057084531</v>
+        <v>458.499689886394</v>
       </c>
       <c r="E5" t="n">
-        <v>48.5732900501279</v>
+        <v>48.9056401316216</v>
       </c>
       <c r="F5" t="n">
-        <v>224.141755109756</v>
+        <v>224.150029526996</v>
       </c>
       <c r="G5" t="n">
-        <v>1034.30355102226</v>
+        <v>1027.35053874628</v>
       </c>
     </row>
     <row r="6">
@@ -494,22 +494,22 @@
         <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>52.6816356080482</v>
+        <v>52.3537623807752</v>
       </c>
       <c r="C6" t="n">
-        <v>152.165659818869</v>
+        <v>151.942374344323</v>
       </c>
       <c r="D6" t="n">
-        <v>439.515359780791</v>
+        <v>440.970888653227</v>
       </c>
       <c r="E6" t="n">
-        <v>30.6479497040554</v>
+        <v>30.9472008180977</v>
       </c>
       <c r="F6" t="n">
-        <v>116.278199409447</v>
+        <v>116.280889300707</v>
       </c>
       <c r="G6" t="n">
-        <v>441.159026573122</v>
+        <v>436.91335109882</v>
       </c>
     </row>
     <row r="7">
@@ -517,22 +517,22 @@
         <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>32.9052444087686</v>
+        <v>32.7515369763285</v>
       </c>
       <c r="C7" t="n">
-        <v>95.0435226463726</v>
+        <v>95.0523145865934</v>
       </c>
       <c r="D7" t="n">
-        <v>274.523753259962</v>
+        <v>275.863160705979</v>
       </c>
       <c r="E7" t="n">
-        <v>20.6569642290944</v>
+        <v>20.8563638204237</v>
       </c>
       <c r="F7" t="n">
-        <v>78.3724402127503</v>
+        <v>78.3656184891436</v>
       </c>
       <c r="G7" t="n">
-        <v>297.344726784686</v>
+        <v>294.450663311322</v>
       </c>
     </row>
     <row r="8">
@@ -540,22 +540,22 @@
         <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>41.380245487755</v>
+        <v>41.1456378537875</v>
       </c>
       <c r="C8" t="n">
-        <v>104.543629163951</v>
+        <v>104.385237633791</v>
       </c>
       <c r="D8" t="n">
-        <v>264.120482368908</v>
+        <v>264.822187824219</v>
       </c>
       <c r="E8" t="n">
-        <v>23.2388840812079</v>
+        <v>23.4652601292741</v>
       </c>
       <c r="F8" t="n">
-        <v>88.1682338734115</v>
+        <v>88.1682751064442</v>
       </c>
       <c r="G8" t="n">
-        <v>334.509929013448</v>
+        <v>331.283126307542</v>
       </c>
     </row>
     <row r="9">
@@ -563,22 +563,22 @@
         <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>30.3758395368435</v>
+        <v>30.1682710235373</v>
       </c>
       <c r="C9" t="n">
-        <v>76.7419445354221</v>
+        <v>76.5359903031052</v>
       </c>
       <c r="D9" t="n">
-        <v>193.881918685227</v>
+        <v>194.16949042611</v>
       </c>
       <c r="E9" t="n">
-        <v>25.7296505256324</v>
+        <v>25.9798026804227</v>
       </c>
       <c r="F9" t="n">
-        <v>97.6181918674637</v>
+        <v>97.6164072897283</v>
       </c>
       <c r="G9" t="n">
-        <v>370.363032097139</v>
+        <v>366.783500605059</v>
       </c>
     </row>
     <row r="10">
@@ -586,22 +586,22 @@
         <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>37.1694107157704</v>
+        <v>36.9055366902539</v>
       </c>
       <c r="C10" t="n">
-        <v>93.9053174844477</v>
+        <v>93.6282293424234</v>
       </c>
       <c r="D10" t="n">
-        <v>237.243703412104</v>
+        <v>237.531983435766</v>
       </c>
       <c r="E10" t="n">
-        <v>32.7035133091711</v>
+        <v>33.0224108461631</v>
       </c>
       <c r="F10" t="n">
-        <v>124.076999560271</v>
+        <v>124.078275208646</v>
       </c>
       <c r="G10" t="n">
-        <v>470.747643359844</v>
+        <v>466.211217905107</v>
       </c>
     </row>
     <row r="11">
@@ -609,22 +609,22 @@
         <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>30.0836944587184</v>
+        <v>29.9294526096988</v>
       </c>
       <c r="C11" t="n">
-        <v>76.0038651366757</v>
+        <v>75.930115216945</v>
       </c>
       <c r="D11" t="n">
-        <v>192.017224601213</v>
+        <v>192.632403674173</v>
       </c>
       <c r="E11" t="n">
-        <v>26.2966484882549</v>
+        <v>26.602571045345</v>
       </c>
       <c r="F11" t="n">
-        <v>89.5809532683459</v>
+        <v>89.5799642885223</v>
       </c>
       <c r="G11" t="n">
-        <v>305.162355273134</v>
+        <v>301.646408095472</v>
       </c>
     </row>
     <row r="12">
@@ -632,22 +632,22 @@
         <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>34.6356217607722</v>
+        <v>34.4504353375317</v>
       </c>
       <c r="C12" t="n">
-        <v>87.5039177399862</v>
+        <v>87.3997115338142</v>
       </c>
       <c r="D12" t="n">
-        <v>221.071117843145</v>
+        <v>221.730422311152</v>
       </c>
       <c r="E12" t="n">
-        <v>28.8969406978966</v>
+        <v>29.2325142233983</v>
       </c>
       <c r="F12" t="n">
-        <v>98.4389891134836</v>
+        <v>98.4358833487243</v>
       </c>
       <c r="G12" t="n">
-        <v>335.337732772171</v>
+        <v>331.467319457861</v>
       </c>
     </row>
     <row r="13">
@@ -655,22 +655,22 @@
         <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>21.5132043262992</v>
+        <v>21.4283094577875</v>
       </c>
       <c r="C13" t="n">
-        <v>54.35125936801</v>
+        <v>54.3629723955214</v>
       </c>
       <c r="D13" t="n">
-        <v>137.313779485535</v>
+        <v>137.917215238003</v>
       </c>
       <c r="E13" t="n">
-        <v>24.8309667230852</v>
+        <v>25.1181531080212</v>
       </c>
       <c r="F13" t="n">
-        <v>84.8793570638567</v>
+        <v>84.8781572436116</v>
       </c>
       <c r="G13" t="n">
-        <v>290.141956046992</v>
+        <v>286.816532493013</v>
       </c>
     </row>
     <row r="14">
@@ -678,22 +678,22 @@
         <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>15.4090912599705</v>
+        <v>15.3468279574416</v>
       </c>
       <c r="C14" t="n">
-        <v>38.929743007748</v>
+        <v>38.9344379337402</v>
       </c>
       <c r="D14" t="n">
-        <v>98.3526455311683</v>
+        <v>98.7754903762515</v>
       </c>
       <c r="E14" t="n">
-        <v>34.237241606093</v>
+        <v>34.6830817623644</v>
       </c>
       <c r="F14" t="n">
-        <v>108.989456122212</v>
+        <v>108.993736303878</v>
       </c>
       <c r="G14" t="n">
-        <v>346.952645381968</v>
+        <v>342.519578706242</v>
       </c>
     </row>
     <row r="15">
@@ -701,22 +701,22 @@
         <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>14.3729729979706</v>
+        <v>14.3142369999141</v>
       </c>
       <c r="C15" t="n">
-        <v>36.3120793840611</v>
+        <v>36.3147859341035</v>
       </c>
       <c r="D15" t="n">
-        <v>91.7393436542693</v>
+        <v>92.1295125578595</v>
       </c>
       <c r="E15" t="n">
-        <v>15.6423921268227</v>
+        <v>15.8616167601336</v>
       </c>
       <c r="F15" t="n">
-        <v>47.3962106283799</v>
+        <v>47.3950580231713</v>
       </c>
       <c r="G15" t="n">
-        <v>143.609798534443</v>
+        <v>141.618068258059</v>
       </c>
     </row>
     <row r="16">
@@ -724,22 +724,22 @@
         <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>27.3452635176201</v>
+        <v>27.2592720310957</v>
       </c>
       <c r="C16" t="n">
-        <v>63.1170942184757</v>
+        <v>63.1556723981053</v>
       </c>
       <c r="D16" t="n">
-        <v>145.684007763062</v>
+        <v>146.32228445084</v>
       </c>
       <c r="E16" t="n">
-        <v>41.1632408511598</v>
+        <v>41.699864569037</v>
       </c>
       <c r="F16" t="n">
-        <v>131.037403194219</v>
+        <v>131.044411620797</v>
       </c>
       <c r="G16" t="n">
-        <v>417.139192173218</v>
+        <v>411.815193994462</v>
       </c>
     </row>
     <row r="17">
@@ -747,22 +747,22 @@
         <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>44.0925621528954</v>
+        <v>44.010876899467</v>
       </c>
       <c r="C17" t="n">
-        <v>90.592761000659</v>
+        <v>90.7178936883747</v>
       </c>
       <c r="D17" t="n">
-        <v>186.132262336304</v>
+        <v>186.993234741817</v>
       </c>
       <c r="E17" t="n">
-        <v>18.5614116327734</v>
+        <v>18.8363050109327</v>
       </c>
       <c r="F17" t="n">
-        <v>54.2683646728034</v>
+        <v>54.2660377837805</v>
       </c>
       <c r="G17" t="n">
-        <v>158.665486360981</v>
+        <v>156.336545572048</v>
       </c>
     </row>
     <row r="18">
@@ -770,22 +770,22 @@
         <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>58.272087148107</v>
+        <v>58.0701850628363</v>
       </c>
       <c r="C18" t="n">
-        <v>119.726071842059</v>
+        <v>119.697793957349</v>
       </c>
       <c r="D18" t="n">
-        <v>245.989683573493</v>
+        <v>246.728366075509</v>
       </c>
       <c r="E18" t="n">
-        <v>34.5891042956604</v>
+        <v>35.1274971494151</v>
       </c>
       <c r="F18" t="n">
-        <v>98.1542859234716</v>
+        <v>98.1538494577097</v>
       </c>
       <c r="G18" t="n">
-        <v>278.534643822949</v>
+        <v>274.263154086603</v>
       </c>
     </row>
     <row r="19">
@@ -793,22 +793,22 @@
         <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>62.4328429532086</v>
+        <v>62.3537881993427</v>
       </c>
       <c r="C19" t="n">
-        <v>128.336664753114</v>
+        <v>128.589685906285</v>
       </c>
       <c r="D19" t="n">
-        <v>263.808257655304</v>
+        <v>265.185288640593</v>
       </c>
       <c r="E19" t="n">
-        <v>26.2879383201658</v>
+        <v>26.6961093662282</v>
       </c>
       <c r="F19" t="n">
-        <v>74.6007592171555</v>
+        <v>74.5976723190148</v>
       </c>
       <c r="G19" t="n">
-        <v>211.704440568732</v>
+        <v>208.45032656537</v>
       </c>
     </row>
     <row r="20">
@@ -816,22 +816,22 @@
         <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>54.5261132463118</v>
+        <v>54.4903082567314</v>
       </c>
       <c r="C20" t="n">
-        <v>113.408566026248</v>
+        <v>113.707141741954</v>
       </c>
       <c r="D20" t="n">
-        <v>235.877858926609</v>
+        <v>237.277315852358</v>
       </c>
       <c r="E20" t="n">
-        <v>19.411684002936</v>
+        <v>19.7133470609332</v>
       </c>
       <c r="F20" t="n">
-        <v>55.0871029392086</v>
+        <v>55.0855476424909</v>
       </c>
       <c r="G20" t="n">
-        <v>156.327957418635</v>
+        <v>153.927060163546</v>
       </c>
     </row>
     <row r="21">
@@ -839,22 +839,22 @@
         <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>83.1787174443065</v>
+        <v>83.5034643869908</v>
       </c>
       <c r="C21" t="n">
-        <v>173.002961473681</v>
+        <v>174.250074274867</v>
       </c>
       <c r="D21" t="n">
-        <v>359.827917504308</v>
+        <v>363.614714762982</v>
       </c>
       <c r="E21" t="n">
-        <v>34.8261374174017</v>
+        <v>35.4057192586615</v>
       </c>
       <c r="F21" t="n">
-        <v>94.7578875210414</v>
+        <v>94.7580583226359</v>
       </c>
       <c r="G21" t="n">
-        <v>257.825240273811</v>
+        <v>253.605626579086</v>
       </c>
     </row>
     <row r="22">
@@ -862,22 +862,22 @@
         <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>66.7624896487048</v>
+        <v>66.9650687249105</v>
       </c>
       <c r="C22" t="n">
-        <v>133.209749919796</v>
+        <v>134.028518760378</v>
       </c>
       <c r="D22" t="n">
-        <v>265.790529488421</v>
+        <v>268.253944678155</v>
       </c>
       <c r="E22" t="n">
-        <v>29.3958865767603</v>
+        <v>29.8705862081605</v>
       </c>
       <c r="F22" t="n">
-        <v>81.5540392999122</v>
+        <v>81.5550730014752</v>
       </c>
       <c r="G22" t="n">
-        <v>226.258232040866</v>
+        <v>222.66820898409</v>
       </c>
     </row>
     <row r="23">
@@ -885,22 +885,22 @@
         <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>49.9790339396649</v>
+        <v>50.052420407291</v>
       </c>
       <c r="C23" t="n">
-        <v>99.7220841728284</v>
+        <v>100.178375013979</v>
       </c>
       <c r="D23" t="n">
-        <v>198.973315166071</v>
+        <v>200.503926459058</v>
       </c>
       <c r="E23" t="n">
-        <v>21.7178989190813</v>
+        <v>22.0881534099729</v>
       </c>
       <c r="F23" t="n">
-        <v>58.1414555848454</v>
+        <v>58.1399822649144</v>
       </c>
       <c r="G23" t="n">
-        <v>155.65174467934</v>
+        <v>153.034863305429</v>
       </c>
     </row>
     <row r="24">
@@ -908,22 +908,22 @@
         <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>56.8949105054493</v>
+        <v>56.9865112781084</v>
       </c>
       <c r="C24" t="n">
-        <v>105.563000475372</v>
+        <v>106.026797288717</v>
       </c>
       <c r="D24" t="n">
-        <v>195.861931592213</v>
+        <v>197.269169337994</v>
       </c>
       <c r="E24" t="n">
-        <v>10.7989209548383</v>
+        <v>10.9779694613518</v>
       </c>
       <c r="F24" t="n">
-        <v>29.3513163620014</v>
+        <v>29.3487690378275</v>
       </c>
       <c r="G24" t="n">
-        <v>79.7764680179743</v>
+        <v>78.4617088859782</v>
       </c>
     </row>
     <row r="25">
@@ -931,22 +931,22 @@
         <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>24.5347543701856</v>
+        <v>24.5230903113008</v>
       </c>
       <c r="C25" t="n">
-        <v>46.8097430173014</v>
+        <v>46.9232929898931</v>
       </c>
       <c r="D25" t="n">
-        <v>89.3080895893731</v>
+        <v>89.784582492065</v>
       </c>
       <c r="E25" t="n">
-        <v>8.65804413239714</v>
+        <v>8.8012573705171</v>
       </c>
       <c r="F25" t="n">
-        <v>23.5324430532387</v>
+        <v>23.529494294838</v>
       </c>
       <c r="G25" t="n">
-        <v>63.9608516179505</v>
+        <v>62.9043190607534</v>
       </c>
     </row>
     <row r="26">
@@ -954,22 +954,22 @@
         <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>31.4111178829013</v>
+        <v>31.336249078421</v>
       </c>
       <c r="C26" t="n">
-        <v>58.2802894414797</v>
+        <v>58.3029572140669</v>
       </c>
       <c r="D26" t="n">
-        <v>108.133437022042</v>
+        <v>108.476123335582</v>
       </c>
       <c r="E26" t="n">
-        <v>3.61296744174355</v>
+        <v>3.6743961944365</v>
       </c>
       <c r="F26" t="n">
-        <v>9.67235305893532</v>
+        <v>9.67166994966412</v>
       </c>
       <c r="G26" t="n">
-        <v>25.8940649771114</v>
+        <v>25.4575703504345</v>
       </c>
     </row>
     <row r="27">
@@ -977,22 +977,22 @@
         <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>34.7419753943682</v>
+        <v>34.6194021106948</v>
       </c>
       <c r="C27" t="n">
-        <v>62.9782765782917</v>
+        <v>62.9239755529231</v>
       </c>
       <c r="D27" t="n">
-        <v>114.163437045515</v>
+        <v>114.370164069405</v>
       </c>
       <c r="E27" t="n">
-        <v>2.94628744162033</v>
+        <v>2.99627790421604</v>
       </c>
       <c r="F27" t="n">
-        <v>7.88756965235948</v>
+        <v>7.88674095921579</v>
       </c>
       <c r="G27" t="n">
-        <v>21.1159828270548</v>
+        <v>20.7593170414032</v>
       </c>
     </row>
     <row r="28">
@@ -1000,22 +1000,22 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>17.3135976261957</v>
+        <v>17.3542335999091</v>
       </c>
       <c r="C28" t="n">
-        <v>33.0325318672043</v>
+        <v>33.2061651890717</v>
       </c>
       <c r="D28" t="n">
-        <v>63.0226129263246</v>
+        <v>63.5377759678017</v>
       </c>
       <c r="E28" t="n">
-        <v>2.99309648377677</v>
+        <v>3.04261409028638</v>
       </c>
       <c r="F28" t="n">
-        <v>8.14315246333624</v>
+        <v>8.14236188865917</v>
       </c>
       <c r="G28" t="n">
-        <v>22.1546256195077</v>
+        <v>21.7898343853555</v>
       </c>
     </row>
     <row r="29">
@@ -1023,22 +1023,22 @@
         <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>40.7128251278122</v>
+        <v>40.7256400546774</v>
       </c>
       <c r="C29" t="n">
-        <v>73.8133205817068</v>
+        <v>74.0338555681433</v>
       </c>
       <c r="D29" t="n">
-        <v>133.825306354774</v>
+        <v>134.583809190623</v>
       </c>
       <c r="E29" t="n">
-        <v>3.43623589297067</v>
+        <v>3.49306140814516</v>
       </c>
       <c r="F29" t="n">
-        <v>9.34898271909118</v>
+        <v>9.34801788137999</v>
       </c>
       <c r="G29" t="n">
-        <v>25.4358200671444</v>
+        <v>25.0168628890502</v>
       </c>
     </row>
     <row r="30">
@@ -1046,22 +1046,22 @@
         <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>50.4463414719235</v>
+        <v>50.5398006115292</v>
       </c>
       <c r="C30" t="n">
-        <v>93.7289703203036</v>
+        <v>94.1640155466307</v>
       </c>
       <c r="D30" t="n">
-        <v>174.147809751354</v>
+        <v>175.443150083251</v>
       </c>
       <c r="E30" t="n">
-        <v>3.50743237236092</v>
+        <v>3.56705716968312</v>
       </c>
       <c r="F30" t="n">
-        <v>9.38699715381104</v>
+        <v>9.38623349626358</v>
       </c>
       <c r="G30" t="n">
-        <v>25.1225700771942</v>
+        <v>24.6986171108121</v>
       </c>
     </row>
     <row r="31">
@@ -1069,22 +1069,22 @@
         <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>27.1453203542315</v>
+        <v>27.0879611025853</v>
       </c>
       <c r="C31" t="n">
-        <v>51.8218197827335</v>
+        <v>51.8627433183124</v>
       </c>
       <c r="D31" t="n">
-        <v>98.9305327971746</v>
+        <v>99.2966629830416</v>
       </c>
       <c r="E31" t="n">
-        <v>1.50117622331256</v>
+        <v>1.52720277001036</v>
       </c>
       <c r="F31" t="n">
-        <v>3.96338445815958</v>
+        <v>3.96292319379576</v>
       </c>
       <c r="G31" t="n">
-        <v>10.4640721850217</v>
+        <v>10.2833497609606</v>
       </c>
     </row>
     <row r="32">
@@ -1092,22 +1092,22 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>23.2733425137692</v>
+        <v>23.2749612137037</v>
       </c>
       <c r="C32" t="n">
-        <v>43.1814347719063</v>
+        <v>43.3044511615176</v>
       </c>
       <c r="D32" t="n">
-        <v>80.1189733643642</v>
+        <v>80.5705097929938</v>
       </c>
       <c r="E32" t="n">
-        <v>5.38662543497848</v>
+        <v>5.47644873673987</v>
       </c>
       <c r="F32" t="n">
-        <v>14.6187699253752</v>
+        <v>14.6182953342461</v>
       </c>
       <c r="G32" t="n">
-        <v>39.6738991249184</v>
+        <v>39.0206443540005</v>
       </c>
     </row>
     <row r="33">
@@ -1115,22 +1115,22 @@
         <v>1991</v>
       </c>
       <c r="B33" t="n">
-        <v>10.5354742840948</v>
+        <v>10.5157556125317</v>
       </c>
       <c r="C33" t="n">
-        <v>20.1005820707605</v>
+        <v>20.1211949780063</v>
       </c>
       <c r="D33" t="n">
-        <v>38.3498064432981</v>
+        <v>38.5005607072559</v>
       </c>
       <c r="E33" t="n">
-        <v>1.21636825976748</v>
+        <v>1.23666252864004</v>
       </c>
       <c r="F33" t="n">
-        <v>3.2953889119175</v>
+        <v>3.295162313084</v>
       </c>
       <c r="G33" t="n">
-        <v>8.92787853808742</v>
+        <v>8.78015983997657</v>
       </c>
     </row>
     <row r="34">
@@ -1138,22 +1138,22 @@
         <v>1992</v>
       </c>
       <c r="B34" t="n">
-        <v>10.8052608830886</v>
+        <v>10.8027340214601</v>
       </c>
       <c r="C34" t="n">
-        <v>20.6153066601275</v>
+        <v>20.6703089678412</v>
       </c>
       <c r="D34" t="n">
-        <v>39.3318470779592</v>
+        <v>39.5512535972136</v>
       </c>
       <c r="E34" t="n">
-        <v>2.91861080329167</v>
+        <v>2.96835464130493</v>
       </c>
       <c r="F34" t="n">
-        <v>7.79070415312664</v>
+        <v>7.78986262226882</v>
       </c>
       <c r="G34" t="n">
-        <v>20.7958769744467</v>
+        <v>20.442961507842</v>
       </c>
     </row>
     <row r="35">
@@ -1161,22 +1161,22 @@
         <v>1993</v>
       </c>
       <c r="B35" t="n">
-        <v>11.7435829561703</v>
+        <v>11.7345933380748</v>
       </c>
       <c r="C35" t="n">
-        <v>21.7890816976685</v>
+        <v>21.8329095994255</v>
       </c>
       <c r="D35" t="n">
-        <v>40.4275324659942</v>
+        <v>40.6214282714028</v>
       </c>
       <c r="E35" t="n">
-        <v>2.59322160840707</v>
+        <v>2.63738612693718</v>
       </c>
       <c r="F35" t="n">
-        <v>6.92213649446143</v>
+        <v>6.92130088663745</v>
       </c>
       <c r="G35" t="n">
-        <v>18.4773925578184</v>
+        <v>18.1635921544034</v>
       </c>
     </row>
     <row r="36">
@@ -1184,22 +1184,22 @@
         <v>1994</v>
       </c>
       <c r="B36" t="n">
-        <v>13.0309357806627</v>
+        <v>13.0704707721123</v>
       </c>
       <c r="C36" t="n">
-        <v>23.1558318321084</v>
+        <v>23.2860620663353</v>
       </c>
       <c r="D36" t="n">
-        <v>41.147662521104</v>
+        <v>41.4859339048574</v>
       </c>
       <c r="E36" t="n">
-        <v>2.53857858930866</v>
+        <v>2.58181306606276</v>
       </c>
       <c r="F36" t="n">
-        <v>6.7762768288461</v>
+        <v>6.77546032443279</v>
       </c>
       <c r="G36" t="n">
-        <v>18.0880465369644</v>
+        <v>17.7808622984353</v>
       </c>
     </row>
     <row r="37">
@@ -1207,22 +1207,22 @@
         <v>1995</v>
       </c>
       <c r="B37" t="n">
-        <v>17.2191111325259</v>
+        <v>17.2689786437063</v>
       </c>
       <c r="C37" t="n">
-        <v>31.2215014471512</v>
+        <v>31.3957004254399</v>
       </c>
       <c r="D37" t="n">
-        <v>56.6104803617395</v>
+        <v>57.0786510042504</v>
       </c>
       <c r="E37" t="n">
-        <v>1.83453120594987</v>
+        <v>1.86576802701004</v>
       </c>
       <c r="F37" t="n">
-        <v>4.89694955871296</v>
+        <v>4.89634102784982</v>
       </c>
       <c r="G37" t="n">
-        <v>13.07152197946</v>
+        <v>12.8494834909487</v>
       </c>
     </row>
     <row r="38">
@@ -1230,22 +1230,22 @@
         <v>1996</v>
       </c>
       <c r="B38" t="n">
-        <v>14.0677869181068</v>
+        <v>14.0704958183489</v>
       </c>
       <c r="C38" t="n">
-        <v>25.0015983129406</v>
+        <v>25.0709555668908</v>
       </c>
       <c r="D38" t="n">
-        <v>44.4334223883562</v>
+        <v>44.6716889832224</v>
       </c>
       <c r="E38" t="n">
-        <v>1.82738314269597</v>
+        <v>1.85848463485277</v>
       </c>
       <c r="F38" t="n">
-        <v>4.87786909549528</v>
+        <v>4.87722719841051</v>
       </c>
       <c r="G38" t="n">
-        <v>13.0205901306963</v>
+        <v>12.7993230069398</v>
       </c>
     </row>
     <row r="39">
@@ -1253,22 +1253,22 @@
         <v>1997</v>
       </c>
       <c r="B39" t="n">
-        <v>30.3372585700257</v>
+        <v>30.4197734368568</v>
       </c>
       <c r="C39" t="n">
-        <v>52.9713638257829</v>
+        <v>53.2480743026044</v>
       </c>
       <c r="D39" t="n">
-        <v>92.4923845405021</v>
+        <v>93.2077098740106</v>
       </c>
       <c r="E39" t="n">
-        <v>1.59046364912362</v>
+        <v>1.61752046356143</v>
       </c>
       <c r="F39" t="n">
-        <v>4.24545531821155</v>
+        <v>4.24486414949154</v>
       </c>
       <c r="G39" t="n">
-        <v>11.3324758279526</v>
+        <v>11.1398106259286</v>
       </c>
     </row>
     <row r="40">
@@ -1276,22 +1276,22 @@
         <v>1998</v>
       </c>
       <c r="B40" t="n">
-        <v>9.22655373702719</v>
+        <v>9.21588003201352</v>
       </c>
       <c r="C40" t="n">
-        <v>16.1335554634479</v>
+        <v>16.1551818630861</v>
       </c>
       <c r="D40" t="n">
-        <v>28.2111413763918</v>
+        <v>28.3195853377839</v>
       </c>
       <c r="E40" t="n">
-        <v>1.16147975860719</v>
+        <v>1.18126006657878</v>
       </c>
       <c r="F40" t="n">
-        <v>3.10036033888047</v>
+        <v>3.0999845880193</v>
       </c>
       <c r="G40" t="n">
-        <v>8.2758516966578</v>
+        <v>8.13529951434812</v>
       </c>
     </row>
     <row r="41">
@@ -1299,22 +1299,22 @@
         <v>1999</v>
       </c>
       <c r="B41" t="n">
-        <v>9.41253841030416</v>
+        <v>9.38721011130263</v>
       </c>
       <c r="C41" t="n">
-        <v>16.7396517364593</v>
+        <v>16.7378240143492</v>
       </c>
       <c r="D41" t="n">
-        <v>29.7704963361622</v>
+        <v>29.8443040491878</v>
       </c>
       <c r="E41" t="n">
-        <v>2.43616476281458</v>
+        <v>2.47665376592071</v>
       </c>
       <c r="F41" t="n">
-        <v>6.60463426427342</v>
+        <v>6.6038815697226</v>
       </c>
       <c r="G41" t="n">
-        <v>17.9056829121925</v>
+        <v>17.6089417047397</v>
       </c>
     </row>
     <row r="42">
@@ -1322,22 +1322,22 @@
         <v>2000</v>
       </c>
       <c r="B42" t="n">
-        <v>7.70566358300954</v>
+        <v>7.68355269872122</v>
       </c>
       <c r="C42" t="n">
-        <v>13.4642589339886</v>
+        <v>13.4592744907925</v>
       </c>
       <c r="D42" t="n">
-        <v>23.5263668973578</v>
+        <v>23.5766027671869</v>
       </c>
       <c r="E42" t="n">
-        <v>1.776183621726</v>
+        <v>1.80645492559393</v>
       </c>
       <c r="F42" t="n">
-        <v>4.74120122590163</v>
+        <v>4.74068546523516</v>
       </c>
       <c r="G42" t="n">
-        <v>12.6557799483858</v>
+        <v>12.4409960978698</v>
       </c>
     </row>
     <row r="43">
@@ -1345,22 +1345,22 @@
         <v>2001</v>
       </c>
       <c r="B43" t="n">
-        <v>5.2356804394267</v>
+        <v>5.21360936109646</v>
       </c>
       <c r="C43" t="n">
-        <v>9.00720555728804</v>
+        <v>8.99103359468584</v>
       </c>
       <c r="D43" t="n">
-        <v>15.4955507483425</v>
+        <v>15.505320690879</v>
       </c>
       <c r="E43" t="n">
-        <v>0.37800256615656</v>
+        <v>0.384441898407975</v>
       </c>
       <c r="F43" t="n">
-        <v>1.00900954616049</v>
+        <v>1.00889210917393</v>
       </c>
       <c r="G43" t="n">
-        <v>2.69336865777077</v>
+        <v>2.64763880359692</v>
       </c>
     </row>
     <row r="44">
@@ -1368,22 +1368,22 @@
         <v>2002</v>
       </c>
       <c r="B44" t="n">
-        <v>6.65597928017498</v>
+        <v>6.62285379063689</v>
       </c>
       <c r="C44" t="n">
-        <v>11.6307852491283</v>
+        <v>11.6019065290811</v>
       </c>
       <c r="D44" t="n">
-        <v>20.3238561625726</v>
+        <v>20.3242045445473</v>
       </c>
       <c r="E44" t="n">
-        <v>0.94803992330544</v>
+        <v>0.963805838026598</v>
       </c>
       <c r="F44" t="n">
-        <v>2.56796049850729</v>
+        <v>2.56763442603607</v>
       </c>
       <c r="G44" t="n">
-        <v>6.95584749100194</v>
+        <v>6.84032642846852</v>
       </c>
     </row>
     <row r="45">
@@ -1391,22 +1391,22 @@
         <v>2003</v>
       </c>
       <c r="B45" t="n">
-        <v>8.85042630433154</v>
+        <v>8.85346341219623</v>
       </c>
       <c r="C45" t="n">
-        <v>15.22583547927</v>
+        <v>15.2680765771138</v>
       </c>
       <c r="D45" t="n">
-        <v>26.1937739573447</v>
+        <v>26.3302790683566</v>
       </c>
       <c r="E45" t="n">
-        <v>0.702865884120151</v>
+        <v>0.714207152475751</v>
       </c>
       <c r="F45" t="n">
-        <v>1.93798233638079</v>
+        <v>1.93768056685584</v>
       </c>
       <c r="G45" t="n">
-        <v>5.34351662383701</v>
+        <v>5.25702657297072</v>
       </c>
     </row>
     <row r="46">
@@ -1414,22 +1414,22 @@
         <v>2004</v>
       </c>
       <c r="B46" t="n">
-        <v>3.50855738807604</v>
+        <v>3.50027034063236</v>
       </c>
       <c r="C46" t="n">
-        <v>6.24064419487076</v>
+        <v>6.24202087664803</v>
       </c>
       <c r="D46" t="n">
-        <v>11.1001861047883</v>
+        <v>11.1313758175235</v>
       </c>
       <c r="E46" t="n">
-        <v>0.24322084401861</v>
+        <v>0.247356437618706</v>
       </c>
       <c r="F46" t="n">
-        <v>0.649109775059659</v>
+        <v>0.649010660001027</v>
       </c>
       <c r="G46" t="n">
-        <v>1.73234946938084</v>
+        <v>1.70286587585912</v>
       </c>
     </row>
     <row r="47">
@@ -1437,22 +1437,22 @@
         <v>2005</v>
       </c>
       <c r="B47" t="n">
-        <v>3.85544991474533</v>
+        <v>3.85649211109577</v>
       </c>
       <c r="C47" t="n">
-        <v>6.85804733054822</v>
+        <v>6.87766009787329</v>
       </c>
       <c r="D47" t="n">
-        <v>12.1990466036559</v>
+        <v>12.2656048707534</v>
       </c>
       <c r="E47" t="n">
-        <v>0.40556659408309</v>
+        <v>0.412297188875586</v>
       </c>
       <c r="F47" t="n">
-        <v>1.09857656784185</v>
+        <v>1.09840024955506</v>
       </c>
       <c r="G47" t="n">
-        <v>2.97576401266402</v>
+        <v>2.92624626307284</v>
       </c>
     </row>
     <row r="48">
@@ -1460,22 +1460,22 @@
         <v>2006</v>
       </c>
       <c r="B48" t="n">
-        <v>3.13962622914509</v>
+        <v>3.13034388775052</v>
       </c>
       <c r="C48" t="n">
-        <v>5.40411005917053</v>
+        <v>5.40126399474084</v>
       </c>
       <c r="D48" t="n">
-        <v>9.30187334419751</v>
+        <v>9.31963189573019</v>
       </c>
       <c r="E48" t="n">
-        <v>0.182722352843019</v>
+        <v>0.185893460227514</v>
       </c>
       <c r="F48" t="n">
-        <v>0.481715454996184</v>
+        <v>0.481648306518502</v>
       </c>
       <c r="G48" t="n">
-        <v>1.26995836016593</v>
+        <v>1.24794648982388</v>
       </c>
     </row>
     <row r="49">
@@ -1483,22 +1483,22 @@
         <v>2007</v>
       </c>
       <c r="B49" t="n">
-        <v>3.71815544629591</v>
+        <v>3.70745289360513</v>
       </c>
       <c r="C49" t="n">
-        <v>6.50694781348385</v>
+        <v>6.50447053046564</v>
       </c>
       <c r="D49" t="n">
-        <v>11.3874663012227</v>
+        <v>11.4116451633605</v>
       </c>
       <c r="E49" t="n">
-        <v>0.504653411169094</v>
+        <v>0.513417927894026</v>
       </c>
       <c r="F49" t="n">
-        <v>1.33043026096292</v>
+        <v>1.33026129700175</v>
       </c>
       <c r="G49" t="n">
-        <v>3.50744618011266</v>
+        <v>3.44669522071313</v>
       </c>
     </row>
     <row r="50">
@@ -1506,22 +1506,22 @@
         <v>2008</v>
       </c>
       <c r="B50" t="n">
-        <v>2.46119526530347</v>
+        <v>2.45282785105669</v>
       </c>
       <c r="C50" t="n">
-        <v>4.38143023341315</v>
+        <v>4.3778037689968</v>
       </c>
       <c r="D50" t="n">
-        <v>7.7998406550241</v>
+        <v>7.81349813505506</v>
       </c>
       <c r="E50" t="n">
-        <v>0.492867298692975</v>
+        <v>0.501783651238983</v>
       </c>
       <c r="F50" t="n">
-        <v>1.26753960033602</v>
+        <v>1.26739847585941</v>
       </c>
       <c r="G50" t="n">
-        <v>3.25981586256718</v>
+        <v>3.20117822221699</v>
       </c>
     </row>
     <row r="51">
@@ -1529,22 +1529,22 @@
         <v>2009</v>
       </c>
       <c r="B51" t="n">
-        <v>2.06730459774089</v>
+        <v>2.0561325534276</v>
       </c>
       <c r="C51" t="n">
-        <v>3.75033567792319</v>
+        <v>3.74005541354011</v>
       </c>
       <c r="D51" t="n">
-        <v>6.80355362846557</v>
+        <v>6.80307039204862</v>
       </c>
       <c r="E51" t="n">
-        <v>0.367506063813052</v>
+        <v>0.374130978923712</v>
       </c>
       <c r="F51" t="n">
-        <v>0.945139777952362</v>
+        <v>0.944975053070967</v>
       </c>
       <c r="G51" t="n">
-        <v>2.43067880458771</v>
+        <v>2.38680542706024</v>
       </c>
     </row>
     <row r="52">
@@ -1552,22 +1552,22 @@
         <v>2010</v>
       </c>
       <c r="B52" t="n">
-        <v>2.71893040970418</v>
+        <v>2.70996722926339</v>
       </c>
       <c r="C52" t="n">
-        <v>4.68050675442864</v>
+        <v>4.67644936231182</v>
       </c>
       <c r="D52" t="n">
-        <v>8.05726523932461</v>
+        <v>8.06990520110865</v>
       </c>
       <c r="E52" t="n">
-        <v>0.287711307723091</v>
+        <v>0.292749763125414</v>
       </c>
       <c r="F52" t="n">
-        <v>0.75374882396574</v>
+        <v>0.753629783244443</v>
       </c>
       <c r="G52" t="n">
-        <v>1.97467834728464</v>
+        <v>1.9400796233941</v>
       </c>
     </row>
     <row r="53">
@@ -1575,22 +1575,22 @@
         <v>2011</v>
       </c>
       <c r="B53" t="n">
-        <v>2.09205413859351</v>
+        <v>2.0840595275911</v>
       </c>
       <c r="C53" t="n">
-        <v>3.60136967513731</v>
+        <v>3.59635302729193</v>
       </c>
       <c r="D53" t="n">
-        <v>6.19958312633261</v>
+        <v>6.20603918730744</v>
       </c>
       <c r="E53" t="n">
-        <v>0.185315371584239</v>
+        <v>0.188665410827865</v>
       </c>
       <c r="F53" t="n">
-        <v>0.476295523278327</v>
+        <v>0.476227900075094</v>
       </c>
       <c r="G53" t="n">
-        <v>1.22416949849113</v>
+        <v>1.20209110835295</v>
       </c>
     </row>
     <row r="54">
@@ -1598,22 +1598,22 @@
         <v>2012</v>
       </c>
       <c r="B54" t="n">
-        <v>2.93910129315146</v>
+        <v>2.69614275646596</v>
       </c>
       <c r="C54" t="n">
-        <v>5.23129794780478</v>
+        <v>4.6616937309549</v>
       </c>
       <c r="D54" t="n">
-        <v>9.31117218806797</v>
+        <v>8.06017722507735</v>
       </c>
       <c r="E54" t="n">
-        <v>0.174771916966253</v>
+        <v>0.178039583813885</v>
       </c>
       <c r="F54" t="n">
-        <v>0.439552923036744</v>
+        <v>0.439478279479693</v>
       </c>
       <c r="G54" t="n">
-        <v>1.10547950439574</v>
+        <v>1.08482144249636</v>
       </c>
     </row>
     <row r="55">
@@ -1621,22 +1621,22 @@
         <v>2013</v>
       </c>
       <c r="B55" t="n">
-        <v>3.89638627068457</v>
+        <v>3.79811417548692</v>
       </c>
       <c r="C55" t="n">
-        <v>6.80797729518493</v>
+        <v>6.46892017820276</v>
       </c>
       <c r="D55" t="n">
-        <v>11.8952669555553</v>
+        <v>11.017817353159</v>
       </c>
       <c r="E55" t="n">
-        <v>0.443267405574966</v>
+        <v>0.451369994223271</v>
       </c>
       <c r="F55" t="n">
-        <v>1.12952253771742</v>
+        <v>1.12930477274834</v>
       </c>
       <c r="G55" t="n">
-        <v>2.87822011536516</v>
+        <v>2.82546311468221</v>
       </c>
     </row>
     <row r="56">
@@ -1644,22 +1644,22 @@
         <v>2014</v>
       </c>
       <c r="B56" t="n">
-        <v>5.85061602764444</v>
+        <v>5.97340316440069</v>
       </c>
       <c r="C56" t="n">
-        <v>10.2225134552819</v>
+        <v>10.1738564133023</v>
       </c>
       <c r="D56" t="n">
-        <v>17.8613296189072</v>
+        <v>17.3280375473997</v>
       </c>
       <c r="E56" t="n">
-        <v>1.27143471385916</v>
+        <v>1.29497021740123</v>
       </c>
       <c r="F56" t="n">
-        <v>3.21817523064245</v>
+        <v>3.21765327860389</v>
       </c>
       <c r="G56" t="n">
-        <v>8.14564185028832</v>
+        <v>7.99500442727365</v>
       </c>
     </row>
     <row r="57">
@@ -1667,22 +1667,22 @@
         <v>2015</v>
       </c>
       <c r="B57" t="n">
-        <v>4.61050419624199</v>
+        <v>4.59812673755341</v>
       </c>
       <c r="C57" t="n">
-        <v>8.05572284337602</v>
+        <v>7.83149570027857</v>
       </c>
       <c r="D57" t="n">
-        <v>14.0753956112188</v>
+        <v>13.338545978425</v>
       </c>
       <c r="E57" t="n">
-        <v>0.327881218521897</v>
+        <v>0.333949794344916</v>
       </c>
       <c r="F57" t="n">
-        <v>0.830355456415155</v>
+        <v>0.830231815570457</v>
       </c>
       <c r="G57" t="n">
-        <v>2.10286574847645</v>
+        <v>2.06403740699268</v>
       </c>
     </row>
     <row r="58">
@@ -1690,22 +1690,22 @@
         <v>2016</v>
       </c>
       <c r="B58" t="n">
-        <v>6.255708150009</v>
+        <v>7.64620846780991</v>
       </c>
       <c r="C58" t="n">
-        <v>11.1323907210792</v>
+        <v>13.2168841303892</v>
       </c>
       <c r="D58" t="n">
-        <v>19.8107264909076</v>
+        <v>22.8460977557114</v>
       </c>
       <c r="E58" t="n">
-        <v>0.678980884229304</v>
+        <v>0.691194106787992</v>
       </c>
       <c r="F58" t="n">
-        <v>1.74737590318471</v>
+        <v>1.7470385231646</v>
       </c>
       <c r="G58" t="n">
-        <v>4.49691974833185</v>
+        <v>4.4157546649299</v>
       </c>
     </row>
     <row r="59">
@@ -1713,22 +1713,22 @@
         <v>2017</v>
       </c>
       <c r="B59" t="n">
-        <v>7.12982686963849</v>
+        <v>6.69257869260475</v>
       </c>
       <c r="C59" t="n">
-        <v>12.4576199778494</v>
+        <v>11.3987508928034</v>
       </c>
       <c r="D59" t="n">
-        <v>21.7666288887576</v>
+        <v>19.4142688317972</v>
       </c>
       <c r="E59" t="n">
-        <v>0.512781809146948</v>
+        <v>0.522339766675483</v>
       </c>
       <c r="F59" t="n">
-        <v>1.28965080319016</v>
+        <v>1.289359237114</v>
       </c>
       <c r="G59" t="n">
-        <v>3.24348322132541</v>
+        <v>3.18269323607527</v>
       </c>
     </row>
     <row r="60">
@@ -1736,22 +1736,22 @@
         <v>2018</v>
       </c>
       <c r="B60" t="n">
-        <v>6.00594650002057</v>
+        <v>7.11141871897334</v>
       </c>
       <c r="C60" t="n">
-        <v>11.6245673872715</v>
+        <v>13.1371796531813</v>
       </c>
       <c r="D60" t="n">
-        <v>22.4994623146832</v>
+        <v>24.2687846209225</v>
       </c>
       <c r="E60" t="n">
-        <v>0.789011234016432</v>
+        <v>0.803787881926017</v>
       </c>
       <c r="F60" t="n">
-        <v>1.9843702594835</v>
+        <v>1.98409425504354</v>
       </c>
       <c r="G60" t="n">
-        <v>4.99070882258262</v>
+        <v>4.89759811190972</v>
       </c>
     </row>
     <row r="61">
@@ -1759,22 +1759,22 @@
         <v>2019</v>
       </c>
       <c r="B61" t="n">
-        <v>3.49541500900778</v>
+        <v>3.51830491558193</v>
       </c>
       <c r="C61" t="n">
-        <v>6.34992373636606</v>
+        <v>6.18247753241634</v>
       </c>
       <c r="D61" t="n">
-        <v>11.535549098964</v>
+        <v>10.8640465667288</v>
       </c>
       <c r="E61" t="n">
-        <v>0.656800784761461</v>
+        <v>0.668946084896688</v>
       </c>
       <c r="F61" t="n">
-        <v>1.66245265600007</v>
+        <v>1.66215140267597</v>
       </c>
       <c r="G61" t="n">
-        <v>4.20789514501787</v>
+        <v>4.12999993242261</v>
       </c>
     </row>
     <row r="62">
@@ -1782,22 +1782,22 @@
         <v>2020</v>
       </c>
       <c r="B62" t="n">
-        <v>4.61669284467119</v>
+        <v>4.87728479863872</v>
       </c>
       <c r="C62" t="n">
-        <v>8.38688607857484</v>
+        <v>8.5705202960762</v>
       </c>
       <c r="D62" t="n">
-        <v>15.2359839524915</v>
+        <v>15.0603914222839</v>
       </c>
       <c r="E62" t="n">
-        <v>0.292382907979087</v>
+        <v>0.297654547834972</v>
       </c>
       <c r="F62" t="n">
-        <v>0.75134921855266</v>
+        <v>0.751203695778358</v>
       </c>
       <c r="G62" t="n">
-        <v>1.93077513361373</v>
+        <v>1.89584535716193</v>
       </c>
     </row>
     <row r="63">
@@ -1805,22 +1805,22 @@
         <v>2021</v>
       </c>
       <c r="B63" t="n">
-        <v>3.01817961576493</v>
+        <v>3.4658774394981</v>
       </c>
       <c r="C63" t="n">
-        <v>5.48295705470524</v>
+        <v>6.09035030048302</v>
       </c>
       <c r="D63" t="n">
-        <v>9.96057951843358</v>
+        <v>10.7021576585135</v>
       </c>
       <c r="E63" t="n">
-        <v>0.264364302290921</v>
+        <v>0.273261215108193</v>
       </c>
       <c r="F63" t="n">
-        <v>0.480255750415593</v>
+        <v>0.480183316518411</v>
       </c>
       <c r="G63" t="n">
-        <v>0.872453594560694</v>
+        <v>0.843793428098929</v>
       </c>
     </row>
   </sheetData>
@@ -1856,13 +1856,13 @@
         <v>1950</v>
       </c>
       <c r="B2" t="n">
-        <v>48.6211222114679</v>
+        <v>47.9049576415035</v>
       </c>
       <c r="C2" t="n">
-        <v>181.782198563785</v>
+        <v>181.845062807373</v>
       </c>
       <c r="D2" t="n">
-        <v>679.638112237757</v>
+        <v>690.275672820311</v>
       </c>
     </row>
     <row r="3">
@@ -1870,13 +1870,13 @@
         <v>1951</v>
       </c>
       <c r="B3" t="n">
-        <v>77.1158381169509</v>
+        <v>75.8753779438938</v>
       </c>
       <c r="C3" t="n">
-        <v>262.220339907963</v>
+        <v>262.242830599742</v>
       </c>
       <c r="D3" t="n">
-        <v>891.639231841971</v>
+        <v>906.371791015236</v>
       </c>
     </row>
     <row r="4">
@@ -1884,13 +1884,13 @@
         <v>1952</v>
       </c>
       <c r="B4" t="n">
-        <v>74.1228712786351</v>
+        <v>72.942903763646</v>
       </c>
       <c r="C4" t="n">
-        <v>252.043224533998</v>
+        <v>252.107522538972</v>
       </c>
       <c r="D4" t="n">
-        <v>857.033543596762</v>
+        <v>871.341825473294</v>
       </c>
     </row>
     <row r="5">
@@ -1898,13 +1898,13 @@
         <v>1953</v>
       </c>
       <c r="B5" t="n">
-        <v>117.527579250398</v>
+        <v>115.650396843975</v>
       </c>
       <c r="C5" t="n">
-        <v>399.634141729256</v>
+        <v>399.71448248698</v>
       </c>
       <c r="D5" t="n">
-        <v>1358.89336149275</v>
+        <v>1381.50557084023</v>
       </c>
     </row>
     <row r="6">
@@ -1912,13 +1912,13 @@
         <v>1954</v>
       </c>
       <c r="B6" t="n">
-        <v>57.725253037941</v>
+        <v>56.7734884370819</v>
       </c>
       <c r="C6" t="n">
-        <v>196.285689716896</v>
+        <v>196.222288629276</v>
       </c>
       <c r="D6" t="n">
-        <v>667.438771767955</v>
+        <v>678.189549644837</v>
       </c>
     </row>
     <row r="7">
@@ -1926,13 +1926,13 @@
         <v>1955</v>
       </c>
       <c r="B7" t="n">
-        <v>89.3157115578561</v>
+        <v>87.8671853124194</v>
       </c>
       <c r="C7" t="n">
-        <v>303.704100424924</v>
+        <v>303.689286532449</v>
       </c>
       <c r="D7" t="n">
-        <v>1032.69826782004</v>
+        <v>1049.6203153278</v>
       </c>
     </row>
     <row r="8">
@@ -1940,13 +1940,13 @@
         <v>1956</v>
       </c>
       <c r="B8" t="n">
-        <v>39.7198985749305</v>
+        <v>39.0748748821943</v>
       </c>
       <c r="C8" t="n">
-        <v>135.061299465262</v>
+        <v>135.051792453865</v>
       </c>
       <c r="D8" t="n">
-        <v>459.254813524587</v>
+        <v>466.770186724593</v>
       </c>
     </row>
     <row r="9">
@@ -1954,13 +1954,13 @@
         <v>1957</v>
       </c>
       <c r="B9" t="n">
-        <v>46.0487364361292</v>
+        <v>45.3079575595545</v>
       </c>
       <c r="C9" t="n">
-        <v>156.581522232848</v>
+        <v>156.5947658</v>
       </c>
       <c r="D9" t="n">
-        <v>532.430963415522</v>
+        <v>541.227678244476</v>
       </c>
     </row>
     <row r="10">
@@ -1968,13 +1968,13 @@
         <v>1958</v>
       </c>
       <c r="B10" t="n">
-        <v>45.0926445873869</v>
+        <v>44.3524046584678</v>
       </c>
       <c r="C10" t="n">
-        <v>153.33048151693</v>
+        <v>153.29215427622</v>
       </c>
       <c r="D10" t="n">
-        <v>521.376308205922</v>
+        <v>529.813090036325</v>
       </c>
     </row>
     <row r="11">
@@ -1982,13 +1982,13 @@
         <v>1959</v>
       </c>
       <c r="B11" t="n">
-        <v>98.1997019128598</v>
+        <v>96.5831732327912</v>
       </c>
       <c r="C11" t="n">
-        <v>333.912719400125</v>
+        <v>333.813753858354</v>
       </c>
       <c r="D11" t="n">
-        <v>1135.41794939588</v>
+        <v>1153.73743205171</v>
       </c>
     </row>
     <row r="12">
@@ -1996,13 +1996,13 @@
         <v>1960</v>
       </c>
       <c r="B12" t="n">
-        <v>52.2810386204738</v>
+        <v>51.3771157255092</v>
       </c>
       <c r="C12" t="n">
-        <v>166.225751813145</v>
+        <v>166.190589937837</v>
       </c>
       <c r="D12" t="n">
-        <v>528.509021529363</v>
+        <v>537.580045003829</v>
       </c>
     </row>
     <row r="13">
@@ -2010,13 +2010,13 @@
         <v>1961</v>
       </c>
       <c r="B13" t="n">
-        <v>56.9385860828052</v>
+        <v>55.945770420126</v>
       </c>
       <c r="C13" t="n">
-        <v>181.034262679804</v>
+        <v>180.96890919922</v>
       </c>
       <c r="D13" t="n">
-        <v>575.592169014494</v>
+        <v>585.383771656387</v>
       </c>
     </row>
     <row r="14">
@@ -2024,13 +2024,13 @@
         <v>1962</v>
       </c>
       <c r="B14" t="n">
-        <v>56.0021307782678</v>
+        <v>55.0341121066753</v>
       </c>
       <c r="C14" t="n">
-        <v>178.056835468262</v>
+        <v>178.019949710261</v>
       </c>
       <c r="D14" t="n">
-        <v>566.125542303027</v>
+        <v>575.84471306479</v>
       </c>
     </row>
     <row r="15">
@@ -2038,13 +2038,13 @@
         <v>1963</v>
       </c>
       <c r="B15" t="n">
-        <v>47.3023016072656</v>
+        <v>46.486772304032</v>
       </c>
       <c r="C15" t="n">
-        <v>150.396029892198</v>
+        <v>150.371697679344</v>
       </c>
       <c r="D15" t="n">
-        <v>478.178968861435</v>
+        <v>486.410355941335</v>
       </c>
     </row>
     <row r="16">
@@ -2052,13 +2052,13 @@
         <v>1964</v>
       </c>
       <c r="B16" t="n">
-        <v>19.1699852572635</v>
+        <v>18.8411176662674</v>
       </c>
       <c r="C16" t="n">
-        <v>60.9503042731759</v>
+        <v>60.945742395782</v>
       </c>
       <c r="D16" t="n">
-        <v>193.789381741185</v>
+        <v>197.142419147625</v>
       </c>
     </row>
     <row r="17">
@@ -2066,13 +2066,13 @@
         <v>1965</v>
       </c>
       <c r="B17" t="n">
-        <v>36.0640455483708</v>
+        <v>35.4410955998756</v>
       </c>
       <c r="C17" t="n">
-        <v>114.66438393123</v>
+        <v>114.642025006908</v>
       </c>
       <c r="D17" t="n">
-        <v>364.571437907428</v>
+        <v>370.834864871688</v>
       </c>
     </row>
     <row r="18">
@@ -2080,13 +2080,13 @@
         <v>1966</v>
       </c>
       <c r="B18" t="n">
-        <v>49.1516386479159</v>
+        <v>48.3126027818442</v>
       </c>
       <c r="C18" t="n">
-        <v>156.275932970819</v>
+        <v>156.277748261383</v>
       </c>
       <c r="D18" t="n">
-        <v>496.873917080189</v>
+        <v>505.51477658799</v>
       </c>
     </row>
     <row r="19">
@@ -2094,13 +2094,13 @@
         <v>1967</v>
       </c>
       <c r="B19" t="n">
-        <v>36.727739373935</v>
+        <v>36.0805087857076</v>
       </c>
       <c r="C19" t="n">
-        <v>110.970783031742</v>
+        <v>110.99450757344</v>
       </c>
       <c r="D19" t="n">
-        <v>335.291931836603</v>
+        <v>341.452521765731</v>
       </c>
     </row>
     <row r="20">
@@ -2108,13 +2108,13 @@
         <v>1968</v>
       </c>
       <c r="B20" t="n">
-        <v>57.4610222053425</v>
+        <v>56.4169469834167</v>
       </c>
       <c r="C20" t="n">
-        <v>173.61522208079</v>
+        <v>173.555514042578</v>
       </c>
       <c r="D20" t="n">
-        <v>524.568554148686</v>
+        <v>533.909012542589</v>
       </c>
     </row>
     <row r="21">
@@ -2122,13 +2122,13 @@
         <v>1969</v>
       </c>
       <c r="B21" t="n">
-        <v>38.3890627835185</v>
+        <v>37.7063461207245</v>
       </c>
       <c r="C21" t="n">
-        <v>115.990377560919</v>
+        <v>115.996072697328</v>
       </c>
       <c r="D21" t="n">
-        <v>350.45835222892</v>
+        <v>356.838841878889</v>
       </c>
     </row>
     <row r="22">
@@ -2136,13 +2136,13 @@
         <v>1970</v>
       </c>
       <c r="B22" t="n">
-        <v>19.6366261867948</v>
+        <v>19.2948780444987</v>
       </c>
       <c r="C22" t="n">
-        <v>59.3309531486351</v>
+        <v>59.3568538614138</v>
       </c>
       <c r="D22" t="n">
-        <v>179.265112450568</v>
+        <v>182.599552699933</v>
       </c>
     </row>
     <row r="23">
@@ -2150,13 +2150,13 @@
         <v>1971</v>
       </c>
       <c r="B23" t="n">
-        <v>20.5650859691924</v>
+        <v>20.1963350142934</v>
       </c>
       <c r="C23" t="n">
-        <v>62.1362417621581</v>
+        <v>62.1300068969016</v>
       </c>
       <c r="D23" t="n">
-        <v>187.741133011027</v>
+        <v>191.130606334126</v>
       </c>
     </row>
     <row r="24">
@@ -2164,13 +2164,13 @@
         <v>1972</v>
       </c>
       <c r="B24" t="n">
-        <v>34.1184486404942</v>
+        <v>33.5222701795648</v>
       </c>
       <c r="C24" t="n">
-        <v>108.47842593822</v>
+        <v>108.435161813324</v>
       </c>
       <c r="D24" t="n">
-        <v>344.903398686989</v>
+        <v>350.757399618164</v>
       </c>
     </row>
     <row r="25">
@@ -2178,13 +2178,13 @@
         <v>1973</v>
       </c>
       <c r="B25" t="n">
-        <v>44.6687856151227</v>
+        <v>43.8628728839157</v>
       </c>
       <c r="C25" t="n">
-        <v>134.964204203241</v>
+        <v>134.935402530554</v>
       </c>
       <c r="D25" t="n">
-        <v>407.786694117052</v>
+        <v>415.101922399599</v>
       </c>
     </row>
     <row r="26">
@@ -2192,13 +2192,13 @@
         <v>1974</v>
       </c>
       <c r="B26" t="n">
-        <v>21.4780094803794</v>
+        <v>21.0966887643715</v>
       </c>
       <c r="C26" t="n">
-        <v>64.8945884127126</v>
+        <v>64.8997660964006</v>
       </c>
       <c r="D26" t="n">
-        <v>196.075321090741</v>
+        <v>199.651219507053</v>
       </c>
     </row>
     <row r="27">
@@ -2206,13 +2206,13 @@
         <v>1975</v>
       </c>
       <c r="B27" t="n">
-        <v>40.4743971556868</v>
+        <v>39.7536004121368</v>
       </c>
       <c r="C27" t="n">
-        <v>122.291097183394</v>
+        <v>122.294043252637</v>
       </c>
       <c r="D27" t="n">
-        <v>369.4956194849</v>
+        <v>376.213295400327</v>
       </c>
     </row>
     <row r="28">
@@ -2220,13 +2220,13 @@
         <v>1976</v>
       </c>
       <c r="B28" t="n">
-        <v>12.415598759648</v>
+        <v>12.2009973102983</v>
       </c>
       <c r="C28" t="n">
-        <v>37.5130280178323</v>
+        <v>37.5339410096641</v>
       </c>
       <c r="D28" t="n">
-        <v>113.343488164285</v>
+        <v>115.465702670703</v>
       </c>
     </row>
     <row r="29">
@@ -2234,13 +2234,13 @@
         <v>1977</v>
       </c>
       <c r="B29" t="n">
-        <v>25.8712051320292</v>
+        <v>25.4148589094053</v>
       </c>
       <c r="C29" t="n">
-        <v>78.1683800967494</v>
+        <v>78.1837575088555</v>
       </c>
       <c r="D29" t="n">
-        <v>236.181330392885</v>
+        <v>240.516776425675</v>
       </c>
     </row>
     <row r="30">
@@ -2248,13 +2248,13 @@
         <v>1978</v>
       </c>
       <c r="B30" t="n">
-        <v>23.0408738456407</v>
+        <v>22.6434846257692</v>
       </c>
       <c r="C30" t="n">
-        <v>69.6166945194804</v>
+        <v>69.6581758508792</v>
       </c>
       <c r="D30" t="n">
-        <v>210.342897074436</v>
+        <v>214.289520498535</v>
       </c>
     </row>
     <row r="31">
@@ -2262,13 +2262,13 @@
         <v>1979</v>
       </c>
       <c r="B31" t="n">
-        <v>19.2441295561846</v>
+        <v>18.9029192233182</v>
       </c>
       <c r="C31" t="n">
-        <v>58.1450468233728</v>
+        <v>58.151070522704</v>
       </c>
       <c r="D31" t="n">
-        <v>175.681963698156</v>
+        <v>178.890200131898</v>
       </c>
     </row>
     <row r="32">
@@ -2276,13 +2276,13 @@
         <v>1980</v>
       </c>
       <c r="B32" t="n">
-        <v>33.9468415169517</v>
+        <v>33.3245045584003</v>
       </c>
       <c r="C32" t="n">
-        <v>98.5876038926354</v>
+        <v>98.6024452517102</v>
       </c>
       <c r="D32" t="n">
-        <v>286.315757430264</v>
+        <v>291.750540284198</v>
       </c>
     </row>
     <row r="33">
@@ -2290,13 +2290,13 @@
         <v>1981</v>
       </c>
       <c r="B33" t="n">
-        <v>14.1206363567383</v>
+        <v>13.8635251559416</v>
       </c>
       <c r="C33" t="n">
-        <v>41.0088138289653</v>
+        <v>41.0201891460639</v>
       </c>
       <c r="D33" t="n">
-        <v>119.096814702422</v>
+        <v>121.372875848803</v>
       </c>
     </row>
     <row r="34">
@@ -2304,13 +2304,13 @@
         <v>1982</v>
       </c>
       <c r="B34" t="n">
-        <v>17.8430664235896</v>
+        <v>17.5235998679521</v>
       </c>
       <c r="C34" t="n">
-        <v>51.8194060534439</v>
+        <v>51.8498270113687</v>
       </c>
       <c r="D34" t="n">
-        <v>150.492677658905</v>
+        <v>153.416226195938</v>
       </c>
     </row>
     <row r="35">
@@ -2318,13 +2318,13 @@
         <v>1983</v>
       </c>
       <c r="B35" t="n">
-        <v>16.1040744164775</v>
+        <v>15.8060353610768</v>
       </c>
       <c r="C35" t="n">
-        <v>46.7690671262127</v>
+        <v>46.7677991613023</v>
       </c>
       <c r="D35" t="n">
-        <v>135.825604333902</v>
+        <v>138.379232263271</v>
       </c>
     </row>
     <row r="36">
@@ -2332,13 +2332,13 @@
         <v>1984</v>
       </c>
       <c r="B36" t="n">
-        <v>12.0435645163947</v>
+        <v>11.8264172244314</v>
       </c>
       <c r="C36" t="n">
-        <v>34.9766315492064</v>
+        <v>34.9926779812225</v>
       </c>
       <c r="D36" t="n">
-        <v>101.578295434345</v>
+        <v>103.538331944517</v>
       </c>
     </row>
     <row r="37">
@@ -2346,13 +2346,13 @@
         <v>1985</v>
       </c>
       <c r="B37" t="n">
-        <v>22.4753163210188</v>
+        <v>22.0891587757604</v>
       </c>
       <c r="C37" t="n">
-        <v>65.1819881363839</v>
+        <v>65.3053948513851</v>
       </c>
       <c r="D37" t="n">
-        <v>189.038121498576</v>
+        <v>193.0718430697</v>
       </c>
     </row>
     <row r="38">
@@ -2360,13 +2360,13 @@
         <v>1986</v>
       </c>
       <c r="B38" t="n">
-        <v>17.4290643278303</v>
+        <v>17.1477484012885</v>
       </c>
       <c r="C38" t="n">
-        <v>48.9664982800706</v>
+        <v>49.1356333453511</v>
       </c>
       <c r="D38" t="n">
-        <v>137.570090322264</v>
+        <v>140.794605084558</v>
       </c>
     </row>
     <row r="39">
@@ -2374,13 +2374,13 @@
         <v>1987</v>
       </c>
       <c r="B39" t="n">
-        <v>16.8206378417319</v>
+        <v>16.521033639494</v>
       </c>
       <c r="C39" t="n">
-        <v>47.2571400537937</v>
+        <v>47.3398275038487</v>
       </c>
       <c r="D39" t="n">
-        <v>132.767693298956</v>
+        <v>135.648853273734</v>
       </c>
     </row>
     <row r="40">
@@ -2388,13 +2388,13 @@
         <v>1988</v>
       </c>
       <c r="B40" t="n">
-        <v>21.7254844985368</v>
+        <v>21.3476395946478</v>
       </c>
       <c r="C40" t="n">
-        <v>61.0371778611564</v>
+        <v>61.1701179282813</v>
       </c>
       <c r="D40" t="n">
-        <v>171.48234744801</v>
+        <v>175.278550622429</v>
       </c>
     </row>
     <row r="41">
@@ -2402,13 +2402,13 @@
         <v>1989</v>
       </c>
       <c r="B41" t="n">
-        <v>12.0043833127385</v>
+        <v>11.8150281185317</v>
       </c>
       <c r="C41" t="n">
-        <v>36.2280251918801</v>
+        <v>36.3275352061576</v>
       </c>
       <c r="D41" t="n">
-        <v>109.332547546259</v>
+        <v>111.695867408449</v>
       </c>
     </row>
     <row r="42">
@@ -2416,13 +2416,13 @@
         <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>10.9793023550659</v>
+        <v>10.8076831978728</v>
       </c>
       <c r="C42" t="n">
-        <v>31.8484591329302</v>
+        <v>31.9590356077444</v>
       </c>
       <c r="D42" t="n">
-        <v>92.3851367180825</v>
+        <v>94.5049867096496</v>
       </c>
     </row>
     <row r="43">
@@ -2430,13 +2430,13 @@
         <v>1991</v>
       </c>
       <c r="B43" t="n">
-        <v>12.3679897297067</v>
+        <v>12.1572344932185</v>
       </c>
       <c r="C43" t="n">
-        <v>37.3253529004911</v>
+        <v>37.3797133304486</v>
       </c>
       <c r="D43" t="n">
-        <v>112.644172544865</v>
+        <v>114.930987754322</v>
       </c>
     </row>
     <row r="44">
@@ -2444,13 +2444,13 @@
         <v>1992</v>
       </c>
       <c r="B44" t="n">
-        <v>6.28548977514357</v>
+        <v>6.18091230672056</v>
       </c>
       <c r="C44" t="n">
-        <v>17.6436200089336</v>
+        <v>17.6955699849274</v>
       </c>
       <c r="D44" t="n">
-        <v>49.5263437148035</v>
+        <v>50.6613233698515</v>
       </c>
     </row>
     <row r="45">
@@ -2458,13 +2458,13 @@
         <v>1993</v>
       </c>
       <c r="B45" t="n">
-        <v>4.99570095592787</v>
+        <v>4.91900538283597</v>
       </c>
       <c r="C45" t="n">
-        <v>14.02313145003</v>
+        <v>14.0828084413307</v>
       </c>
       <c r="D45" t="n">
-        <v>39.3634882070912</v>
+        <v>40.3182103209804</v>
       </c>
     </row>
     <row r="46">
@@ -2472,13 +2472,13 @@
         <v>1994</v>
       </c>
       <c r="B46" t="n">
-        <v>19.7925439828897</v>
+        <v>19.4139306691216</v>
       </c>
       <c r="C46" t="n">
-        <v>55.5584588531504</v>
+        <v>55.5808838226744</v>
       </c>
       <c r="D46" t="n">
-        <v>155.954805648311</v>
+        <v>159.124635765963</v>
       </c>
     </row>
     <row r="47">
@@ -2486,13 +2486,13 @@
         <v>1995</v>
       </c>
       <c r="B47" t="n">
-        <v>4.55155175088758</v>
+        <v>4.49372026543548</v>
       </c>
       <c r="C47" t="n">
-        <v>13.1864083183006</v>
+        <v>13.2713638104487</v>
       </c>
       <c r="D47" t="n">
-        <v>38.202655677383</v>
+        <v>39.1944952034569</v>
       </c>
     </row>
     <row r="48">
@@ -2500,13 +2500,13 @@
         <v>1996</v>
       </c>
       <c r="B48" t="n">
-        <v>3.579665185274</v>
+        <v>3.51494220205943</v>
       </c>
       <c r="C48" t="n">
-        <v>10.0482626728545</v>
+        <v>10.063062318792</v>
       </c>
       <c r="D48" t="n">
-        <v>28.2058733196727</v>
+        <v>28.8099255721928</v>
       </c>
     </row>
     <row r="49">
@@ -2514,13 +2514,13 @@
         <v>1997</v>
       </c>
       <c r="B49" t="n">
-        <v>7.97364742296273</v>
+        <v>7.83912305610189</v>
       </c>
       <c r="C49" t="n">
-        <v>21.3126016280396</v>
+        <v>21.3876227973111</v>
       </c>
       <c r="D49" t="n">
-        <v>56.9660237104817</v>
+        <v>58.3522424187488</v>
       </c>
     </row>
     <row r="50">
@@ -2528,13 +2528,13 @@
         <v>1998</v>
       </c>
       <c r="B50" t="n">
-        <v>6.32566294294684</v>
+        <v>6.2075488705784</v>
       </c>
       <c r="C50" t="n">
-        <v>17.2787342587909</v>
+        <v>17.3009798736355</v>
       </c>
       <c r="D50" t="n">
-        <v>47.1973705015072</v>
+        <v>48.2193391995078</v>
       </c>
     </row>
     <row r="51">
@@ -2542,13 +2542,13 @@
         <v>1999</v>
       </c>
       <c r="B51" t="n">
-        <v>7.77723132226125</v>
+        <v>7.64446168937878</v>
       </c>
       <c r="C51" t="n">
-        <v>21.2437359528195</v>
+        <v>21.3057811690489</v>
       </c>
       <c r="D51" t="n">
-        <v>58.0278891719917</v>
+        <v>59.38106954661</v>
       </c>
     </row>
     <row r="52">
@@ -2556,13 +2556,13 @@
         <v>2000</v>
       </c>
       <c r="B52" t="n">
-        <v>6.3075027318525</v>
+        <v>6.19819318854311</v>
       </c>
       <c r="C52" t="n">
-        <v>17.6863755190623</v>
+        <v>17.7255176423868</v>
       </c>
       <c r="D52" t="n">
-        <v>49.5929835149538</v>
+        <v>50.6912201883817</v>
       </c>
     </row>
     <row r="53">
@@ -2570,13 +2570,13 @@
         <v>2001</v>
       </c>
       <c r="B53" t="n">
-        <v>6.50707761635584</v>
+        <v>6.37956470953037</v>
       </c>
       <c r="C53" t="n">
-        <v>17.7742737715269</v>
+        <v>17.7804030130585</v>
       </c>
       <c r="D53" t="n">
-        <v>48.5509512459324</v>
+        <v>49.5555332849741</v>
       </c>
     </row>
     <row r="54">
@@ -2584,13 +2584,13 @@
         <v>2002</v>
       </c>
       <c r="B54" t="n">
-        <v>14.0201902543139</v>
+        <v>13.7564326328846</v>
       </c>
       <c r="C54" t="n">
-        <v>37.4742842001017</v>
+        <v>37.5319267325116</v>
       </c>
       <c r="D54" t="n">
-        <v>100.164259602532</v>
+        <v>102.399042095206</v>
       </c>
     </row>
     <row r="55">
@@ -2598,13 +2598,13 @@
         <v>2003</v>
       </c>
       <c r="B55" t="n">
-        <v>9.06544269590236</v>
+        <v>8.8822266751432</v>
       </c>
       <c r="C55" t="n">
-        <v>23.7593689571346</v>
+        <v>23.7694528800941</v>
       </c>
       <c r="D55" t="n">
-        <v>62.2702753938768</v>
+        <v>63.6086998094886</v>
       </c>
     </row>
     <row r="56">
@@ -2612,13 +2612,13 @@
         <v>2004</v>
       </c>
       <c r="B56" t="n">
-        <v>9.4951009026236</v>
+        <v>9.3046281085428</v>
       </c>
       <c r="C56" t="n">
-        <v>24.8854483116005</v>
+        <v>24.8998283292788</v>
       </c>
       <c r="D56" t="n">
-        <v>65.2215857440993</v>
+        <v>66.6336626886051</v>
       </c>
     </row>
     <row r="57">
@@ -2626,13 +2626,13 @@
         <v>2005</v>
       </c>
       <c r="B57" t="n">
-        <v>5.0557764635599</v>
+        <v>4.97557328124186</v>
       </c>
       <c r="C57" t="n">
-        <v>12.8252711234394</v>
+        <v>12.9054169253984</v>
       </c>
       <c r="D57" t="n">
-        <v>32.5345830804212</v>
+        <v>33.4734866927312</v>
       </c>
     </row>
     <row r="58">
@@ -2640,13 +2640,13 @@
         <v>2006</v>
       </c>
       <c r="B58" t="n">
-        <v>6.62263115735633</v>
+        <v>6.48222452069402</v>
       </c>
       <c r="C58" t="n">
-        <v>16.799999120971</v>
+        <v>16.813300762544</v>
       </c>
       <c r="D58" t="n">
-        <v>42.6174980545483</v>
+        <v>43.6095790309799</v>
       </c>
     </row>
     <row r="59">
@@ -2654,13 +2654,13 @@
         <v>2007</v>
       </c>
       <c r="B59" t="n">
-        <v>7.76723671833805</v>
+        <v>7.61482498678343</v>
       </c>
       <c r="C59" t="n">
-        <v>19.9780172432951</v>
+        <v>20.0212865876203</v>
       </c>
       <c r="D59" t="n">
-        <v>51.3852206964531</v>
+        <v>52.6409887711612</v>
       </c>
     </row>
     <row r="60">
@@ -2668,13 +2668,13 @@
         <v>2008</v>
       </c>
       <c r="B60" t="n">
-        <v>5.40477628411261</v>
+        <v>5.26115151273384</v>
       </c>
       <c r="C60" t="n">
-        <v>13.5306850290623</v>
+        <v>13.4697813054042</v>
       </c>
       <c r="D60" t="n">
-        <v>33.8736383768285</v>
+        <v>34.485798018985</v>
       </c>
     </row>
     <row r="61">
@@ -2682,13 +2682,13 @@
         <v>2009</v>
       </c>
       <c r="B61" t="n">
-        <v>3.22151721778844</v>
+        <v>3.11722552825914</v>
       </c>
       <c r="C61" t="n">
-        <v>8.17021572772472</v>
+        <v>8.08347897768604</v>
       </c>
       <c r="D61" t="n">
-        <v>20.7208034366446</v>
+        <v>20.9617917569101</v>
       </c>
     </row>
     <row r="62">
@@ -2696,13 +2696,13 @@
         <v>2010</v>
       </c>
       <c r="B62" t="n">
-        <v>4.83648093899823</v>
+        <v>4.72428915404538</v>
       </c>
       <c r="C62" t="n">
-        <v>12.2562291913738</v>
+        <v>12.2406563611233</v>
       </c>
       <c r="D62" t="n">
-        <v>31.0587710126685</v>
+        <v>31.7156006470955</v>
       </c>
     </row>
     <row r="63">
@@ -2710,13 +2710,13 @@
         <v>2011</v>
       </c>
       <c r="B63" t="n">
-        <v>12.3327473899627</v>
+        <v>11.0508077132827</v>
       </c>
       <c r="C63" t="n">
-        <v>30.0782474043101</v>
+        <v>27.4771389467739</v>
       </c>
       <c r="D63" t="n">
-        <v>73.3576175938866</v>
+        <v>68.3201793288686</v>
       </c>
     </row>
     <row r="64">
@@ -2724,13 +2724,13 @@
         <v>2012</v>
       </c>
       <c r="B64" t="n">
-        <v>5.82389322583964</v>
+        <v>5.68031029807032</v>
       </c>
       <c r="C64" t="n">
-        <v>14.5631598084787</v>
+        <v>14.5246577460356</v>
       </c>
       <c r="D64" t="n">
-        <v>36.4164683971715</v>
+        <v>37.1398165890936</v>
       </c>
     </row>
     <row r="65">
@@ -2738,13 +2738,13 @@
         <v>2013</v>
       </c>
       <c r="B65" t="n">
-        <v>6.7671607134545</v>
+        <v>6.90754190551394</v>
       </c>
       <c r="C65" t="n">
-        <v>16.1614997640239</v>
+        <v>16.8420688579162</v>
       </c>
       <c r="D65" t="n">
-        <v>38.597291490837</v>
+        <v>41.0645765591903</v>
       </c>
     </row>
     <row r="66">
@@ -2752,13 +2752,13 @@
         <v>2014</v>
       </c>
       <c r="B66" t="n">
-        <v>12.7763572968221</v>
+        <v>12.5330439281045</v>
       </c>
       <c r="C66" t="n">
-        <v>30.2519502585688</v>
+        <v>30.3051278731831</v>
       </c>
       <c r="D66" t="n">
-        <v>71.6307843609347</v>
+        <v>73.2783496713456</v>
       </c>
     </row>
     <row r="67">
@@ -2766,13 +2766,13 @@
         <v>2015</v>
       </c>
       <c r="B67" t="n">
-        <v>5.00295993667391</v>
+        <v>4.89512858436899</v>
       </c>
       <c r="C67" t="n">
-        <v>11.8460443484558</v>
+        <v>11.836509834001</v>
       </c>
       <c r="D67" t="n">
-        <v>28.0491486003934</v>
+        <v>28.6208957815279</v>
       </c>
     </row>
     <row r="68">
@@ -2780,13 +2780,13 @@
         <v>2016</v>
       </c>
       <c r="B68" t="n">
-        <v>6.32477372080841</v>
+        <v>6.23200142412448</v>
       </c>
       <c r="C68" t="n">
-        <v>15.2438285529157</v>
+        <v>15.3292974712969</v>
       </c>
       <c r="D68" t="n">
-        <v>36.7403355769363</v>
+        <v>37.7065640668595</v>
       </c>
     </row>
     <row r="69">
@@ -2794,13 +2794,13 @@
         <v>2017</v>
       </c>
       <c r="B69" t="n">
-        <v>5.16131481488943</v>
+        <v>5.04160748244588</v>
       </c>
       <c r="C69" t="n">
-        <v>12.4298901185708</v>
+        <v>12.3910114199459</v>
       </c>
       <c r="D69" t="n">
-        <v>29.9346530682517</v>
+        <v>30.4540098656675</v>
       </c>
     </row>
     <row r="70">
@@ -2808,13 +2808,13 @@
         <v>2018</v>
       </c>
       <c r="B70" t="n">
-        <v>7.90842642515397</v>
+        <v>7.75272685505791</v>
       </c>
       <c r="C70" t="n">
-        <v>19.2414817913416</v>
+        <v>19.2429223002107</v>
       </c>
       <c r="D70" t="n">
-        <v>46.8152071755944</v>
+        <v>47.7625570427994</v>
       </c>
     </row>
     <row r="71">
@@ -2822,13 +2822,13 @@
         <v>2019</v>
       </c>
       <c r="B71" t="n">
-        <v>6.21448670275267</v>
+        <v>6.05249950287061</v>
       </c>
       <c r="C71" t="n">
-        <v>15.1218050923059</v>
+        <v>15.0247370931928</v>
       </c>
       <c r="D71" t="n">
-        <v>36.7961185190729</v>
+        <v>37.297437961374</v>
       </c>
     </row>
     <row r="72">
@@ -2836,13 +2836,13 @@
         <v>2020</v>
       </c>
       <c r="B72" t="n">
-        <v>5.3731189087101</v>
+        <v>5.30178186852774</v>
       </c>
       <c r="C72" t="n">
-        <v>13.6331487459812</v>
+        <v>13.7045001485905</v>
       </c>
       <c r="D72" t="n">
-        <v>34.5912212046445</v>
+        <v>35.4245664910524</v>
       </c>
     </row>
     <row r="73">
@@ -2850,13 +2850,13 @@
         <v>2021</v>
       </c>
       <c r="B73" t="n">
-        <v>0.283615836977768</v>
+        <v>0.658601440274251</v>
       </c>
       <c r="C73" t="n">
-        <v>1.10406186638558</v>
+        <v>3.77067150958418</v>
       </c>
       <c r="D73" t="n">
-        <v>4.29790034927548</v>
+        <v>21.5881150021009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-running latest version and inclusion
working on which years new series were included
</commit_message>
<xml_diff>
--- a/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
+++ b/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
@@ -402,22 +402,22 @@
         <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>58.4807609927735</v>
+        <v>58.5203681203694</v>
       </c>
       <c r="C2" t="n">
-        <v>169.724300119598</v>
+        <v>169.724396264616</v>
       </c>
       <c r="D2" t="n">
-        <v>492.578030143061</v>
+        <v>492.245206457643</v>
       </c>
       <c r="E2" t="n">
-        <v>45.3764559826106</v>
+        <v>45.765160151316</v>
       </c>
       <c r="F2" t="n">
-        <v>207.974661428798</v>
+        <v>207.984442354086</v>
       </c>
       <c r="G2" t="n">
-        <v>953.213706530961</v>
+        <v>945.206530870106</v>
       </c>
     </row>
     <row r="3">
@@ -425,22 +425,22 @@
         <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>74.2828367059565</v>
+        <v>74.3332889770088</v>
       </c>
       <c r="C3" t="n">
-        <v>215.585472158523</v>
+        <v>215.586008755722</v>
       </c>
       <c r="D3" t="n">
-        <v>625.677449419302</v>
+        <v>625.255895586666</v>
       </c>
       <c r="E3" t="n">
-        <v>25.5638530321481</v>
+        <v>25.7813320972424</v>
       </c>
       <c r="F3" t="n">
-        <v>117.167230539424</v>
+        <v>117.165895665204</v>
       </c>
       <c r="G3" t="n">
-        <v>537.014506186314</v>
+        <v>532.47237401274</v>
       </c>
     </row>
     <row r="4">
@@ -448,22 +448,22 @@
         <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>61.9072142208721</v>
+        <v>61.9491762755955</v>
       </c>
       <c r="C4" t="n">
-        <v>179.668636789625</v>
+        <v>179.668838050348</v>
       </c>
       <c r="D4" t="n">
-        <v>521.438728137095</v>
+        <v>521.086692464689</v>
       </c>
       <c r="E4" t="n">
-        <v>39.063577026526</v>
+        <v>39.3954660629964</v>
       </c>
       <c r="F4" t="n">
-        <v>179.040738866934</v>
+        <v>179.036717304178</v>
       </c>
       <c r="G4" t="n">
-        <v>820.6003805604</v>
+        <v>813.650639182673</v>
       </c>
     </row>
     <row r="5">
@@ -471,22 +471,22 @@
         <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>54.434849178556</v>
+        <v>54.4716634254717</v>
       </c>
       <c r="C5" t="n">
-        <v>157.98215553467</v>
+        <v>157.982092139295</v>
       </c>
       <c r="D5" t="n">
-        <v>458.499689886394</v>
+        <v>458.18944873708</v>
       </c>
       <c r="E5" t="n">
-        <v>48.9056401316216</v>
+        <v>49.3217430883044</v>
       </c>
       <c r="F5" t="n">
-        <v>224.150029526996</v>
+        <v>224.147696593552</v>
       </c>
       <c r="G5" t="n">
-        <v>1027.35053874628</v>
+        <v>1018.66208982603</v>
       </c>
     </row>
     <row r="6">
@@ -494,22 +494,22 @@
         <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>52.3537623807752</v>
+        <v>52.3893185467204</v>
       </c>
       <c r="C6" t="n">
-        <v>151.942374344323</v>
+        <v>151.942746545396</v>
       </c>
       <c r="D6" t="n">
-        <v>440.970888653227</v>
+        <v>440.67376457989</v>
       </c>
       <c r="E6" t="n">
-        <v>30.9472008180977</v>
+        <v>31.2441119665853</v>
       </c>
       <c r="F6" t="n">
-        <v>116.280889300707</v>
+        <v>116.290940812823</v>
       </c>
       <c r="G6" t="n">
-        <v>436.91335109882</v>
+        <v>432.836207013805</v>
       </c>
     </row>
     <row r="7">
@@ -517,22 +517,22 @@
         <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>32.7515369763285</v>
+        <v>32.7737108800033</v>
       </c>
       <c r="C7" t="n">
-        <v>95.0523145865934</v>
+        <v>95.0523462364114</v>
       </c>
       <c r="D7" t="n">
-        <v>275.863160705979</v>
+        <v>275.676701919014</v>
       </c>
       <c r="E7" t="n">
-        <v>20.8563638204237</v>
+        <v>21.0519803555137</v>
       </c>
       <c r="F7" t="n">
-        <v>78.3656184891436</v>
+        <v>78.3557108018942</v>
       </c>
       <c r="G7" t="n">
-        <v>294.450663311322</v>
+        <v>291.640848584682</v>
       </c>
     </row>
     <row r="8">
@@ -540,22 +540,22 @@
         <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>41.1456378537875</v>
+        <v>41.1699112936083</v>
       </c>
       <c r="C8" t="n">
-        <v>104.385237633791</v>
+        <v>104.385101132585</v>
       </c>
       <c r="D8" t="n">
-        <v>264.822187824219</v>
+        <v>264.665358658464</v>
       </c>
       <c r="E8" t="n">
-        <v>23.4652601292741</v>
+        <v>23.6871443649212</v>
       </c>
       <c r="F8" t="n">
-        <v>88.1682751064442</v>
+        <v>88.1638212765278</v>
       </c>
       <c r="G8" t="n">
-        <v>331.283126307542</v>
+        <v>328.146747549296</v>
       </c>
     </row>
     <row r="9">
@@ -563,22 +563,22 @@
         <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>30.1682710235373</v>
+        <v>30.1861357461074</v>
       </c>
       <c r="C9" t="n">
-        <v>76.5359903031052</v>
+        <v>76.5360607699082</v>
       </c>
       <c r="D9" t="n">
-        <v>194.16949042611</v>
+        <v>194.054934604554</v>
       </c>
       <c r="E9" t="n">
-        <v>25.9798026804227</v>
+        <v>26.2237387923519</v>
       </c>
       <c r="F9" t="n">
-        <v>97.6164072897283</v>
+        <v>97.6050546436963</v>
       </c>
       <c r="G9" t="n">
-        <v>366.783500605059</v>
+        <v>363.287125738813</v>
       </c>
     </row>
     <row r="10">
@@ -586,22 +586,22 @@
         <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>36.9055366902539</v>
+        <v>36.9273969241656</v>
       </c>
       <c r="C10" t="n">
-        <v>93.6282293424234</v>
+        <v>93.628330530083</v>
       </c>
       <c r="D10" t="n">
-        <v>237.531983435766</v>
+        <v>237.391882667845</v>
       </c>
       <c r="E10" t="n">
-        <v>33.0224108461631</v>
+        <v>33.3351275892259</v>
       </c>
       <c r="F10" t="n">
-        <v>124.078275208646</v>
+        <v>124.073724790529</v>
       </c>
       <c r="G10" t="n">
-        <v>466.211217905107</v>
+        <v>461.803817675244</v>
       </c>
     </row>
     <row r="11">
@@ -609,22 +609,22 @@
         <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>29.9294526096988</v>
+        <v>29.9471033570274</v>
       </c>
       <c r="C11" t="n">
-        <v>75.930115216945</v>
+        <v>75.93000116657</v>
       </c>
       <c r="D11" t="n">
-        <v>192.632403674173</v>
+        <v>192.518288277201</v>
       </c>
       <c r="E11" t="n">
-        <v>26.602571045345</v>
+        <v>26.8804369279122</v>
       </c>
       <c r="F11" t="n">
-        <v>89.5799642885223</v>
+        <v>89.5928940956807</v>
       </c>
       <c r="G11" t="n">
-        <v>301.646408095472</v>
+        <v>298.614441944017</v>
       </c>
     </row>
     <row r="12">
@@ -632,22 +632,22 @@
         <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>34.4504353375317</v>
+        <v>34.4707690833426</v>
       </c>
       <c r="C12" t="n">
-        <v>87.3997115338142</v>
+        <v>87.3996227784279</v>
       </c>
       <c r="D12" t="n">
-        <v>221.730422311152</v>
+        <v>221.59917706921</v>
       </c>
       <c r="E12" t="n">
-        <v>29.2325142233983</v>
+        <v>29.5328747990004</v>
       </c>
       <c r="F12" t="n">
-        <v>98.4358833487243</v>
+        <v>98.4335087745665</v>
       </c>
       <c r="G12" t="n">
-        <v>331.467319457861</v>
+        <v>328.080341504736</v>
       </c>
     </row>
     <row r="13">
@@ -655,22 +655,22 @@
         <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>21.4283094577875</v>
+        <v>21.4409099269619</v>
       </c>
       <c r="C13" t="n">
-        <v>54.3629723955214</v>
+        <v>54.3627975085779</v>
       </c>
       <c r="D13" t="n">
-        <v>137.917215238003</v>
+        <v>137.835276722204</v>
       </c>
       <c r="E13" t="n">
-        <v>25.1181531080212</v>
+        <v>25.3761105865637</v>
       </c>
       <c r="F13" t="n">
-        <v>84.8781572436116</v>
+        <v>84.8824515450684</v>
       </c>
       <c r="G13" t="n">
-        <v>286.816532493013</v>
+        <v>283.929665096741</v>
       </c>
     </row>
     <row r="14">
@@ -678,22 +678,22 @@
         <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>15.3468279574416</v>
+        <v>15.3558543453169</v>
       </c>
       <c r="C14" t="n">
-        <v>38.9344379337402</v>
+        <v>38.9343177686658</v>
       </c>
       <c r="D14" t="n">
-        <v>98.7754903762515</v>
+        <v>98.7168193981822</v>
       </c>
       <c r="E14" t="n">
-        <v>34.6830817623644</v>
+        <v>35.0595334102456</v>
       </c>
       <c r="F14" t="n">
-        <v>108.993736303878</v>
+        <v>108.993310144378</v>
       </c>
       <c r="G14" t="n">
-        <v>342.519578706242</v>
+        <v>338.839125929637</v>
       </c>
     </row>
     <row r="15">
@@ -701,22 +701,22 @@
         <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>14.3142369999141</v>
+        <v>14.3226593978062</v>
       </c>
       <c r="C15" t="n">
-        <v>36.3147859341035</v>
+        <v>36.3146823189701</v>
       </c>
       <c r="D15" t="n">
-        <v>92.1295125578595</v>
+        <v>92.074810640942</v>
       </c>
       <c r="E15" t="n">
-        <v>15.8616167601336</v>
+        <v>16.0437535044172</v>
       </c>
       <c r="F15" t="n">
-        <v>47.3950580231713</v>
+        <v>47.4019878415912</v>
       </c>
       <c r="G15" t="n">
-        <v>141.618068258059</v>
+        <v>140.051294774364</v>
       </c>
     </row>
     <row r="16">
@@ -724,22 +724,22 @@
         <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>27.2592720310957</v>
+        <v>27.2737744438532</v>
       </c>
       <c r="C16" t="n">
-        <v>63.1556723981053</v>
+        <v>63.1555730721424</v>
       </c>
       <c r="D16" t="n">
-        <v>146.32228445084</v>
+        <v>146.244019810381</v>
       </c>
       <c r="E16" t="n">
-        <v>41.699864569037</v>
+        <v>42.1493802448434</v>
       </c>
       <c r="F16" t="n">
-        <v>131.044411620797</v>
+        <v>131.034273036759</v>
       </c>
       <c r="G16" t="n">
-        <v>411.815193994462</v>
+        <v>407.360217648103</v>
       </c>
     </row>
     <row r="17">
@@ -747,22 +747,22 @@
         <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>44.010876899467</v>
+        <v>44.031467762427</v>
       </c>
       <c r="C17" t="n">
-        <v>90.7178936883747</v>
+        <v>90.7186661038016</v>
       </c>
       <c r="D17" t="n">
-        <v>186.993234741817</v>
+        <v>186.908972102805</v>
       </c>
       <c r="E17" t="n">
-        <v>18.8363050109327</v>
+        <v>19.0525204749844</v>
       </c>
       <c r="F17" t="n">
-        <v>54.2660377837805</v>
+        <v>54.2581442005292</v>
       </c>
       <c r="G17" t="n">
-        <v>156.336545572048</v>
+        <v>154.517414950466</v>
       </c>
     </row>
     <row r="18">
@@ -770,22 +770,22 @@
         <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>58.0701850628363</v>
+        <v>58.0969553260892</v>
       </c>
       <c r="C18" t="n">
-        <v>119.697793957349</v>
+        <v>119.6979923611</v>
       </c>
       <c r="D18" t="n">
-        <v>246.728366075509</v>
+        <v>246.615494647858</v>
       </c>
       <c r="E18" t="n">
-        <v>35.1274971494151</v>
+        <v>35.5457810538773</v>
       </c>
       <c r="F18" t="n">
-        <v>98.1538494577097</v>
+        <v>98.1535342609755</v>
       </c>
       <c r="G18" t="n">
-        <v>274.263154086603</v>
+        <v>271.034029982852</v>
       </c>
     </row>
     <row r="19">
@@ -793,22 +793,22 @@
         <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>62.3537881993427</v>
+        <v>62.3823282607324</v>
       </c>
       <c r="C19" t="n">
-        <v>128.589685906285</v>
+        <v>128.589437067268</v>
       </c>
       <c r="D19" t="n">
-        <v>265.185288640593</v>
+        <v>265.062939878847</v>
       </c>
       <c r="E19" t="n">
-        <v>26.6961093662282</v>
+        <v>27.016562193891</v>
       </c>
       <c r="F19" t="n">
-        <v>74.5976723190148</v>
+        <v>74.6036110632612</v>
       </c>
       <c r="G19" t="n">
-        <v>208.45032656537</v>
+        <v>206.010622067113</v>
       </c>
     </row>
     <row r="20">
@@ -816,22 +816,22 @@
         <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>54.4903082567314</v>
+        <v>54.5155556473616</v>
       </c>
       <c r="C20" t="n">
-        <v>113.707141741954</v>
+        <v>113.706709112145</v>
       </c>
       <c r="D20" t="n">
-        <v>237.277315852358</v>
+        <v>237.165622611418</v>
       </c>
       <c r="E20" t="n">
-        <v>19.7133470609332</v>
+        <v>19.9482703943109</v>
       </c>
       <c r="F20" t="n">
-        <v>55.0855476424909</v>
+        <v>55.0852101463323</v>
       </c>
       <c r="G20" t="n">
-        <v>153.927060163546</v>
+        <v>152.112454708403</v>
       </c>
     </row>
     <row r="21">
@@ -839,22 +839,22 @@
         <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>83.5034643869908</v>
+        <v>83.5426031827933</v>
       </c>
       <c r="C21" t="n">
-        <v>174.250074274867</v>
+        <v>174.250346818889</v>
       </c>
       <c r="D21" t="n">
-        <v>363.614714762982</v>
+        <v>363.445502171719</v>
       </c>
       <c r="E21" t="n">
-        <v>35.4057192586615</v>
+        <v>35.8477946582684</v>
       </c>
       <c r="F21" t="n">
-        <v>94.7580583226359</v>
+        <v>94.7656594098464</v>
       </c>
       <c r="G21" t="n">
-        <v>253.605626579086</v>
+        <v>250.518345381997</v>
       </c>
     </row>
     <row r="22">
@@ -862,22 +862,22 @@
         <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>66.9650687249105</v>
+        <v>66.9948045609279</v>
       </c>
       <c r="C22" t="n">
-        <v>134.028518760378</v>
+        <v>134.028975246608</v>
       </c>
       <c r="D22" t="n">
-        <v>268.253944678155</v>
+        <v>268.136705874243</v>
       </c>
       <c r="E22" t="n">
-        <v>29.8705862081605</v>
+        <v>30.2447241602705</v>
       </c>
       <c r="F22" t="n">
-        <v>81.5550730014752</v>
+        <v>81.5810480917608</v>
       </c>
       <c r="G22" t="n">
-        <v>222.66820898409</v>
+        <v>220.05383062785</v>
       </c>
     </row>
     <row r="23">
@@ -885,22 +885,22 @@
         <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>50.052420407291</v>
+        <v>50.0744268370124</v>
       </c>
       <c r="C23" t="n">
-        <v>100.178375013979</v>
+        <v>100.178277390486</v>
       </c>
       <c r="D23" t="n">
-        <v>200.503926459058</v>
+        <v>200.41541950326</v>
       </c>
       <c r="E23" t="n">
-        <v>22.0881534099729</v>
+        <v>22.3757034310169</v>
       </c>
       <c r="F23" t="n">
-        <v>58.1399822649144</v>
+        <v>58.1645415555138</v>
       </c>
       <c r="G23" t="n">
-        <v>153.034863305429</v>
+        <v>151.195867642465</v>
       </c>
     </row>
     <row r="24">
@@ -908,22 +908,22 @@
         <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>56.9865112781084</v>
+        <v>57.0088841113487</v>
       </c>
       <c r="C24" t="n">
-        <v>106.026797288717</v>
+        <v>106.026619861694</v>
       </c>
       <c r="D24" t="n">
-        <v>197.269169337994</v>
+        <v>197.19109213468</v>
       </c>
       <c r="E24" t="n">
-        <v>10.9779694613518</v>
+        <v>11.115650557114</v>
       </c>
       <c r="F24" t="n">
-        <v>29.3487690378275</v>
+        <v>29.3534523593756</v>
       </c>
       <c r="G24" t="n">
-        <v>78.4617088859782</v>
+        <v>77.5145962880865</v>
       </c>
     </row>
     <row r="25">
@@ -931,22 +931,22 @@
         <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>24.5230903113008</v>
+        <v>24.5332826526787</v>
       </c>
       <c r="C25" t="n">
-        <v>46.9232929898931</v>
+        <v>46.9234595542151</v>
       </c>
       <c r="D25" t="n">
-        <v>89.784582492065</v>
+        <v>89.7479186828531</v>
       </c>
       <c r="E25" t="n">
-        <v>8.8012573705171</v>
+        <v>8.91514722969266</v>
       </c>
       <c r="F25" t="n">
-        <v>23.529494294838</v>
+        <v>23.5425131564722</v>
       </c>
       <c r="G25" t="n">
-        <v>62.9043190607534</v>
+        <v>62.1694641089816</v>
       </c>
     </row>
     <row r="26">
@@ -954,22 +954,22 @@
         <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>31.336249078421</v>
+        <v>31.348518100205</v>
       </c>
       <c r="C26" t="n">
-        <v>58.3029572140669</v>
+        <v>58.3027972507925</v>
       </c>
       <c r="D26" t="n">
-        <v>108.476123335582</v>
+        <v>108.433073499726</v>
       </c>
       <c r="E26" t="n">
-        <v>3.6743961944365</v>
+        <v>3.72171299203157</v>
       </c>
       <c r="F26" t="n">
-        <v>9.67166994966412</v>
+        <v>9.67441004257524</v>
       </c>
       <c r="G26" t="n">
-        <v>25.4575703504345</v>
+        <v>25.1481535175528</v>
       </c>
     </row>
     <row r="27">
@@ -977,22 +977,22 @@
         <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>34.6194021106948</v>
+        <v>34.6325127587531</v>
       </c>
       <c r="C27" t="n">
-        <v>62.9239755529231</v>
+        <v>62.9239299506316</v>
       </c>
       <c r="D27" t="n">
-        <v>114.370164069405</v>
+        <v>114.326701848432</v>
       </c>
       <c r="E27" t="n">
-        <v>2.99627790421604</v>
+        <v>3.03448404305928</v>
       </c>
       <c r="F27" t="n">
-        <v>7.88674095921579</v>
+        <v>7.88799215927237</v>
       </c>
       <c r="G27" t="n">
-        <v>20.7593170414032</v>
+        <v>20.5044480121944</v>
       </c>
     </row>
     <row r="28">
@@ -1000,22 +1000,22 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>17.3542335999091</v>
+        <v>17.3612977284784</v>
       </c>
       <c r="C28" t="n">
-        <v>33.2061651890717</v>
+        <v>33.2059986958977</v>
       </c>
       <c r="D28" t="n">
-        <v>63.5377759678017</v>
+        <v>63.5112862319768</v>
       </c>
       <c r="E28" t="n">
-        <v>3.04261409028638</v>
+        <v>3.08119997342816</v>
       </c>
       <c r="F28" t="n">
-        <v>8.14236188865917</v>
+        <v>8.14458014968105</v>
       </c>
       <c r="G28" t="n">
-        <v>21.7898343853555</v>
+        <v>21.52868570253</v>
       </c>
     </row>
     <row r="29">
@@ -1023,22 +1023,22 @@
         <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>40.7256400546774</v>
+        <v>40.7412475740055</v>
       </c>
       <c r="C29" t="n">
-        <v>74.0338555681433</v>
+        <v>74.0341298550489</v>
       </c>
       <c r="D29" t="n">
-        <v>134.583809190623</v>
+        <v>134.533248483323</v>
       </c>
       <c r="E29" t="n">
-        <v>3.49306140814516</v>
+        <v>3.5380313968606</v>
       </c>
       <c r="F29" t="n">
-        <v>9.34801788137999</v>
+        <v>9.35224337797172</v>
       </c>
       <c r="G29" t="n">
-        <v>25.0168628890502</v>
+        <v>24.7212210378986</v>
       </c>
     </row>
     <row r="30">
@@ -1046,22 +1046,22 @@
         <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>50.5398006115292</v>
+        <v>50.5600546972978</v>
       </c>
       <c r="C30" t="n">
-        <v>94.1640155466307</v>
+        <v>94.1645420281229</v>
       </c>
       <c r="D30" t="n">
-        <v>175.443150083251</v>
+        <v>175.374829565602</v>
       </c>
       <c r="E30" t="n">
-        <v>3.56705716968312</v>
+        <v>3.62229007167019</v>
       </c>
       <c r="F30" t="n">
-        <v>9.38623349626358</v>
+        <v>9.41303628896164</v>
       </c>
       <c r="G30" t="n">
-        <v>24.6986171108121</v>
+        <v>24.4611144950228</v>
       </c>
     </row>
     <row r="31">
@@ -1069,22 +1069,22 @@
         <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>27.0879611025853</v>
+        <v>27.0992749159474</v>
       </c>
       <c r="C31" t="n">
-        <v>51.8627433183124</v>
+        <v>51.8630133872927</v>
       </c>
       <c r="D31" t="n">
-        <v>99.2966629830416</v>
+        <v>99.256240838666</v>
       </c>
       <c r="E31" t="n">
-        <v>1.52720277001036</v>
+        <v>1.54968647328441</v>
       </c>
       <c r="F31" t="n">
-        <v>3.96292319379576</v>
+        <v>3.97062439311369</v>
       </c>
       <c r="G31" t="n">
-        <v>10.2833497609606</v>
+        <v>10.1735792000399</v>
       </c>
     </row>
     <row r="32">
@@ -1092,22 +1092,22 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>23.2749612137037</v>
+        <v>23.2842087699054</v>
       </c>
       <c r="C32" t="n">
-        <v>43.3044511615176</v>
+        <v>43.3045829700014</v>
       </c>
       <c r="D32" t="n">
-        <v>80.5705097929938</v>
+        <v>80.5390006908685</v>
       </c>
       <c r="E32" t="n">
-        <v>5.47644873673987</v>
+        <v>5.5519864949092</v>
       </c>
       <c r="F32" t="n">
-        <v>14.6182953342461</v>
+        <v>14.6380681901082</v>
       </c>
       <c r="G32" t="n">
-        <v>39.0206443540005</v>
+        <v>38.5939412018978</v>
       </c>
     </row>
     <row r="33">
@@ -1115,22 +1115,22 @@
         <v>1991</v>
       </c>
       <c r="B33" t="n">
-        <v>10.5157556125317</v>
+        <v>10.5200677557481</v>
       </c>
       <c r="C33" t="n">
-        <v>20.1211949780063</v>
+        <v>20.1211546303426</v>
       </c>
       <c r="D33" t="n">
-        <v>38.5005607072559</v>
+        <v>38.4846251049044</v>
       </c>
       <c r="E33" t="n">
-        <v>1.23666252864004</v>
+        <v>1.25481116674617</v>
       </c>
       <c r="F33" t="n">
-        <v>3.295162313084</v>
+        <v>3.30245779474087</v>
       </c>
       <c r="G33" t="n">
-        <v>8.78015983997657</v>
+        <v>8.69152887308575</v>
       </c>
     </row>
     <row r="34">
@@ -1138,22 +1138,22 @@
         <v>1992</v>
       </c>
       <c r="B34" t="n">
-        <v>10.8027340214601</v>
+        <v>10.8071330956641</v>
       </c>
       <c r="C34" t="n">
-        <v>20.6703089678412</v>
+        <v>20.6702087075184</v>
       </c>
       <c r="D34" t="n">
-        <v>39.5512535972136</v>
+        <v>39.5347706214326</v>
       </c>
       <c r="E34" t="n">
-        <v>2.96835464130493</v>
+        <v>3.01957473651003</v>
       </c>
       <c r="F34" t="n">
-        <v>7.78986262226882</v>
+        <v>7.82499212064161</v>
       </c>
       <c r="G34" t="n">
-        <v>20.442961507842</v>
+        <v>20.2778559999718</v>
       </c>
     </row>
     <row r="35">
@@ -1161,22 +1161,22 @@
         <v>1993</v>
       </c>
       <c r="B35" t="n">
-        <v>11.7345933380748</v>
+        <v>11.7391520106596</v>
       </c>
       <c r="C35" t="n">
-        <v>21.8329095994255</v>
+        <v>21.8327832079961</v>
       </c>
       <c r="D35" t="n">
-        <v>40.6214282714028</v>
+        <v>40.6051835920109</v>
       </c>
       <c r="E35" t="n">
-        <v>2.63738612693718</v>
+        <v>2.67931856457513</v>
       </c>
       <c r="F35" t="n">
-        <v>6.92130088663745</v>
+        <v>6.9432448228524</v>
       </c>
       <c r="G35" t="n">
-        <v>18.1635921544034</v>
+        <v>17.9928767364441</v>
       </c>
     </row>
     <row r="36">
@@ -1184,22 +1184,22 @@
         <v>1994</v>
       </c>
       <c r="B36" t="n">
-        <v>13.0704707721123</v>
+        <v>13.075131356227</v>
       </c>
       <c r="C36" t="n">
-        <v>23.2860620663353</v>
+        <v>23.285825841138</v>
       </c>
       <c r="D36" t="n">
-        <v>41.4859339048574</v>
+        <v>41.4703049882226</v>
       </c>
       <c r="E36" t="n">
-        <v>2.58181306606276</v>
+        <v>2.6202955656442</v>
       </c>
       <c r="F36" t="n">
-        <v>6.77546032443279</v>
+        <v>6.79029133043282</v>
       </c>
       <c r="G36" t="n">
-        <v>17.7808622984353</v>
+        <v>17.5965097055054</v>
       </c>
     </row>
     <row r="37">
@@ -1207,22 +1207,22 @@
         <v>1995</v>
       </c>
       <c r="B37" t="n">
-        <v>17.2689786437063</v>
+        <v>17.275489639803</v>
       </c>
       <c r="C37" t="n">
-        <v>31.3957004254399</v>
+        <v>31.395620231949</v>
       </c>
       <c r="D37" t="n">
-        <v>57.0786510042504</v>
+        <v>57.056847030126</v>
       </c>
       <c r="E37" t="n">
-        <v>1.86576802701004</v>
+        <v>1.89350514854988</v>
       </c>
       <c r="F37" t="n">
-        <v>4.89634102784982</v>
+        <v>4.90687072210771</v>
       </c>
       <c r="G37" t="n">
-        <v>12.8494834909487</v>
+        <v>12.7157722818537</v>
       </c>
     </row>
     <row r="38">
@@ -1230,22 +1230,22 @@
         <v>1996</v>
       </c>
       <c r="B38" t="n">
-        <v>14.0704958183489</v>
+        <v>14.0755263222142</v>
       </c>
       <c r="C38" t="n">
-        <v>25.0709555668908</v>
+        <v>25.0707229137898</v>
       </c>
       <c r="D38" t="n">
-        <v>44.6716889832224</v>
+        <v>44.6548948175427</v>
       </c>
       <c r="E38" t="n">
-        <v>1.85848463485277</v>
+        <v>1.88053191870664</v>
       </c>
       <c r="F38" t="n">
-        <v>4.87722719841051</v>
+        <v>4.87325161009329</v>
       </c>
       <c r="G38" t="n">
-        <v>12.7993230069398</v>
+        <v>12.6286509785009</v>
       </c>
     </row>
     <row r="39">
@@ -1253,22 +1253,22 @@
         <v>1997</v>
       </c>
       <c r="B39" t="n">
-        <v>30.4197734368568</v>
+        <v>30.4306370323785</v>
       </c>
       <c r="C39" t="n">
-        <v>53.2480743026044</v>
+        <v>53.248159406007</v>
       </c>
       <c r="D39" t="n">
-        <v>93.2077098740106</v>
+        <v>93.174732987373</v>
       </c>
       <c r="E39" t="n">
-        <v>1.61752046356143</v>
+        <v>1.63929363415814</v>
       </c>
       <c r="F39" t="n">
-        <v>4.24486414949154</v>
+        <v>4.248101434817</v>
       </c>
       <c r="G39" t="n">
-        <v>11.1398106259286</v>
+        <v>11.0086231194096</v>
       </c>
     </row>
     <row r="40">
@@ -1276,22 +1276,22 @@
         <v>1998</v>
       </c>
       <c r="B40" t="n">
-        <v>9.21588003201352</v>
+        <v>9.21906920474681</v>
       </c>
       <c r="C40" t="n">
-        <v>16.1551818630861</v>
+        <v>16.1550140830677</v>
       </c>
       <c r="D40" t="n">
-        <v>28.3195853377839</v>
+        <v>28.3092006609234</v>
       </c>
       <c r="E40" t="n">
-        <v>1.18126006657878</v>
+        <v>1.19850393169109</v>
       </c>
       <c r="F40" t="n">
-        <v>3.0999845880193</v>
+        <v>3.10582934366446</v>
       </c>
       <c r="G40" t="n">
-        <v>8.13529951434812</v>
+        <v>8.04851419916204</v>
       </c>
     </row>
     <row r="41">
@@ -1299,22 +1299,22 @@
         <v>1999</v>
       </c>
       <c r="B41" t="n">
-        <v>9.38721011130263</v>
+        <v>9.39058361772542</v>
       </c>
       <c r="C41" t="n">
-        <v>16.7378240143492</v>
+        <v>16.7376923000794</v>
       </c>
       <c r="D41" t="n">
-        <v>29.8443040491878</v>
+        <v>29.8331131414805</v>
       </c>
       <c r="E41" t="n">
-        <v>2.47665376592071</v>
+        <v>2.51020297041268</v>
       </c>
       <c r="F41" t="n">
-        <v>6.6038815697226</v>
+        <v>6.61057050742767</v>
       </c>
       <c r="G41" t="n">
-        <v>17.6089417047397</v>
+        <v>17.4088083508594</v>
       </c>
     </row>
     <row r="42">
@@ -1322,22 +1322,22 @@
         <v>2000</v>
       </c>
       <c r="B42" t="n">
-        <v>7.68355269872122</v>
+        <v>7.6862460226818</v>
       </c>
       <c r="C42" t="n">
-        <v>13.4592744907925</v>
+        <v>13.4592011812858</v>
       </c>
       <c r="D42" t="n">
-        <v>23.5766027671869</v>
+        <v>23.5680845895069</v>
       </c>
       <c r="E42" t="n">
-        <v>1.80645492559393</v>
+        <v>1.83754667810155</v>
       </c>
       <c r="F42" t="n">
-        <v>4.74068546523516</v>
+        <v>4.76185871593116</v>
       </c>
       <c r="G42" t="n">
-        <v>12.4409960978698</v>
+        <v>12.3399849923357</v>
       </c>
     </row>
     <row r="43">
@@ -1345,22 +1345,22 @@
         <v>2001</v>
       </c>
       <c r="B43" t="n">
-        <v>5.21360936109646</v>
+        <v>5.21537713107292</v>
       </c>
       <c r="C43" t="n">
-        <v>8.99103359468584</v>
+        <v>8.99097082459017</v>
       </c>
       <c r="D43" t="n">
-        <v>15.505320690879</v>
+        <v>15.4998486853436</v>
       </c>
       <c r="E43" t="n">
-        <v>0.384441898407975</v>
+        <v>0.390280247147461</v>
       </c>
       <c r="F43" t="n">
-        <v>1.00889210917393</v>
+        <v>1.01138078214968</v>
       </c>
       <c r="G43" t="n">
-        <v>2.64763880359692</v>
+        <v>2.6209143147212</v>
       </c>
     </row>
     <row r="44">
@@ -1368,22 +1368,22 @@
         <v>2002</v>
       </c>
       <c r="B44" t="n">
-        <v>6.62285379063689</v>
+        <v>6.62516385477503</v>
       </c>
       <c r="C44" t="n">
-        <v>11.6019065290811</v>
+        <v>11.6018228643858</v>
       </c>
       <c r="D44" t="n">
-        <v>20.3242045445473</v>
+        <v>20.3168248706138</v>
       </c>
       <c r="E44" t="n">
-        <v>0.963805838026598</v>
+        <v>0.980403885901218</v>
       </c>
       <c r="F44" t="n">
-        <v>2.56763442603607</v>
+        <v>2.57956949793773</v>
       </c>
       <c r="G44" t="n">
-        <v>6.84032642846852</v>
+        <v>6.78718117133325</v>
       </c>
     </row>
     <row r="45">
@@ -1391,22 +1391,22 @@
         <v>2003</v>
       </c>
       <c r="B45" t="n">
-        <v>8.85346341219623</v>
+        <v>8.85649809565106</v>
       </c>
       <c r="C45" t="n">
-        <v>15.2680765771138</v>
+        <v>15.2680264504009</v>
       </c>
       <c r="D45" t="n">
-        <v>26.3302790683566</v>
+        <v>26.3210841545383</v>
       </c>
       <c r="E45" t="n">
-        <v>0.714207152475751</v>
+        <v>0.724065326043487</v>
       </c>
       <c r="F45" t="n">
-        <v>1.93768056685584</v>
+        <v>1.94059088337406</v>
       </c>
       <c r="G45" t="n">
-        <v>5.25702657297072</v>
+        <v>5.20104034978792</v>
       </c>
     </row>
     <row r="46">
@@ -1414,22 +1414,22 @@
         <v>2004</v>
       </c>
       <c r="B46" t="n">
-        <v>3.50027034063236</v>
+        <v>3.50154259111575</v>
       </c>
       <c r="C46" t="n">
-        <v>6.24202087664803</v>
+        <v>6.24199677770753</v>
       </c>
       <c r="D46" t="n">
-        <v>11.1313758175235</v>
+        <v>11.127245423708</v>
       </c>
       <c r="E46" t="n">
-        <v>0.247356437618706</v>
+        <v>0.250878787792961</v>
       </c>
       <c r="F46" t="n">
-        <v>0.649010660001027</v>
+        <v>0.649936175043669</v>
       </c>
       <c r="G46" t="n">
-        <v>1.70286587585912</v>
+        <v>1.68374949251986</v>
       </c>
     </row>
     <row r="47">
@@ -1437,22 +1437,22 @@
         <v>2005</v>
       </c>
       <c r="B47" t="n">
-        <v>3.85649211109577</v>
+        <v>3.85786197081026</v>
       </c>
       <c r="C47" t="n">
-        <v>6.87766009787329</v>
+        <v>6.877576485775</v>
       </c>
       <c r="D47" t="n">
-        <v>12.2656048707534</v>
+        <v>12.2609514481283</v>
       </c>
       <c r="E47" t="n">
-        <v>0.412297188875586</v>
+        <v>0.418479000526672</v>
       </c>
       <c r="F47" t="n">
-        <v>1.09840024955506</v>
+        <v>1.10099553796024</v>
       </c>
       <c r="G47" t="n">
-        <v>2.92624626307284</v>
+        <v>2.89665950521474</v>
       </c>
     </row>
     <row r="48">
@@ -1460,22 +1460,22 @@
         <v>2006</v>
       </c>
       <c r="B48" t="n">
-        <v>3.13034388775052</v>
+        <v>3.13141238054383</v>
       </c>
       <c r="C48" t="n">
-        <v>5.40126399474084</v>
+        <v>5.40123668571875</v>
       </c>
       <c r="D48" t="n">
-        <v>9.31963189573019</v>
+        <v>9.31635766544665</v>
       </c>
       <c r="E48" t="n">
-        <v>0.185893460227514</v>
+        <v>0.188516030406125</v>
       </c>
       <c r="F48" t="n">
-        <v>0.481648306518502</v>
+        <v>0.482146410231171</v>
       </c>
       <c r="G48" t="n">
-        <v>1.24794648982388</v>
+        <v>1.23313205989962</v>
       </c>
     </row>
     <row r="49">
@@ -1483,22 +1483,22 @@
         <v>2007</v>
       </c>
       <c r="B49" t="n">
-        <v>3.70745289360513</v>
+        <v>3.70876867361485</v>
       </c>
       <c r="C49" t="n">
-        <v>6.50447053046564</v>
+        <v>6.50445708331067</v>
       </c>
       <c r="D49" t="n">
-        <v>11.4116451633605</v>
+        <v>11.4075494245894</v>
       </c>
       <c r="E49" t="n">
-        <v>0.513417927894026</v>
+        <v>0.521261882030104</v>
       </c>
       <c r="F49" t="n">
-        <v>1.33026129700175</v>
+        <v>1.33317333634559</v>
       </c>
       <c r="G49" t="n">
-        <v>3.44669522071313</v>
+        <v>3.40970864361069</v>
       </c>
     </row>
     <row r="50">
@@ -1506,22 +1506,22 @@
         <v>2008</v>
       </c>
       <c r="B50" t="n">
-        <v>2.45282785105669</v>
+        <v>2.45373730224129</v>
       </c>
       <c r="C50" t="n">
-        <v>4.3778037689968</v>
+        <v>4.37781649366914</v>
       </c>
       <c r="D50" t="n">
-        <v>7.81349813505506</v>
+        <v>7.81064755169009</v>
       </c>
       <c r="E50" t="n">
-        <v>0.501783651238983</v>
+        <v>0.50629097101843</v>
       </c>
       <c r="F50" t="n">
-        <v>1.26739847585941</v>
+        <v>1.26211982135512</v>
       </c>
       <c r="G50" t="n">
-        <v>3.20117822221699</v>
+        <v>3.1463062441212</v>
       </c>
     </row>
     <row r="51">
@@ -1529,22 +1529,22 @@
         <v>2009</v>
       </c>
       <c r="B51" t="n">
-        <v>2.0561325534276</v>
+        <v>2.05691050874166</v>
       </c>
       <c r="C51" t="n">
-        <v>3.74005541354011</v>
+        <v>3.74004959000618</v>
       </c>
       <c r="D51" t="n">
-        <v>6.80307039204862</v>
+        <v>6.80047618807814</v>
       </c>
       <c r="E51" t="n">
-        <v>0.374130978923712</v>
+        <v>0.378521156791862</v>
       </c>
       <c r="F51" t="n">
-        <v>0.944975053070967</v>
+        <v>0.943605717139852</v>
       </c>
       <c r="G51" t="n">
-        <v>2.38680542706024</v>
+        <v>2.3522905746286</v>
       </c>
     </row>
     <row r="52">
@@ -1552,22 +1552,22 @@
         <v>2010</v>
       </c>
       <c r="B52" t="n">
-        <v>2.70996722926339</v>
+        <v>2.71088867251947</v>
       </c>
       <c r="C52" t="n">
-        <v>4.67644936231182</v>
+        <v>4.67641924169846</v>
       </c>
       <c r="D52" t="n">
-        <v>8.06990520110865</v>
+        <v>8.06705828454509</v>
       </c>
       <c r="E52" t="n">
-        <v>0.292749763125414</v>
+        <v>0.298348241824436</v>
       </c>
       <c r="F52" t="n">
-        <v>0.753629783244443</v>
+        <v>0.758340640663272</v>
       </c>
       <c r="G52" t="n">
-        <v>1.9400796233941</v>
+        <v>1.92754790095257</v>
       </c>
     </row>
     <row r="53">
@@ -1575,22 +1575,22 @@
         <v>2011</v>
       </c>
       <c r="B53" t="n">
-        <v>2.0840595275911</v>
+        <v>2.08477322966783</v>
       </c>
       <c r="C53" t="n">
-        <v>3.59635302729193</v>
+        <v>3.59633862674841</v>
       </c>
       <c r="D53" t="n">
-        <v>6.20603918730744</v>
+        <v>6.20386492602046</v>
       </c>
       <c r="E53" t="n">
-        <v>0.188665410827865</v>
+        <v>0.192397071940734</v>
       </c>
       <c r="F53" t="n">
-        <v>0.476227900075094</v>
+        <v>0.479314466085003</v>
       </c>
       <c r="G53" t="n">
-        <v>1.20209110835295</v>
+        <v>1.19410526927936</v>
       </c>
     </row>
     <row r="54">
@@ -1598,22 +1598,22 @@
         <v>2012</v>
       </c>
       <c r="B54" t="n">
-        <v>2.69614275646596</v>
+        <v>2.69708145960495</v>
       </c>
       <c r="C54" t="n">
-        <v>4.6616937309549</v>
+        <v>4.66169587882547</v>
       </c>
       <c r="D54" t="n">
-        <v>8.06017722507735</v>
+        <v>8.0573793532515</v>
       </c>
       <c r="E54" t="n">
-        <v>0.178039583813885</v>
+        <v>0.180428436514133</v>
       </c>
       <c r="F54" t="n">
-        <v>0.439478279479693</v>
+        <v>0.43617382195116</v>
       </c>
       <c r="G54" t="n">
-        <v>1.08482144249636</v>
+        <v>1.05442139072452</v>
       </c>
     </row>
     <row r="55">
@@ -1621,22 +1621,22 @@
         <v>2013</v>
       </c>
       <c r="B55" t="n">
-        <v>3.79811417548692</v>
+        <v>3.79939221855547</v>
       </c>
       <c r="C55" t="n">
-        <v>6.46892017820276</v>
+        <v>6.46890950622339</v>
       </c>
       <c r="D55" t="n">
-        <v>11.017817353159</v>
+        <v>11.0140748289519</v>
       </c>
       <c r="E55" t="n">
-        <v>0.451369994223271</v>
+        <v>0.439671415825975</v>
       </c>
       <c r="F55" t="n">
-        <v>1.12930477274834</v>
+        <v>1.0758917226411</v>
       </c>
       <c r="G55" t="n">
-        <v>2.82546311468221</v>
+        <v>2.63274563044555</v>
       </c>
     </row>
     <row r="56">
@@ -1644,22 +1644,22 @@
         <v>2014</v>
       </c>
       <c r="B56" t="n">
-        <v>5.97340316440069</v>
+        <v>5.97540670665384</v>
       </c>
       <c r="C56" t="n">
-        <v>10.1738564133023</v>
+        <v>10.1738286085454</v>
       </c>
       <c r="D56" t="n">
-        <v>17.3280375473997</v>
+        <v>17.3221328082651</v>
       </c>
       <c r="E56" t="n">
-        <v>1.29497021740123</v>
+        <v>1.25621281675549</v>
       </c>
       <c r="F56" t="n">
-        <v>3.21765327860389</v>
+        <v>3.05492931891714</v>
       </c>
       <c r="G56" t="n">
-        <v>7.99500442727365</v>
+        <v>7.42914975798729</v>
       </c>
     </row>
     <row r="57">
@@ -1667,22 +1667,22 @@
         <v>2015</v>
       </c>
       <c r="B57" t="n">
-        <v>4.59812673755341</v>
+        <v>4.59966726280687</v>
       </c>
       <c r="C57" t="n">
-        <v>7.83149570027857</v>
+        <v>7.83147134336892</v>
       </c>
       <c r="D57" t="n">
-        <v>13.338545978425</v>
+        <v>13.3339956778921</v>
       </c>
       <c r="E57" t="n">
-        <v>0.333949794344916</v>
+        <v>0.351769441380263</v>
       </c>
       <c r="F57" t="n">
-        <v>0.830231815570457</v>
+        <v>0.855870742786111</v>
       </c>
       <c r="G57" t="n">
-        <v>2.06403740699268</v>
+        <v>2.08237169631059</v>
       </c>
     </row>
     <row r="58">
@@ -1690,22 +1690,22 @@
         <v>2016</v>
       </c>
       <c r="B58" t="n">
-        <v>7.64620846780991</v>
+        <v>7.64885153155102</v>
       </c>
       <c r="C58" t="n">
-        <v>13.2168841303892</v>
+        <v>13.2168595286573</v>
       </c>
       <c r="D58" t="n">
-        <v>22.8460977557114</v>
+        <v>22.8381182560144</v>
       </c>
       <c r="E58" t="n">
-        <v>0.691194106787992</v>
+        <v>0.706965084475307</v>
       </c>
       <c r="F58" t="n">
-        <v>1.7470385231646</v>
+        <v>1.74571101941651</v>
       </c>
       <c r="G58" t="n">
-        <v>4.4157546649299</v>
+        <v>4.31068949547067</v>
       </c>
     </row>
     <row r="59">
@@ -1713,22 +1713,22 @@
         <v>2017</v>
       </c>
       <c r="B59" t="n">
-        <v>6.69257869260475</v>
+        <v>6.69482951923167</v>
       </c>
       <c r="C59" t="n">
-        <v>11.3987508928034</v>
+        <v>11.3987300674024</v>
       </c>
       <c r="D59" t="n">
-        <v>19.4142688317972</v>
+        <v>19.4076707668598</v>
       </c>
       <c r="E59" t="n">
-        <v>0.522339766675483</v>
+        <v>0.549874459086836</v>
       </c>
       <c r="F59" t="n">
-        <v>1.289359237114</v>
+        <v>1.32928516727708</v>
       </c>
       <c r="G59" t="n">
-        <v>3.18269323607527</v>
+        <v>3.21345904822944</v>
       </c>
     </row>
     <row r="60">
@@ -1736,22 +1736,22 @@
         <v>2018</v>
       </c>
       <c r="B60" t="n">
-        <v>7.11141871897334</v>
+        <v>7.1141620207033</v>
       </c>
       <c r="C60" t="n">
-        <v>13.1371796531813</v>
+        <v>13.1371273561421</v>
       </c>
       <c r="D60" t="n">
-        <v>24.2687846209225</v>
+        <v>24.2592331562385</v>
       </c>
       <c r="E60" t="n">
-        <v>0.803787881926017</v>
+        <v>0.811186857001668</v>
       </c>
       <c r="F60" t="n">
-        <v>1.98409425504354</v>
+        <v>1.96099062082851</v>
       </c>
       <c r="G60" t="n">
-        <v>4.89759811190972</v>
+        <v>4.7405652369556</v>
       </c>
     </row>
     <row r="61">
@@ -1759,22 +1759,22 @@
         <v>2019</v>
       </c>
       <c r="B61" t="n">
-        <v>3.51830491558193</v>
+        <v>3.51956622140865</v>
       </c>
       <c r="C61" t="n">
-        <v>6.18247753241634</v>
+        <v>6.18248071886489</v>
       </c>
       <c r="D61" t="n">
-        <v>10.8640465667288</v>
+        <v>10.8601644164655</v>
       </c>
       <c r="E61" t="n">
-        <v>0.668946084896688</v>
+        <v>0.669414875267091</v>
       </c>
       <c r="F61" t="n">
-        <v>1.66215140267597</v>
+        <v>1.62792092366523</v>
       </c>
       <c r="G61" t="n">
-        <v>4.12999993242261</v>
+        <v>3.9588700992784</v>
       </c>
     </row>
     <row r="62">
@@ -1782,22 +1782,22 @@
         <v>2020</v>
       </c>
       <c r="B62" t="n">
-        <v>4.87728479863872</v>
+        <v>4.8790261106236</v>
       </c>
       <c r="C62" t="n">
-        <v>8.5705202960762</v>
+        <v>8.57051209103148</v>
       </c>
       <c r="D62" t="n">
-        <v>15.0603914222839</v>
+        <v>15.0549875809393</v>
       </c>
       <c r="E62" t="n">
-        <v>0.297654547834972</v>
+        <v>0.297565239931755</v>
       </c>
       <c r="F62" t="n">
-        <v>0.751203695778358</v>
+        <v>0.733809560301186</v>
       </c>
       <c r="G62" t="n">
-        <v>1.89584535716193</v>
+        <v>1.80960810783181</v>
       </c>
     </row>
     <row r="63">
@@ -1805,22 +1805,22 @@
         <v>2021</v>
       </c>
       <c r="B63" t="n">
-        <v>3.4658774394981</v>
+        <v>3.46711196567276</v>
       </c>
       <c r="C63" t="n">
-        <v>6.09035030048302</v>
+        <v>6.09033941385496</v>
       </c>
       <c r="D63" t="n">
-        <v>10.7021576585135</v>
+        <v>10.6983087201102</v>
       </c>
       <c r="E63" t="n">
-        <v>0.273261215108193</v>
+        <v>0.336740960384031</v>
       </c>
       <c r="F63" t="n">
-        <v>0.480183316518411</v>
+        <v>0.59152019421106</v>
       </c>
       <c r="G63" t="n">
-        <v>0.843793428098929</v>
+        <v>1.0390661705082</v>
       </c>
     </row>
   </sheetData>
@@ -1856,13 +1856,13 @@
         <v>1950</v>
       </c>
       <c r="B2" t="n">
-        <v>47.9049576415035</v>
+        <v>46.5888780842677</v>
       </c>
       <c r="C2" t="n">
-        <v>181.845062807373</v>
+        <v>182.139812335102</v>
       </c>
       <c r="D2" t="n">
-        <v>690.275672820311</v>
+        <v>712.077916481716</v>
       </c>
     </row>
     <row r="3">
@@ -1870,13 +1870,13 @@
         <v>1951</v>
       </c>
       <c r="B3" t="n">
-        <v>75.8753779438938</v>
+        <v>73.6253462942716</v>
       </c>
       <c r="C3" t="n">
-        <v>262.242830599742</v>
+        <v>262.526230944689</v>
       </c>
       <c r="D3" t="n">
-        <v>906.371791015236</v>
+        <v>936.090971423881</v>
       </c>
     </row>
     <row r="4">
@@ -1884,13 +1884,13 @@
         <v>1952</v>
       </c>
       <c r="B4" t="n">
-        <v>72.942903763646</v>
+        <v>70.7314311982929</v>
       </c>
       <c r="C4" t="n">
-        <v>252.107522538972</v>
+        <v>252.207384772003</v>
       </c>
       <c r="D4" t="n">
-        <v>871.341825473294</v>
+        <v>899.297014861879</v>
       </c>
     </row>
     <row r="5">
@@ -1898,13 +1898,13 @@
         <v>1953</v>
       </c>
       <c r="B5" t="n">
-        <v>115.650396843975</v>
+        <v>112.273356842914</v>
       </c>
       <c r="C5" t="n">
-        <v>399.71448248698</v>
+        <v>400.333617307159</v>
       </c>
       <c r="D5" t="n">
-        <v>1381.50557084023</v>
+        <v>1427.47139350675</v>
       </c>
     </row>
     <row r="6">
@@ -1912,13 +1912,13 @@
         <v>1954</v>
       </c>
       <c r="B6" t="n">
-        <v>56.7734884370819</v>
+        <v>55.2346644006901</v>
       </c>
       <c r="C6" t="n">
-        <v>196.222288629276</v>
+        <v>196.950493171889</v>
       </c>
       <c r="D6" t="n">
-        <v>678.189549644837</v>
+        <v>702.267266064276</v>
       </c>
     </row>
     <row r="7">
@@ -1926,13 +1926,13 @@
         <v>1955</v>
       </c>
       <c r="B7" t="n">
-        <v>87.8671853124194</v>
+        <v>85.3025814254597</v>
       </c>
       <c r="C7" t="n">
-        <v>303.689286532449</v>
+        <v>304.163801172106</v>
       </c>
       <c r="D7" t="n">
-        <v>1049.6203153278</v>
+        <v>1084.55824428136</v>
       </c>
     </row>
     <row r="8">
@@ -1940,13 +1940,13 @@
         <v>1956</v>
       </c>
       <c r="B8" t="n">
-        <v>39.0748748821943</v>
+        <v>38.042119410264</v>
       </c>
       <c r="C8" t="n">
-        <v>135.051792453865</v>
+        <v>135.646957584515</v>
       </c>
       <c r="D8" t="n">
-        <v>466.770186724593</v>
+        <v>483.676971398465</v>
       </c>
     </row>
     <row r="9">
@@ -1954,13 +1954,13 @@
         <v>1957</v>
       </c>
       <c r="B9" t="n">
-        <v>45.3079575595545</v>
+        <v>43.9961760038632</v>
       </c>
       <c r="C9" t="n">
-        <v>156.5947658</v>
+        <v>156.877364163542</v>
       </c>
       <c r="D9" t="n">
-        <v>541.227678244476</v>
+        <v>559.378328351526</v>
       </c>
     </row>
     <row r="10">
@@ -1968,13 +1968,13 @@
         <v>1958</v>
       </c>
       <c r="B10" t="n">
-        <v>44.3524046584678</v>
+        <v>43.150439501884</v>
       </c>
       <c r="C10" t="n">
-        <v>153.29215427622</v>
+        <v>153.861717685638</v>
       </c>
       <c r="D10" t="n">
-        <v>529.813090036325</v>
+        <v>548.625424038646</v>
       </c>
     </row>
     <row r="11">
@@ -1982,13 +1982,13 @@
         <v>1959</v>
       </c>
       <c r="B11" t="n">
-        <v>96.5831732327912</v>
+        <v>93.9846246373864</v>
       </c>
       <c r="C11" t="n">
-        <v>333.813753858354</v>
+        <v>335.121401999082</v>
       </c>
       <c r="D11" t="n">
-        <v>1153.73743205171</v>
+        <v>1194.94390184706</v>
       </c>
     </row>
     <row r="12">
@@ -1996,13 +1996,13 @@
         <v>1960</v>
       </c>
       <c r="B12" t="n">
-        <v>51.3771157255092</v>
+        <v>49.898704279325</v>
       </c>
       <c r="C12" t="n">
-        <v>166.190589937837</v>
+        <v>166.757658857556</v>
       </c>
       <c r="D12" t="n">
-        <v>537.580045003829</v>
+        <v>557.291360352518</v>
       </c>
     </row>
     <row r="13">
@@ -2010,13 +2010,13 @@
         <v>1961</v>
       </c>
       <c r="B13" t="n">
-        <v>55.945770420126</v>
+        <v>54.2110020030467</v>
       </c>
       <c r="C13" t="n">
-        <v>180.96890919922</v>
+        <v>181.169028513152</v>
       </c>
       <c r="D13" t="n">
-        <v>585.383771656387</v>
+        <v>605.453057122143</v>
       </c>
     </row>
     <row r="14">
@@ -2024,13 +2024,13 @@
         <v>1962</v>
       </c>
       <c r="B14" t="n">
-        <v>55.0341121066753</v>
+        <v>53.2967661507886</v>
       </c>
       <c r="C14" t="n">
-        <v>178.019949710261</v>
+        <v>178.113722116561</v>
       </c>
       <c r="D14" t="n">
-        <v>575.84471306479</v>
+        <v>595.242456483378</v>
       </c>
     </row>
     <row r="15">
@@ -2038,13 +2038,13 @@
         <v>1963</v>
       </c>
       <c r="B15" t="n">
-        <v>46.486772304032</v>
+        <v>45.0423296750026</v>
       </c>
       <c r="C15" t="n">
-        <v>150.371697679344</v>
+        <v>150.528025819017</v>
       </c>
       <c r="D15" t="n">
-        <v>486.410355941335</v>
+        <v>503.053166220786</v>
       </c>
     </row>
     <row r="16">
@@ -2052,13 +2052,13 @@
         <v>1964</v>
       </c>
       <c r="B16" t="n">
-        <v>18.8411176662674</v>
+        <v>18.2070708597859</v>
       </c>
       <c r="C16" t="n">
-        <v>60.945742395782</v>
+        <v>60.8466403102479</v>
       </c>
       <c r="D16" t="n">
-        <v>197.142419147625</v>
+        <v>203.344824961494</v>
       </c>
     </row>
     <row r="17">
@@ -2066,13 +2066,13 @@
         <v>1965</v>
       </c>
       <c r="B17" t="n">
-        <v>35.4410955998756</v>
+        <v>34.2607694235953</v>
       </c>
       <c r="C17" t="n">
-        <v>114.642025006908</v>
+        <v>114.496874863834</v>
       </c>
       <c r="D17" t="n">
-        <v>370.834864871688</v>
+        <v>382.639811485261</v>
       </c>
     </row>
     <row r="18">
@@ -2080,13 +2080,13 @@
         <v>1966</v>
       </c>
       <c r="B18" t="n">
-        <v>48.3126027818442</v>
+        <v>46.7958810412926</v>
       </c>
       <c r="C18" t="n">
-        <v>156.277748261383</v>
+        <v>156.388260563632</v>
       </c>
       <c r="D18" t="n">
-        <v>505.51477658799</v>
+        <v>522.63762318178</v>
       </c>
     </row>
     <row r="19">
@@ -2094,13 +2094,13 @@
         <v>1967</v>
       </c>
       <c r="B19" t="n">
-        <v>36.0805087857076</v>
+        <v>34.868313847839</v>
       </c>
       <c r="C19" t="n">
-        <v>110.99450757344</v>
+        <v>110.950536936397</v>
       </c>
       <c r="D19" t="n">
-        <v>341.452521765731</v>
+        <v>353.043215688437</v>
       </c>
     </row>
     <row r="20">
@@ -2108,13 +2108,13 @@
         <v>1968</v>
       </c>
       <c r="B20" t="n">
-        <v>56.4169469834167</v>
+        <v>54.5195407402208</v>
       </c>
       <c r="C20" t="n">
-        <v>173.555514042578</v>
+        <v>173.480494211742</v>
       </c>
       <c r="D20" t="n">
-        <v>533.909012542589</v>
+        <v>552.012754754327</v>
       </c>
     </row>
     <row r="21">
@@ -2122,13 +2122,13 @@
         <v>1969</v>
       </c>
       <c r="B21" t="n">
-        <v>37.7063461207245</v>
+        <v>36.425239392479</v>
       </c>
       <c r="C21" t="n">
-        <v>115.996072697328</v>
+        <v>115.904654474218</v>
       </c>
       <c r="D21" t="n">
-        <v>356.838841878889</v>
+        <v>368.807155501127</v>
       </c>
     </row>
     <row r="22">
@@ -2136,13 +2136,13 @@
         <v>1970</v>
       </c>
       <c r="B22" t="n">
-        <v>19.2948780444987</v>
+        <v>18.629615456957</v>
       </c>
       <c r="C22" t="n">
-        <v>59.3568538614138</v>
+        <v>59.2792025128593</v>
       </c>
       <c r="D22" t="n">
-        <v>182.599552699933</v>
+        <v>188.625678220766</v>
       </c>
     </row>
     <row r="23">
@@ -2150,13 +2150,13 @@
         <v>1971</v>
       </c>
       <c r="B23" t="n">
-        <v>20.1963350142934</v>
+        <v>19.5025332431098</v>
       </c>
       <c r="C23" t="n">
-        <v>62.1300068969016</v>
+        <v>62.0568159500228</v>
       </c>
       <c r="D23" t="n">
-        <v>191.130606334126</v>
+        <v>197.464009308409</v>
       </c>
     </row>
     <row r="24">
@@ -2164,13 +2164,13 @@
         <v>1972</v>
       </c>
       <c r="B24" t="n">
-        <v>33.5222701795648</v>
+        <v>32.4434817312517</v>
       </c>
       <c r="C24" t="n">
-        <v>108.435161813324</v>
+        <v>108.423638185192</v>
       </c>
       <c r="D24" t="n">
-        <v>350.757399618164</v>
+        <v>362.343518328045</v>
       </c>
     </row>
     <row r="25">
@@ -2178,13 +2178,13 @@
         <v>1973</v>
       </c>
       <c r="B25" t="n">
-        <v>43.8628728839157</v>
+        <v>42.3749112273377</v>
       </c>
       <c r="C25" t="n">
-        <v>134.935402530554</v>
+        <v>134.83643556216</v>
       </c>
       <c r="D25" t="n">
-        <v>415.101922399599</v>
+        <v>429.04784525848</v>
       </c>
     </row>
     <row r="26">
@@ -2192,13 +2192,13 @@
         <v>1974</v>
       </c>
       <c r="B26" t="n">
-        <v>21.0966887643715</v>
+        <v>20.3898463474805</v>
       </c>
       <c r="C26" t="n">
-        <v>64.8997660964006</v>
+        <v>64.8802351090403</v>
       </c>
       <c r="D26" t="n">
-        <v>199.651219507053</v>
+        <v>206.448093627958</v>
       </c>
     </row>
     <row r="27">
@@ -2206,13 +2206,13 @@
         <v>1975</v>
       </c>
       <c r="B27" t="n">
-        <v>39.7536004121368</v>
+        <v>38.4260801577208</v>
       </c>
       <c r="C27" t="n">
-        <v>122.294043252637</v>
+        <v>122.2713046712</v>
       </c>
       <c r="D27" t="n">
-        <v>376.213295400327</v>
+        <v>389.065756502712</v>
       </c>
     </row>
     <row r="28">
@@ -2220,13 +2220,13 @@
         <v>1976</v>
       </c>
       <c r="B28" t="n">
-        <v>12.2009973102983</v>
+        <v>11.7659774315658</v>
       </c>
       <c r="C28" t="n">
-        <v>37.5339410096641</v>
+        <v>37.4391924803285</v>
       </c>
       <c r="D28" t="n">
-        <v>115.465702670703</v>
+        <v>119.13104047086</v>
       </c>
     </row>
     <row r="29">
@@ -2234,13 +2234,13 @@
         <v>1977</v>
       </c>
       <c r="B29" t="n">
-        <v>25.4148589094053</v>
+        <v>24.5844059514899</v>
       </c>
       <c r="C29" t="n">
-        <v>78.1837575088555</v>
+        <v>78.2272711116261</v>
       </c>
       <c r="D29" t="n">
-        <v>240.516776425675</v>
+        <v>248.91819463309</v>
       </c>
     </row>
     <row r="30">
@@ -2248,13 +2248,13 @@
         <v>1978</v>
       </c>
       <c r="B30" t="n">
-        <v>22.6434846257692</v>
+        <v>21.8912848124083</v>
       </c>
       <c r="C30" t="n">
-        <v>69.6581758508792</v>
+        <v>69.6577934557862</v>
       </c>
       <c r="D30" t="n">
-        <v>214.289520498535</v>
+        <v>221.650224311122</v>
       </c>
     </row>
     <row r="31">
@@ -2262,13 +2262,13 @@
         <v>1979</v>
       </c>
       <c r="B31" t="n">
-        <v>18.9029192233182</v>
+        <v>18.339492702917</v>
       </c>
       <c r="C31" t="n">
-        <v>58.151070522704</v>
+        <v>58.356035551627</v>
       </c>
       <c r="D31" t="n">
-        <v>178.890200131898</v>
+        <v>185.688172539314</v>
       </c>
     </row>
     <row r="32">
@@ -2276,13 +2276,13 @@
         <v>1980</v>
       </c>
       <c r="B32" t="n">
-        <v>33.3245045584003</v>
+        <v>32.2485825583568</v>
       </c>
       <c r="C32" t="n">
-        <v>98.6024452517102</v>
+        <v>98.8110375045268</v>
       </c>
       <c r="D32" t="n">
-        <v>291.750540284198</v>
+        <v>302.761248965061</v>
       </c>
     </row>
     <row r="33">
@@ -2290,13 +2290,13 @@
         <v>1981</v>
       </c>
       <c r="B33" t="n">
-        <v>13.8635251559416</v>
+        <v>13.4225418405674</v>
       </c>
       <c r="C33" t="n">
-        <v>41.0201891460639</v>
+        <v>41.1272428118147</v>
       </c>
       <c r="D33" t="n">
-        <v>121.372875848803</v>
+        <v>126.015632612136</v>
       </c>
     </row>
     <row r="34">
@@ -2304,13 +2304,13 @@
         <v>1982</v>
       </c>
       <c r="B34" t="n">
-        <v>17.5235998679521</v>
+        <v>16.9288523021132</v>
       </c>
       <c r="C34" t="n">
-        <v>51.8498270113687</v>
+        <v>51.8707281693912</v>
       </c>
       <c r="D34" t="n">
-        <v>153.416226195938</v>
+        <v>158.934131670995</v>
       </c>
     </row>
     <row r="35">
@@ -2318,13 +2318,13 @@
         <v>1983</v>
       </c>
       <c r="B35" t="n">
-        <v>15.8060353610768</v>
+        <v>15.2830849735131</v>
       </c>
       <c r="C35" t="n">
-        <v>46.7677991613023</v>
+        <v>46.8280266200829</v>
       </c>
       <c r="D35" t="n">
-        <v>138.379232263271</v>
+        <v>143.483078248378</v>
       </c>
     </row>
     <row r="36">
@@ -2332,13 +2332,13 @@
         <v>1984</v>
       </c>
       <c r="B36" t="n">
-        <v>11.8264172244314</v>
+        <v>11.4270821861325</v>
       </c>
       <c r="C36" t="n">
-        <v>34.9926779812225</v>
+        <v>35.0130690059939</v>
       </c>
       <c r="D36" t="n">
-        <v>103.538331944517</v>
+        <v>107.281542326371</v>
       </c>
     </row>
     <row r="37">
@@ -2346,13 +2346,13 @@
         <v>1985</v>
       </c>
       <c r="B37" t="n">
-        <v>22.0891587757604</v>
+        <v>21.4504444367256</v>
       </c>
       <c r="C37" t="n">
-        <v>65.3053948513851</v>
+        <v>65.6695090940473</v>
       </c>
       <c r="D37" t="n">
-        <v>193.0718430697</v>
+        <v>201.044059360826</v>
       </c>
     </row>
     <row r="38">
@@ -2360,13 +2360,13 @@
         <v>1986</v>
       </c>
       <c r="B38" t="n">
-        <v>17.1477484012885</v>
+        <v>16.5872457850743</v>
       </c>
       <c r="C38" t="n">
-        <v>49.1356333453511</v>
+        <v>49.2592189988469</v>
       </c>
       <c r="D38" t="n">
-        <v>140.794605084558</v>
+        <v>146.285325955667</v>
       </c>
     </row>
     <row r="39">
@@ -2374,13 +2374,13 @@
         <v>1987</v>
       </c>
       <c r="B39" t="n">
-        <v>16.521033639494</v>
+        <v>15.9862136200275</v>
       </c>
       <c r="C39" t="n">
-        <v>47.3398275038487</v>
+        <v>47.474331053795</v>
       </c>
       <c r="D39" t="n">
-        <v>135.648853273734</v>
+        <v>140.98473613425</v>
       </c>
     </row>
     <row r="40">
@@ -2388,13 +2388,13 @@
         <v>1988</v>
       </c>
       <c r="B40" t="n">
-        <v>21.3476395946478</v>
+        <v>20.6735646091526</v>
       </c>
       <c r="C40" t="n">
-        <v>61.1701179282813</v>
+        <v>61.3943785342234</v>
       </c>
       <c r="D40" t="n">
-        <v>175.278550622429</v>
+        <v>182.32316423723</v>
       </c>
     </row>
     <row r="41">
@@ -2402,13 +2402,13 @@
         <v>1989</v>
       </c>
       <c r="B41" t="n">
-        <v>11.8150281185317</v>
+        <v>11.4453260768861</v>
       </c>
       <c r="C41" t="n">
-        <v>36.3275352061576</v>
+        <v>36.4051430928974</v>
       </c>
       <c r="D41" t="n">
-        <v>111.695867408449</v>
+        <v>115.797001737753</v>
       </c>
     </row>
     <row r="42">
@@ -2416,13 +2416,13 @@
         <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>10.8076831978728</v>
+        <v>10.4715484754321</v>
       </c>
       <c r="C42" t="n">
-        <v>31.9590356077444</v>
+        <v>32.0650247866808</v>
       </c>
       <c r="D42" t="n">
-        <v>94.5049867096496</v>
+        <v>98.1866069743836</v>
       </c>
     </row>
     <row r="43">
@@ -2430,13 +2430,13 @@
         <v>1991</v>
       </c>
       <c r="B43" t="n">
-        <v>12.1572344932185</v>
+        <v>11.8118785399295</v>
       </c>
       <c r="C43" t="n">
-        <v>37.3797133304486</v>
+        <v>37.5710683604259</v>
       </c>
       <c r="D43" t="n">
-        <v>114.930987754322</v>
+        <v>119.505561538921</v>
       </c>
     </row>
     <row r="44">
@@ -2444,13 +2444,13 @@
         <v>1992</v>
       </c>
       <c r="B44" t="n">
-        <v>6.18091230672056</v>
+        <v>5.99655278398007</v>
       </c>
       <c r="C44" t="n">
-        <v>17.6955699849274</v>
+        <v>17.7927473004229</v>
       </c>
       <c r="D44" t="n">
-        <v>50.6613233698515</v>
+        <v>52.7939747887259</v>
       </c>
     </row>
     <row r="45">
@@ -2458,13 +2458,13 @@
         <v>1993</v>
       </c>
       <c r="B45" t="n">
-        <v>4.91900538283597</v>
+        <v>4.79875156345644</v>
       </c>
       <c r="C45" t="n">
-        <v>14.0828084413307</v>
+        <v>14.2386762865145</v>
       </c>
       <c r="D45" t="n">
-        <v>40.3182103209804</v>
+        <v>42.2484681090934</v>
       </c>
     </row>
     <row r="46">
@@ -2472,13 +2472,13 @@
         <v>1994</v>
       </c>
       <c r="B46" t="n">
-        <v>19.4139306691216</v>
+        <v>18.729072038249</v>
       </c>
       <c r="C46" t="n">
-        <v>55.5808838226744</v>
+        <v>55.5722025558154</v>
       </c>
       <c r="D46" t="n">
-        <v>159.124635765963</v>
+        <v>164.891762421418</v>
       </c>
     </row>
     <row r="47">
@@ -2486,13 +2486,13 @@
         <v>1995</v>
       </c>
       <c r="B47" t="n">
-        <v>4.49372026543548</v>
+        <v>4.36672713790918</v>
       </c>
       <c r="C47" t="n">
-        <v>13.2713638104487</v>
+        <v>13.3554128057449</v>
       </c>
       <c r="D47" t="n">
-        <v>39.1944952034569</v>
+        <v>40.846850645506</v>
       </c>
     </row>
     <row r="48">
@@ -2500,13 +2500,13 @@
         <v>1996</v>
       </c>
       <c r="B48" t="n">
-        <v>3.51494220205943</v>
+        <v>3.40308407744005</v>
       </c>
       <c r="C48" t="n">
-        <v>10.063062318792</v>
+        <v>10.0975038848562</v>
       </c>
       <c r="D48" t="n">
-        <v>28.8099255721928</v>
+        <v>29.9609361345501</v>
       </c>
     </row>
     <row r="49">
@@ -2514,13 +2514,13 @@
         <v>1997</v>
       </c>
       <c r="B49" t="n">
-        <v>7.83912305610189</v>
+        <v>7.60037932373125</v>
       </c>
       <c r="C49" t="n">
-        <v>21.3876227973111</v>
+        <v>21.5212002739427</v>
       </c>
       <c r="D49" t="n">
-        <v>58.3522424187488</v>
+        <v>60.9393349335847</v>
       </c>
     </row>
     <row r="50">
@@ -2528,13 +2528,13 @@
         <v>1998</v>
       </c>
       <c r="B50" t="n">
-        <v>6.2075488705784</v>
+        <v>6.05603064131675</v>
       </c>
       <c r="C50" t="n">
-        <v>17.3009798736355</v>
+        <v>17.5073043817627</v>
       </c>
       <c r="D50" t="n">
-        <v>48.2193391995078</v>
+        <v>50.611650579272</v>
       </c>
     </row>
     <row r="51">
@@ -2542,13 +2542,13 @@
         <v>1999</v>
       </c>
       <c r="B51" t="n">
-        <v>7.64446168937878</v>
+        <v>7.43676870692541</v>
       </c>
       <c r="C51" t="n">
-        <v>21.3057811690489</v>
+        <v>21.4988630474637</v>
       </c>
       <c r="D51" t="n">
-        <v>59.38106954661</v>
+        <v>62.150798357246</v>
       </c>
     </row>
     <row r="52">
@@ -2556,13 +2556,13 @@
         <v>2000</v>
       </c>
       <c r="B52" t="n">
-        <v>6.19819318854311</v>
+        <v>6.01374312484996</v>
       </c>
       <c r="C52" t="n">
-        <v>17.7255176423868</v>
+        <v>17.825428708784</v>
       </c>
       <c r="D52" t="n">
-        <v>50.6912201883817</v>
+        <v>52.8366280460092</v>
       </c>
     </row>
     <row r="53">
@@ -2570,13 +2570,13 @@
         <v>2001</v>
       </c>
       <c r="B53" t="n">
-        <v>6.37956470953037</v>
+        <v>6.221295183602</v>
       </c>
       <c r="C53" t="n">
-        <v>17.7804030130585</v>
+        <v>17.9850656112982</v>
       </c>
       <c r="D53" t="n">
-        <v>49.5555332849741</v>
+        <v>51.9928046325917</v>
       </c>
     </row>
     <row r="54">
@@ -2584,13 +2584,13 @@
         <v>2002</v>
       </c>
       <c r="B54" t="n">
-        <v>13.7564326328846</v>
+        <v>13.3089659609651</v>
       </c>
       <c r="C54" t="n">
-        <v>37.5319267325116</v>
+        <v>37.6856087946411</v>
       </c>
       <c r="D54" t="n">
-        <v>102.399042095206</v>
+        <v>106.710402174606</v>
       </c>
     </row>
     <row r="55">
@@ -2598,13 +2598,13 @@
         <v>2003</v>
       </c>
       <c r="B55" t="n">
-        <v>8.8822266751432</v>
+        <v>8.58623342055338</v>
       </c>
       <c r="C55" t="n">
-        <v>23.7694528800941</v>
+        <v>23.8617139893529</v>
       </c>
       <c r="D55" t="n">
-        <v>63.6086998094886</v>
+        <v>66.3132908950178</v>
       </c>
     </row>
     <row r="56">
@@ -2612,13 +2612,13 @@
         <v>2004</v>
       </c>
       <c r="B56" t="n">
-        <v>9.3046281085428</v>
+        <v>9.26752685806272</v>
       </c>
       <c r="C56" t="n">
-        <v>24.8998283292788</v>
+        <v>25.7550737843192</v>
       </c>
       <c r="D56" t="n">
-        <v>66.6336626886051</v>
+        <v>71.5750637462289</v>
       </c>
     </row>
     <row r="57">
@@ -2626,13 +2626,13 @@
         <v>2005</v>
       </c>
       <c r="B57" t="n">
-        <v>4.97557328124186</v>
+        <v>4.77102103831796</v>
       </c>
       <c r="C57" t="n">
-        <v>12.9054169253984</v>
+        <v>12.8617962898671</v>
       </c>
       <c r="D57" t="n">
-        <v>33.4734866927312</v>
+        <v>34.6730401047155</v>
       </c>
     </row>
     <row r="58">
@@ -2640,13 +2640,13 @@
         <v>2006</v>
       </c>
       <c r="B58" t="n">
-        <v>6.48222452069402</v>
+        <v>6.34366201398147</v>
       </c>
       <c r="C58" t="n">
-        <v>16.813300762544</v>
+        <v>17.1013474684579</v>
       </c>
       <c r="D58" t="n">
-        <v>43.6095790309799</v>
+        <v>46.1020912829774</v>
       </c>
     </row>
     <row r="59">
@@ -2654,13 +2654,13 @@
         <v>2007</v>
       </c>
       <c r="B59" t="n">
-        <v>7.61482498678343</v>
+        <v>7.43584256213831</v>
       </c>
       <c r="C59" t="n">
-        <v>20.0212865876203</v>
+        <v>20.3113032345941</v>
       </c>
       <c r="D59" t="n">
-        <v>52.6409887711612</v>
+        <v>55.4811422700427</v>
       </c>
     </row>
     <row r="60">
@@ -2668,13 +2668,13 @@
         <v>2008</v>
       </c>
       <c r="B60" t="n">
-        <v>5.26115151273384</v>
+        <v>5.14605907377298</v>
       </c>
       <c r="C60" t="n">
-        <v>13.4697813054042</v>
+        <v>13.6987728759957</v>
       </c>
       <c r="D60" t="n">
-        <v>34.485798018985</v>
+        <v>36.466036556889</v>
       </c>
     </row>
     <row r="61">
@@ -2682,13 +2682,13 @@
         <v>2009</v>
       </c>
       <c r="B61" t="n">
-        <v>3.11722552825914</v>
+        <v>3.04391657083825</v>
       </c>
       <c r="C61" t="n">
-        <v>8.08347897768604</v>
+        <v>8.20329082192807</v>
       </c>
       <c r="D61" t="n">
-        <v>20.9617917569101</v>
+        <v>22.1076953796396</v>
       </c>
     </row>
     <row r="62">
@@ -2696,13 +2696,13 @@
         <v>2010</v>
       </c>
       <c r="B62" t="n">
-        <v>4.72428915404538</v>
+        <v>4.57419227651799</v>
       </c>
       <c r="C62" t="n">
-        <v>12.2406563611233</v>
+        <v>12.3179786832975</v>
       </c>
       <c r="D62" t="n">
-        <v>31.7156006470955</v>
+        <v>33.1714518475979</v>
       </c>
     </row>
     <row r="63">
@@ -2710,13 +2710,13 @@
         <v>2011</v>
       </c>
       <c r="B63" t="n">
-        <v>11.0508077132827</v>
+        <v>10.1935278585845</v>
       </c>
       <c r="C63" t="n">
-        <v>27.4771389467739</v>
+        <v>27.4426330337202</v>
       </c>
       <c r="D63" t="n">
-        <v>68.3201793288686</v>
+        <v>73.880026451216</v>
       </c>
     </row>
     <row r="64">
@@ -2724,13 +2724,13 @@
         <v>2012</v>
       </c>
       <c r="B64" t="n">
-        <v>5.68031029807032</v>
+        <v>5.45720568919004</v>
       </c>
       <c r="C64" t="n">
-        <v>14.5246577460356</v>
+        <v>13.5702107326031</v>
       </c>
       <c r="D64" t="n">
-        <v>37.1398165890936</v>
+        <v>33.7444893623915</v>
       </c>
     </row>
     <row r="65">
@@ -2738,13 +2738,13 @@
         <v>2013</v>
       </c>
       <c r="B65" t="n">
-        <v>6.90754190551394</v>
+        <v>5.65953966690286</v>
       </c>
       <c r="C65" t="n">
-        <v>16.8420688579162</v>
+        <v>13.9887334700302</v>
       </c>
       <c r="D65" t="n">
-        <v>41.0645765591903</v>
+        <v>34.5760743121764</v>
       </c>
     </row>
     <row r="66">
@@ -2752,13 +2752,13 @@
         <v>2014</v>
       </c>
       <c r="B66" t="n">
-        <v>12.5330439281045</v>
+        <v>11.1414035889683</v>
       </c>
       <c r="C66" t="n">
-        <v>30.3051278731831</v>
+        <v>28.5100135011109</v>
       </c>
       <c r="D66" t="n">
-        <v>73.2783496713456</v>
+        <v>72.9549794460673</v>
       </c>
     </row>
     <row r="67">
@@ -2766,13 +2766,13 @@
         <v>2015</v>
       </c>
       <c r="B67" t="n">
-        <v>4.89512858436899</v>
+        <v>4.59422975340505</v>
       </c>
       <c r="C67" t="n">
-        <v>11.836509834001</v>
+        <v>11.291518175028</v>
       </c>
       <c r="D67" t="n">
-        <v>28.6208957815279</v>
+        <v>27.7518516792701</v>
       </c>
     </row>
     <row r="68">
@@ -2780,13 +2780,13 @@
         <v>2016</v>
       </c>
       <c r="B68" t="n">
-        <v>6.23200142412448</v>
+        <v>6.15125281196264</v>
       </c>
       <c r="C68" t="n">
-        <v>15.3292974712969</v>
+        <v>15.2923792050218</v>
       </c>
       <c r="D68" t="n">
-        <v>37.7065640668595</v>
+        <v>38.0177614055125</v>
       </c>
     </row>
     <row r="69">
@@ -2794,13 +2794,13 @@
         <v>2017</v>
       </c>
       <c r="B69" t="n">
-        <v>5.04160748244588</v>
+        <v>7.14888886294894</v>
       </c>
       <c r="C69" t="n">
-        <v>12.3910114199459</v>
+        <v>17.7623528638052</v>
       </c>
       <c r="D69" t="n">
-        <v>30.4540098656675</v>
+        <v>44.1328974763476</v>
       </c>
     </row>
     <row r="70">
@@ -2808,13 +2808,13 @@
         <v>2018</v>
       </c>
       <c r="B70" t="n">
-        <v>7.75272685505791</v>
+        <v>7.18877471564012</v>
       </c>
       <c r="C70" t="n">
-        <v>19.2429223002107</v>
+        <v>17.9780972085992</v>
       </c>
       <c r="D70" t="n">
-        <v>47.7625570427994</v>
+        <v>44.9606493494157</v>
       </c>
     </row>
     <row r="71">
@@ -2822,13 +2822,13 @@
         <v>2019</v>
       </c>
       <c r="B71" t="n">
-        <v>6.05249950287061</v>
+        <v>5.98313700617119</v>
       </c>
       <c r="C71" t="n">
-        <v>15.0247370931928</v>
+        <v>14.96547206402</v>
       </c>
       <c r="D71" t="n">
-        <v>37.297437961374</v>
+        <v>37.432763760542</v>
       </c>
     </row>
     <row r="72">
@@ -2836,13 +2836,13 @@
         <v>2020</v>
       </c>
       <c r="B72" t="n">
-        <v>5.30178186852774</v>
+        <v>6.42628938774986</v>
       </c>
       <c r="C72" t="n">
-        <v>13.7045001485905</v>
+        <v>16.6728755652082</v>
       </c>
       <c r="D72" t="n">
-        <v>35.4245664910524</v>
+        <v>43.2574325306338</v>
       </c>
     </row>
     <row r="73">
@@ -2850,13 +2850,13 @@
         <v>2021</v>
       </c>
       <c r="B73" t="n">
-        <v>0.658601440274251</v>
+        <v>1.43930960426354</v>
       </c>
       <c r="C73" t="n">
-        <v>3.77067150958418</v>
+        <v>5.70655857975986</v>
       </c>
       <c r="D73" t="n">
-        <v>21.5881150021009</v>
+        <v>22.6252994684167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in the branch test historical period
</commit_message>
<xml_diff>
--- a/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
+++ b/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
@@ -399,1428 +399,1658 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1960</v>
+        <v>1950</v>
       </c>
       <c r="B2" t="n">
-        <v>61.493762969138</v>
+        <v>22.5072647753047</v>
       </c>
       <c r="C2" t="n">
-        <v>152.048111818896</v>
+        <v>78.0591878051258</v>
       </c>
       <c r="D2" t="n">
-        <v>375.95078250934</v>
+        <v>270.723113698004</v>
       </c>
       <c r="E2" t="n">
-        <v>50.8345557658664</v>
+        <v>6.19797829236237</v>
       </c>
       <c r="F2" t="n">
-        <v>208.076635205517</v>
+        <v>25.2232413607601</v>
       </c>
       <c r="G2" t="n">
-        <v>851.701868269726</v>
+        <v>102.64829509441</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1961</v>
+        <v>1951</v>
       </c>
       <c r="B3" t="n">
-        <v>61.1403408017282</v>
+        <v>18.282908024978</v>
       </c>
       <c r="C3" t="n">
-        <v>130.372135710347</v>
+        <v>63.4083690485344</v>
       </c>
       <c r="D3" t="n">
-        <v>277.99802138487</v>
+        <v>219.911474690032</v>
       </c>
       <c r="E3" t="n">
-        <v>28.6896982592744</v>
+        <v>7.77976896214032</v>
       </c>
       <c r="F3" t="n">
-        <v>117.433029342214</v>
+        <v>31.6604836297711</v>
       </c>
       <c r="G3" t="n">
-        <v>480.678334636417</v>
+        <v>128.845243161982</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1962</v>
+        <v>1952</v>
       </c>
       <c r="B4" t="n">
-        <v>73.9868111169839</v>
+        <v>7.43035124769655</v>
       </c>
       <c r="C4" t="n">
-        <v>150.558796341544</v>
+        <v>42.1616957334171</v>
       </c>
       <c r="D4" t="n">
-        <v>306.378269499588</v>
+        <v>239.236144814595</v>
       </c>
       <c r="E4" t="n">
-        <v>43.8548505490427</v>
+        <v>27.2461100460727</v>
       </c>
       <c r="F4" t="n">
-        <v>179.507219099431</v>
+        <v>110.880544819072</v>
       </c>
       <c r="G4" t="n">
-        <v>734.76117933127</v>
+        <v>451.238551065985</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1963</v>
+        <v>1953</v>
       </c>
       <c r="B5" t="n">
-        <v>95.6318096561446</v>
+        <v>22.7888644215797</v>
       </c>
       <c r="C5" t="n">
-        <v>194.605091588919</v>
+        <v>63.7335972601024</v>
       </c>
       <c r="D5" t="n">
-        <v>396.009882156385</v>
+        <v>178.243695893267</v>
       </c>
       <c r="E5" t="n">
-        <v>54.8839835478431</v>
+        <v>24.6990318100728</v>
       </c>
       <c r="F5" t="n">
-        <v>224.651803310895</v>
+        <v>100.514976228661</v>
       </c>
       <c r="G5" t="n">
-        <v>919.547552280768</v>
+        <v>409.054918587049</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1964</v>
+        <v>1954</v>
       </c>
       <c r="B6" t="n">
-        <v>48.5223266316684</v>
+        <v>31.9678958062832</v>
       </c>
       <c r="C6" t="n">
-        <v>119.975226578793</v>
+        <v>89.4045863312627</v>
       </c>
       <c r="D6" t="n">
-        <v>296.648079180075</v>
+        <v>250.037728648163</v>
       </c>
       <c r="E6" t="n">
-        <v>34.3683156028316</v>
+        <v>41.0659046303732</v>
       </c>
       <c r="F6" t="n">
-        <v>116.378709121198</v>
+        <v>167.121466925153</v>
       </c>
       <c r="G6" t="n">
-        <v>394.084018932853</v>
+        <v>680.116144003263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1965</v>
+        <v>1955</v>
       </c>
       <c r="B7" t="n">
-        <v>66.4211309922307</v>
+        <v>19.5343350525639</v>
       </c>
       <c r="C7" t="n">
-        <v>135.163083566642</v>
+        <v>54.6316578111313</v>
       </c>
       <c r="D7" t="n">
-        <v>275.048902154044</v>
+        <v>152.788309771558</v>
       </c>
       <c r="E7" t="n">
-        <v>23.282747825619</v>
+        <v>40.6956546876374</v>
       </c>
       <c r="F7" t="n">
-        <v>78.8405276549747</v>
+        <v>165.614700810639</v>
       </c>
       <c r="G7" t="n">
-        <v>266.97144372604</v>
+        <v>673.98422104583</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1966</v>
+        <v>1956</v>
       </c>
       <c r="B8" t="n">
-        <v>40.4174143964253</v>
+        <v>21.611775982127</v>
       </c>
       <c r="C8" t="n">
-        <v>75.6222310982888</v>
+        <v>60.441635047691</v>
       </c>
       <c r="D8" t="n">
-        <v>141.491530858263</v>
+        <v>169.037068043805</v>
       </c>
       <c r="E8" t="n">
-        <v>26.0687162261693</v>
+        <v>30.138979835772</v>
       </c>
       <c r="F8" t="n">
-        <v>88.2744321225472</v>
+        <v>122.653343865618</v>
       </c>
       <c r="G8" t="n">
-        <v>298.916728347971</v>
+        <v>499.149037007617</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1967</v>
+        <v>1957</v>
       </c>
       <c r="B9" t="n">
-        <v>43.1856351433704</v>
+        <v>27.0462991059279</v>
       </c>
       <c r="C9" t="n">
-        <v>80.8016576445626</v>
+        <v>75.6403611301129</v>
       </c>
       <c r="D9" t="n">
-        <v>151.182397953255</v>
+        <v>211.543332028</v>
       </c>
       <c r="E9" t="n">
-        <v>28.8813838175803</v>
+        <v>16.4580045293045</v>
       </c>
       <c r="F9" t="n">
-        <v>97.7987459486361</v>
+        <v>66.9773595481411</v>
       </c>
       <c r="G9" t="n">
-        <v>331.168159030657</v>
+        <v>272.570510237339</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1968</v>
+        <v>1958</v>
       </c>
       <c r="B10" t="n">
-        <v>68.7353075349682</v>
+        <v>19.1753448462044</v>
       </c>
       <c r="C10" t="n">
-        <v>128.605884088445</v>
+        <v>53.6276702139795</v>
       </c>
       <c r="D10" t="n">
-        <v>240.625582620057</v>
+        <v>149.980458533897</v>
       </c>
       <c r="E10" t="n">
-        <v>36.6677596715368</v>
+        <v>32.0043178312955</v>
       </c>
       <c r="F10" t="n">
-        <v>124.165134720429</v>
+        <v>130.244507993841</v>
       </c>
       <c r="G10" t="n">
-        <v>420.450576153134</v>
+        <v>530.041975960187</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1969</v>
+        <v>1959</v>
       </c>
       <c r="B11" t="n">
-        <v>35.9771450278742</v>
+        <v>41.4395383250332</v>
       </c>
       <c r="C11" t="n">
-        <v>67.3143499202962</v>
+        <v>115.893920705908</v>
       </c>
       <c r="D11" t="n">
-        <v>125.947228488569</v>
+        <v>324.12042699987</v>
       </c>
       <c r="E11" t="n">
-        <v>29.3888258045362</v>
+        <v>40.2340928306795</v>
       </c>
       <c r="F11" t="n">
-        <v>89.5741510337175</v>
+        <v>163.736332482806</v>
       </c>
       <c r="G11" t="n">
-        <v>273.012899078561</v>
+        <v>666.340028784669</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1970</v>
+        <v>1960</v>
       </c>
       <c r="B12" t="n">
-        <v>54.1880288468947</v>
+        <v>74.9426754326851</v>
       </c>
       <c r="C12" t="n">
-        <v>101.387476200929</v>
+        <v>184.643389458404</v>
       </c>
       <c r="D12" t="n">
-        <v>189.699100504981</v>
+        <v>454.923460816542</v>
       </c>
       <c r="E12" t="n">
-        <v>32.3361808987327</v>
+        <v>49.4460406767533</v>
       </c>
       <c r="F12" t="n">
-        <v>98.557389496984</v>
+        <v>201.225199491356</v>
       </c>
       <c r="G12" t="n">
-        <v>300.392895960108</v>
+        <v>818.904412894129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1971</v>
+        <v>1961</v>
       </c>
       <c r="B13" t="n">
-        <v>30.4267900149791</v>
+        <v>73.9223135669357</v>
       </c>
       <c r="C13" t="n">
-        <v>55.4957607589901</v>
+        <v>157.159370759594</v>
       </c>
       <c r="D13" t="n">
-        <v>101.219335352263</v>
+        <v>334.121953517955</v>
       </c>
       <c r="E13" t="n">
-        <v>27.7503135098608</v>
+        <v>28.8539374713463</v>
       </c>
       <c r="F13" t="n">
-        <v>84.8783838350535</v>
+        <v>117.423746053594</v>
       </c>
       <c r="G13" t="n">
-        <v>259.612924368969</v>
+        <v>477.866708866047</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1972</v>
+        <v>1962</v>
       </c>
       <c r="B14" t="n">
-        <v>28.1050423646579</v>
+        <v>90.0455572607039</v>
       </c>
       <c r="C14" t="n">
-        <v>50.1621954024902</v>
+        <v>182.726581842335</v>
       </c>
       <c r="D14" t="n">
-        <v>89.5300499799918</v>
+        <v>370.801233592394</v>
       </c>
       <c r="E14" t="n">
-        <v>38.1999156648299</v>
+        <v>44.3798374266602</v>
       </c>
       <c r="F14" t="n">
-        <v>108.940385006265</v>
+        <v>180.60782051195</v>
       </c>
       <c r="G14" t="n">
-        <v>310.681510122807</v>
+        <v>735.000097374887</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1973</v>
+        <v>1963</v>
       </c>
       <c r="B15" t="n">
-        <v>31.1073177013833</v>
+        <v>116.763415926878</v>
       </c>
       <c r="C15" t="n">
-        <v>55.5206901572357</v>
+        <v>236.9442816016</v>
       </c>
       <c r="D15" t="n">
-        <v>99.093951626652</v>
+        <v>480.823485147585</v>
       </c>
       <c r="E15" t="n">
-        <v>17.3976509095919</v>
+        <v>55.1676582491326</v>
       </c>
       <c r="F15" t="n">
-        <v>47.2551422983527</v>
+        <v>224.509847193321</v>
       </c>
       <c r="G15" t="n">
-        <v>128.3534475569</v>
+        <v>913.663423217007</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1974</v>
+        <v>1964</v>
       </c>
       <c r="B16" t="n">
-        <v>47.3528068562281</v>
+        <v>58.5221084863328</v>
       </c>
       <c r="C16" t="n">
-        <v>82.952392022457</v>
+        <v>144.186478622248</v>
       </c>
       <c r="D16" t="n">
-        <v>145.315553587767</v>
+        <v>355.245925945049</v>
       </c>
       <c r="E16" t="n">
-        <v>45.9690206521592</v>
+        <v>33.628283214087</v>
       </c>
       <c r="F16" t="n">
-        <v>131.096698017526</v>
+        <v>113.307158791862</v>
       </c>
       <c r="G16" t="n">
-        <v>373.867965583711</v>
+        <v>381.777212703681</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1975</v>
+        <v>1965</v>
       </c>
       <c r="B17" t="n">
-        <v>42.043294402403</v>
+        <v>81.2406814604817</v>
       </c>
       <c r="C17" t="n">
-        <v>71.4364542614649</v>
+        <v>164.859127772805</v>
       </c>
       <c r="D17" t="n">
-        <v>121.378856485583</v>
+        <v>334.543378039369</v>
       </c>
       <c r="E17" t="n">
-        <v>20.6687817599012</v>
+        <v>25.4609029341038</v>
       </c>
       <c r="F17" t="n">
-        <v>54.2019441566602</v>
+        <v>85.7879824959418</v>
       </c>
       <c r="G17" t="n">
-        <v>142.139521549419</v>
+        <v>289.054082636879</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1976</v>
+        <v>1966</v>
       </c>
       <c r="B18" t="n">
-        <v>68.3853680212471</v>
+        <v>49.3421351866702</v>
       </c>
       <c r="C18" t="n">
-        <v>116.194705582445</v>
+        <v>92.0937467647855</v>
       </c>
       <c r="D18" t="n">
-        <v>197.428338781422</v>
+        <v>171.886728474362</v>
       </c>
       <c r="E18" t="n">
-        <v>38.3968649093513</v>
+        <v>27.153867039563</v>
       </c>
       <c r="F18" t="n">
-        <v>97.7610289729989</v>
+        <v>91.492256826718</v>
       </c>
       <c r="G18" t="n">
-        <v>248.906227329303</v>
+        <v>308.274068185201</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1977</v>
+        <v>1967</v>
       </c>
       <c r="B19" t="n">
-        <v>65.7047744199338</v>
+        <v>52.8037458935871</v>
       </c>
       <c r="C19" t="n">
-        <v>114.54653526893</v>
+        <v>98.5546082300426</v>
       </c>
       <c r="D19" t="n">
-        <v>199.694905856576</v>
+        <v>183.945487938514</v>
       </c>
       <c r="E19" t="n">
-        <v>29.137930626554</v>
+        <v>31.0107917775305</v>
       </c>
       <c r="F19" t="n">
-        <v>74.1890875258781</v>
+        <v>104.487781485261</v>
       </c>
       <c r="G19" t="n">
-        <v>188.895387886828</v>
+        <v>352.061197212717</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1978</v>
+        <v>1968</v>
       </c>
       <c r="B20" t="n">
-        <v>63.1711594810196</v>
+        <v>84.5194587455376</v>
       </c>
       <c r="C20" t="n">
-        <v>110.12731373505</v>
+        <v>157.749833908911</v>
       </c>
       <c r="D20" t="n">
-        <v>191.986744111323</v>
+        <v>294.429359435562</v>
       </c>
       <c r="E20" t="n">
-        <v>21.5546674934246</v>
+        <v>37.8967798285119</v>
       </c>
       <c r="F20" t="n">
-        <v>54.8810803950355</v>
+        <v>127.689433991999</v>
       </c>
       <c r="G20" t="n">
-        <v>139.734606727066</v>
+        <v>430.236859885654</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1979</v>
+        <v>1969</v>
       </c>
       <c r="B21" t="n">
-        <v>86.7791024231333</v>
+        <v>44.0017205736623</v>
       </c>
       <c r="C21" t="n">
-        <v>147.468163972069</v>
+        <v>82.1262253122041</v>
       </c>
       <c r="D21" t="n">
-        <v>250.600188041308</v>
+        <v>153.283026120302</v>
       </c>
       <c r="E21" t="n">
-        <v>38.7333137017975</v>
+        <v>31.1192488236091</v>
       </c>
       <c r="F21" t="n">
-        <v>94.5717907249417</v>
+        <v>94.4192359971285</v>
       </c>
       <c r="G21" t="n">
-        <v>230.907783149654</v>
+        <v>286.478384385613</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1980</v>
+        <v>1970</v>
       </c>
       <c r="B22" t="n">
-        <v>68.380598478324</v>
+        <v>66.432550535766</v>
       </c>
       <c r="C22" t="n">
-        <v>114.736724518895</v>
+        <v>123.991847187684</v>
       </c>
       <c r="D22" t="n">
-        <v>192.518290952044</v>
+        <v>231.422368176832</v>
       </c>
       <c r="E22" t="n">
-        <v>32.6946909308633</v>
+        <v>35.1959256762468</v>
       </c>
       <c r="F22" t="n">
-        <v>81.3861581734682</v>
+        <v>106.788323567816</v>
       </c>
       <c r="G22" t="n">
-        <v>202.592731530737</v>
+        <v>324.007561424098</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1981</v>
+        <v>1971</v>
       </c>
       <c r="B23" t="n">
-        <v>52.0057953726676</v>
+        <v>37.4476300790452</v>
       </c>
       <c r="C23" t="n">
-        <v>89.3314090811445</v>
+        <v>68.1401164839777</v>
       </c>
       <c r="D23" t="n">
-        <v>153.446372490571</v>
+        <v>123.988499796899</v>
       </c>
       <c r="E23" t="n">
-        <v>24.1103673945081</v>
+        <v>29.336470477237</v>
       </c>
       <c r="F23" t="n">
-        <v>57.9241143470729</v>
+        <v>89.3210495896821</v>
       </c>
       <c r="G23" t="n">
-        <v>139.160178191935</v>
+        <v>271.956706789012</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1982</v>
+        <v>1972</v>
       </c>
       <c r="B24" t="n">
-        <v>54.948559535706</v>
+        <v>34.5833905978106</v>
       </c>
       <c r="C24" t="n">
-        <v>92.0559830811496</v>
+        <v>61.5845568789784</v>
       </c>
       <c r="D24" t="n">
-        <v>154.222496324589</v>
+        <v>109.667027449305</v>
       </c>
       <c r="E24" t="n">
-        <v>11.9438581285676</v>
+        <v>39.6175713359351</v>
       </c>
       <c r="F24" t="n">
-        <v>29.1342958443738</v>
+        <v>112.502219778151</v>
       </c>
       <c r="G24" t="n">
-        <v>71.0664163296867</v>
+        <v>319.473128417925</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1983</v>
+        <v>1973</v>
       </c>
       <c r="B25" t="n">
-        <v>28.8749373964071</v>
+        <v>38.2532122461216</v>
       </c>
       <c r="C25" t="n">
-        <v>48.9435421681937</v>
+        <v>68.119611312028</v>
       </c>
       <c r="D25" t="n">
-        <v>82.9601909463473</v>
+        <v>121.304360414131</v>
       </c>
       <c r="E25" t="n">
-        <v>9.57547277466898</v>
+        <v>18.9931353335507</v>
       </c>
       <c r="F25" t="n">
-        <v>23.3571642985021</v>
+        <v>51.3796110618647</v>
       </c>
       <c r="G25" t="n">
-        <v>56.9744321669882</v>
+        <v>138.990450313133</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1984</v>
+        <v>1974</v>
       </c>
       <c r="B26" t="n">
-        <v>31.7513717042807</v>
+        <v>58.2470190583936</v>
       </c>
       <c r="C26" t="n">
-        <v>53.82209307889</v>
+        <v>101.812427431538</v>
       </c>
       <c r="D26" t="n">
-        <v>91.2344112365433</v>
+        <v>177.9622467737</v>
       </c>
       <c r="E26" t="n">
-        <v>4.02920169478405</v>
+        <v>47.9748559589327</v>
       </c>
       <c r="F26" t="n">
-        <v>9.67998271769398</v>
+        <v>136.23444362985</v>
       </c>
       <c r="G26" t="n">
-        <v>23.2557396012602</v>
+        <v>386.865645767072</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1985</v>
+        <v>1975</v>
       </c>
       <c r="B27" t="n">
-        <v>31.8037610957742</v>
+        <v>51.7145432158231</v>
       </c>
       <c r="C27" t="n">
-        <v>52.2396834951238</v>
+        <v>87.6863281512495</v>
       </c>
       <c r="D27" t="n">
-        <v>85.806974950309</v>
+        <v>148.679494519755</v>
       </c>
       <c r="E27" t="n">
-        <v>3.25998294081414</v>
+        <v>22.5805092541317</v>
       </c>
       <c r="F27" t="n">
-        <v>7.83196794737511</v>
+        <v>58.9835573989802</v>
       </c>
       <c r="G27" t="n">
-        <v>18.8159640839692</v>
+        <v>154.073586396295</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1986</v>
+        <v>1976</v>
       </c>
       <c r="B28" t="n">
-        <v>20.5379954028191</v>
+        <v>83.8991934076969</v>
       </c>
       <c r="C28" t="n">
-        <v>34.0669623675595</v>
+        <v>142.258091192449</v>
       </c>
       <c r="D28" t="n">
-        <v>56.5078481219942</v>
+        <v>241.210477571321</v>
       </c>
       <c r="E28" t="n">
-        <v>3.309622439834</v>
+        <v>40.4466938938993</v>
       </c>
       <c r="F28" t="n">
-        <v>8.08001721451591</v>
+        <v>102.59005298862</v>
       </c>
       <c r="G28" t="n">
-        <v>19.7263220726011</v>
+        <v>260.212095451274</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1987</v>
+        <v>1977</v>
       </c>
       <c r="B29" t="n">
-        <v>36.2272379452304</v>
+        <v>80.6331846209219</v>
       </c>
       <c r="C29" t="n">
-        <v>58.9683853842759</v>
+        <v>140.265563967692</v>
       </c>
       <c r="D29" t="n">
-        <v>95.9849735186972</v>
+        <v>243.999149080733</v>
       </c>
       <c r="E29" t="n">
-        <v>3.80009070915391</v>
+        <v>31.4112945320344</v>
       </c>
       <c r="F29" t="n">
-        <v>9.27754006609873</v>
+        <v>79.6744866716143</v>
       </c>
       <c r="G29" t="n">
-        <v>22.6501829208259</v>
+        <v>202.093671112831</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1988</v>
+        <v>1978</v>
       </c>
       <c r="B30" t="n">
-        <v>42.4449019816901</v>
+        <v>77.6549234662785</v>
       </c>
       <c r="C30" t="n">
-        <v>69.7467425529649</v>
+        <v>135.078786667961</v>
       </c>
       <c r="D30" t="n">
-        <v>114.609950067692</v>
+        <v>234.966152733533</v>
       </c>
       <c r="E30" t="n">
-        <v>3.89249091842567</v>
+        <v>23.0757879206904</v>
       </c>
       <c r="F30" t="n">
-        <v>9.34867074954462</v>
+        <v>58.531543653797</v>
       </c>
       <c r="G30" t="n">
-        <v>22.4528834144947</v>
+        <v>148.464772439018</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1989</v>
+        <v>1979</v>
       </c>
       <c r="B31" t="n">
-        <v>27.1686358174029</v>
+        <v>106.665619138433</v>
       </c>
       <c r="C31" t="n">
-        <v>45.0778110655666</v>
+        <v>180.881472492476</v>
       </c>
       <c r="D31" t="n">
-        <v>74.7924578959283</v>
+        <v>306.735266295919</v>
       </c>
       <c r="E31" t="n">
-        <v>1.66982794410142</v>
+        <v>41.8625455731069</v>
       </c>
       <c r="F31" t="n">
-        <v>3.95641574358921</v>
+        <v>101.843002903882</v>
       </c>
       <c r="G31" t="n">
-        <v>9.37415473936388</v>
+        <v>247.763175852908</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="B32" t="n">
-        <v>21.5648558935236</v>
+        <v>84.0265714629706</v>
       </c>
       <c r="C32" t="n">
-        <v>35.4097935883272</v>
+        <v>140.700507815319</v>
       </c>
       <c r="D32" t="n">
-        <v>58.1433740229397</v>
+        <v>235.59967466021</v>
       </c>
       <c r="E32" t="n">
-        <v>5.98930679909997</v>
+        <v>34.9099762662668</v>
       </c>
       <c r="F32" t="n">
-        <v>14.5863980930769</v>
+        <v>86.5796234714396</v>
       </c>
       <c r="G32" t="n">
-        <v>35.523812098203</v>
+        <v>214.724614628272</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1991</v>
+        <v>1981</v>
       </c>
       <c r="B33" t="n">
-        <v>10.4338743491426</v>
+        <v>63.8572628798088</v>
       </c>
       <c r="C33" t="n">
-        <v>17.3069668109526</v>
+        <v>109.453951001042</v>
       </c>
       <c r="D33" t="n">
-        <v>28.7075625191928</v>
+        <v>187.608532678379</v>
       </c>
       <c r="E33" t="n">
-        <v>1.35497070199326</v>
+        <v>26.4413502555468</v>
       </c>
       <c r="F33" t="n">
-        <v>3.2943299364804</v>
+        <v>63.2991449894086</v>
       </c>
       <c r="G33" t="n">
-        <v>8.0094792562127</v>
+        <v>151.534687815334</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1992</v>
+        <v>1982</v>
       </c>
       <c r="B34" t="n">
-        <v>13.269479386536</v>
+        <v>67.3810232803671</v>
       </c>
       <c r="C34" t="n">
-        <v>22.0104662617745</v>
+        <v>112.655772065078</v>
       </c>
       <c r="D34" t="n">
-        <v>36.5093920378124</v>
+        <v>188.351591616101</v>
       </c>
       <c r="E34" t="n">
-        <v>3.2447771371577</v>
+        <v>13.0408938164469</v>
       </c>
       <c r="F34" t="n">
-        <v>7.77173752098619</v>
+        <v>31.6955903115603</v>
       </c>
       <c r="G34" t="n">
-        <v>18.6145000232628</v>
+        <v>77.0353979825587</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1993</v>
+        <v>1983</v>
       </c>
       <c r="B35" t="n">
-        <v>14.6871212852401</v>
+        <v>35.4686808931737</v>
       </c>
       <c r="C35" t="n">
-        <v>24.1164576144126</v>
+        <v>59.9956258633898</v>
       </c>
       <c r="D35" t="n">
-        <v>39.5995591356794</v>
+        <v>101.48319678369</v>
       </c>
       <c r="E35" t="n">
-        <v>2.88773684672118</v>
+        <v>10.5631898585782</v>
       </c>
       <c r="F35" t="n">
-        <v>6.91657141730734</v>
+        <v>25.6735882412043</v>
       </c>
       <c r="G35" t="n">
-        <v>16.5662464102401</v>
+        <v>62.3990614580909</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1994</v>
+        <v>1984</v>
       </c>
       <c r="B36" t="n">
-        <v>14.7479492731129</v>
+        <v>38.8740123198991</v>
       </c>
       <c r="C36" t="n">
-        <v>23.6287857263192</v>
+        <v>65.7593553590856</v>
       </c>
       <c r="D36" t="n">
-        <v>37.85743390901</v>
+        <v>111.238654288046</v>
       </c>
       <c r="E36" t="n">
-        <v>2.82243195486673</v>
+        <v>4.42734296606866</v>
       </c>
       <c r="F36" t="n">
-        <v>6.76015621315751</v>
+        <v>10.5988166874432</v>
       </c>
       <c r="G36" t="n">
-        <v>16.1916080731342</v>
+        <v>25.3729869212672</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1995</v>
+        <v>1985</v>
       </c>
       <c r="B37" t="n">
-        <v>19.2808203812939</v>
+        <v>38.9070162965941</v>
       </c>
       <c r="C37" t="n">
-        <v>31.1217346137179</v>
+        <v>63.7828203221515</v>
       </c>
       <c r="D37" t="n">
-        <v>50.2344996847945</v>
+        <v>104.563355288799</v>
       </c>
       <c r="E37" t="n">
-        <v>2.04581268013523</v>
+        <v>3.56016277015165</v>
       </c>
       <c r="F37" t="n">
-        <v>4.90003426893092</v>
+        <v>8.52283477189105</v>
       </c>
       <c r="G37" t="n">
-        <v>11.7363315174634</v>
+        <v>20.4031998643312</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1996</v>
+        <v>1986</v>
       </c>
       <c r="B38" t="n">
-        <v>15.6103758452899</v>
+        <v>25.1959561320029</v>
       </c>
       <c r="C38" t="n">
-        <v>25.0113913128226</v>
+        <v>41.7102990346609</v>
       </c>
       <c r="D38" t="n">
-        <v>40.0739675715041</v>
+        <v>69.0487408553261</v>
       </c>
       <c r="E38" t="n">
-        <v>2.04891382587148</v>
+        <v>3.65461725184123</v>
       </c>
       <c r="F38" t="n">
-        <v>4.90746198727879</v>
+        <v>8.89006290729472</v>
       </c>
       <c r="G38" t="n">
-        <v>11.7541220389505</v>
+        <v>21.6255802042854</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1997</v>
+        <v>1987</v>
       </c>
       <c r="B39" t="n">
-        <v>25.8501675375538</v>
+        <v>44.3256048531172</v>
       </c>
       <c r="C39" t="n">
-        <v>41.1358405365615</v>
+        <v>72.0124921000545</v>
       </c>
       <c r="D39" t="n">
-        <v>65.4602092690942</v>
+        <v>116.993305238467</v>
       </c>
       <c r="E39" t="n">
-        <v>1.7806567604346</v>
+        <v>4.20102969369439</v>
       </c>
       <c r="F39" t="n">
-        <v>4.26494528656273</v>
+        <v>10.2193589611993</v>
       </c>
       <c r="G39" t="n">
-        <v>10.2151962700179</v>
+        <v>24.8594523705933</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1998</v>
+        <v>1988</v>
       </c>
       <c r="B40" t="n">
-        <v>10.266540236628</v>
+        <v>51.8985840573412</v>
       </c>
       <c r="C40" t="n">
-        <v>16.3437769301607</v>
+        <v>85.1151617367637</v>
       </c>
       <c r="D40" t="n">
-        <v>26.0184091413629</v>
+        <v>139.591298858387</v>
       </c>
       <c r="E40" t="n">
-        <v>1.29479875637914</v>
+        <v>4.31207304888727</v>
       </c>
       <c r="F40" t="n">
-        <v>3.10124105654068</v>
+        <v>10.3197326546831</v>
       </c>
       <c r="G40" t="n">
-        <v>7.427946654559</v>
+        <v>24.6973742923055</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1999</v>
+        <v>1989</v>
       </c>
       <c r="B41" t="n">
-        <v>11.8389177440226</v>
+        <v>33.2184032073984</v>
       </c>
       <c r="C41" t="n">
-        <v>19.1201516308863</v>
+        <v>55.0060374988567</v>
       </c>
       <c r="D41" t="n">
-        <v>30.8795285424349</v>
+        <v>91.0839736165209</v>
       </c>
       <c r="E41" t="n">
-        <v>2.7152566990306</v>
+        <v>1.86761621163124</v>
       </c>
       <c r="F41" t="n">
-        <v>6.60479666028117</v>
+        <v>4.40963544922586</v>
       </c>
       <c r="G41" t="n">
-        <v>16.066009132483</v>
+        <v>10.4116063428715</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2000</v>
+        <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>12.080960266145</v>
+        <v>26.406482189543</v>
       </c>
       <c r="C42" t="n">
-        <v>19.3664706601411</v>
+        <v>43.2754641990905</v>
       </c>
       <c r="D42" t="n">
-        <v>31.0455607474477</v>
+        <v>70.9206848607946</v>
       </c>
       <c r="E42" t="n">
-        <v>1.97428012729895</v>
+        <v>6.58728730184773</v>
       </c>
       <c r="F42" t="n">
-        <v>4.72870286423031</v>
+        <v>15.9851108228284</v>
       </c>
       <c r="G42" t="n">
-        <v>11.3259665986568</v>
+        <v>38.7904392672277</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2001</v>
+        <v>1991</v>
       </c>
       <c r="B43" t="n">
-        <v>5.56957895433922</v>
+        <v>12.7517278885925</v>
       </c>
       <c r="C43" t="n">
-        <v>8.80843897289129</v>
+        <v>21.1096725464706</v>
       </c>
       <c r="D43" t="n">
-        <v>13.9307832378786</v>
+        <v>34.9457170755548</v>
       </c>
       <c r="E43" t="n">
-        <v>0.420545141794988</v>
+        <v>1.49214387440668</v>
       </c>
       <c r="F43" t="n">
-        <v>1.00726993553077</v>
+        <v>3.61486298426165</v>
       </c>
       <c r="G43" t="n">
-        <v>2.41256555406547</v>
+        <v>8.75735551987635</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2002</v>
+        <v>1992</v>
       </c>
       <c r="B44" t="n">
-        <v>7.73708835606294</v>
+        <v>16.2352780623079</v>
       </c>
       <c r="C44" t="n">
-        <v>12.3136897061217</v>
+        <v>26.8764677689534</v>
       </c>
       <c r="D44" t="n">
-        <v>19.597417943383</v>
+        <v>44.4922789103684</v>
       </c>
       <c r="E44" t="n">
-        <v>1.05274916457164</v>
+        <v>3.63942422990835</v>
       </c>
       <c r="F44" t="n">
-        <v>2.55864191368098</v>
+        <v>8.68635643890278</v>
       </c>
       <c r="G44" t="n">
-        <v>6.21862136087174</v>
+        <v>20.7320673318614</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2003</v>
+        <v>1993</v>
       </c>
       <c r="B45" t="n">
-        <v>8.36145906684725</v>
+        <v>18.0131137482004</v>
       </c>
       <c r="C45" t="n">
-        <v>13.1477615669177</v>
+        <v>29.5202463368287</v>
       </c>
       <c r="D45" t="n">
-        <v>20.6738600091834</v>
+        <v>48.3783623402762</v>
       </c>
       <c r="E45" t="n">
-        <v>0.773797811831294</v>
+        <v>3.23716657843068</v>
       </c>
       <c r="F45" t="n">
-        <v>1.91441845468173</v>
+        <v>7.72627233760553</v>
       </c>
       <c r="G45" t="n">
-        <v>4.73637682038968</v>
+        <v>18.4405969815083</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2004</v>
+        <v>1994</v>
       </c>
       <c r="B46" t="n">
-        <v>4.58979645069198</v>
+        <v>18.0888027148675</v>
       </c>
       <c r="C46" t="n">
-        <v>7.26017765152278</v>
+        <v>28.927814742594</v>
       </c>
       <c r="D46" t="n">
-        <v>11.4842085260064</v>
+        <v>46.2616834830114</v>
       </c>
       <c r="E46" t="n">
-        <v>0.270691826796919</v>
+        <v>3.1530035654402</v>
       </c>
       <c r="F46" t="n">
-        <v>0.64805628678546</v>
+        <v>7.52539717614469</v>
       </c>
       <c r="G46" t="n">
-        <v>1.55149475997012</v>
+        <v>17.9611603613331</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="B47" t="n">
-        <v>4.66951791775726</v>
+        <v>23.6585086834623</v>
       </c>
       <c r="C47" t="n">
-        <v>7.38639114768742</v>
+        <v>38.1161559236988</v>
       </c>
       <c r="D47" t="n">
-        <v>11.6840271624526</v>
+        <v>61.4088301945792</v>
       </c>
       <c r="E47" t="n">
-        <v>0.447670818874421</v>
+        <v>2.30998349623457</v>
       </c>
       <c r="F47" t="n">
-        <v>1.0878301270177</v>
+        <v>5.51332813893523</v>
       </c>
       <c r="G47" t="n">
-        <v>2.64340299915616</v>
+        <v>13.158876337049</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2006</v>
+        <v>1996</v>
       </c>
       <c r="B48" t="n">
-        <v>3.82001976557222</v>
+        <v>19.139363501048</v>
       </c>
       <c r="C48" t="n">
-        <v>5.977030953534</v>
+        <v>30.6089173708148</v>
       </c>
       <c r="D48" t="n">
-        <v>9.35201941662001</v>
+        <v>48.9517753587819</v>
       </c>
       <c r="E48" t="n">
-        <v>0.193652305624083</v>
+        <v>2.31977551079825</v>
       </c>
       <c r="F48" t="n">
-        <v>0.452860935666484</v>
+        <v>5.53669912384433</v>
       </c>
       <c r="G48" t="n">
-        <v>1.05902703503479</v>
+        <v>13.2146567826427</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2007</v>
+        <v>1997</v>
       </c>
       <c r="B49" t="n">
-        <v>4.08335316136952</v>
+        <v>31.6766564813845</v>
       </c>
       <c r="C49" t="n">
-        <v>6.42812476085872</v>
+        <v>50.315743479358</v>
       </c>
       <c r="D49" t="n">
-        <v>10.1193275007607</v>
+        <v>79.9223883798579</v>
       </c>
       <c r="E49" t="n">
-        <v>0.566512854970824</v>
+        <v>2.0250368843109</v>
       </c>
       <c r="F49" t="n">
-        <v>1.31234860382227</v>
+        <v>4.83323489317225</v>
       </c>
       <c r="G49" t="n">
-        <v>3.04010552071755</v>
+        <v>11.5356711344678</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2008</v>
+        <v>1998</v>
       </c>
       <c r="B50" t="n">
-        <v>3.64090570299035</v>
+        <v>12.5556153587172</v>
       </c>
       <c r="C50" t="n">
-        <v>5.72832290424384</v>
+        <v>19.9513940514608</v>
       </c>
       <c r="D50" t="n">
-        <v>9.01250567086481</v>
+        <v>31.7035934300342</v>
       </c>
       <c r="E50" t="n">
-        <v>0.514946587265635</v>
+        <v>1.45751172061884</v>
       </c>
       <c r="F50" t="n">
-        <v>1.17025035149354</v>
+        <v>3.47870034362346</v>
       </c>
       <c r="G50" t="n">
-        <v>2.65947171811105</v>
+        <v>8.30275044072228</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2009</v>
+        <v>1999</v>
       </c>
       <c r="B51" t="n">
-        <v>2.58543689796428</v>
+        <v>14.5129771362683</v>
       </c>
       <c r="C51" t="n">
-        <v>4.30725534599828</v>
+        <v>23.3947466530869</v>
       </c>
       <c r="D51" t="n">
-        <v>7.1757499207343</v>
+        <v>37.712053552015</v>
       </c>
       <c r="E51" t="n">
-        <v>0.366032614803044</v>
+        <v>3.06139707139913</v>
       </c>
       <c r="F51" t="n">
-        <v>0.825590570449573</v>
+        <v>7.42016984541525</v>
       </c>
       <c r="G51" t="n">
-        <v>1.86212857119853</v>
+        <v>17.9849001128255</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2010</v>
+        <v>2000</v>
       </c>
       <c r="B52" t="n">
-        <v>2.94590518658554</v>
+        <v>14.8178113813803</v>
       </c>
       <c r="C52" t="n">
-        <v>4.78564238776219</v>
+        <v>23.7098172160067</v>
       </c>
       <c r="D52" t="n">
-        <v>7.77430759409174</v>
+        <v>37.9378180722989</v>
       </c>
       <c r="E52" t="n">
-        <v>0.305788603692498</v>
+        <v>2.2181868958931</v>
       </c>
       <c r="F52" t="n">
-        <v>0.704111869046719</v>
+        <v>5.29423359538273</v>
       </c>
       <c r="G52" t="n">
-        <v>1.62129496699954</v>
+        <v>12.6359548036163</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2011</v>
+        <v>2001</v>
       </c>
       <c r="B53" t="n">
-        <v>2.2714902895351</v>
+        <v>6.81452766903141</v>
       </c>
       <c r="C53" t="n">
-        <v>3.69005094342121</v>
+        <v>10.7579719362403</v>
       </c>
       <c r="D53" t="n">
-        <v>5.99451207331843</v>
+        <v>16.9834162838442</v>
       </c>
       <c r="E53" t="n">
-        <v>0.209231740812217</v>
+        <v>0.472761952749897</v>
       </c>
       <c r="F53" t="n">
-        <v>0.466165767554834</v>
+        <v>1.12835948021392</v>
       </c>
       <c r="G53" t="n">
-        <v>1.03861164657145</v>
+        <v>2.69309979194153</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2012</v>
+        <v>2002</v>
       </c>
       <c r="B54" t="n">
-        <v>3.0141610460709</v>
+        <v>9.47323378599359</v>
       </c>
       <c r="C54" t="n">
-        <v>4.94837343175202</v>
+        <v>15.0493005019445</v>
       </c>
       <c r="D54" t="n">
-        <v>8.12378610359538</v>
+        <v>23.9075114912381</v>
       </c>
       <c r="E54" t="n">
-        <v>0.234937016122346</v>
+        <v>1.18628260427267</v>
       </c>
       <c r="F54" t="n">
-        <v>0.516643710741354</v>
+        <v>2.87306492501538</v>
       </c>
       <c r="G54" t="n">
-        <v>1.13613737100327</v>
+        <v>6.95829310286023</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2013</v>
+        <v>2003</v>
       </c>
       <c r="B55" t="n">
-        <v>4.35583782962734</v>
+        <v>10.2459764833412</v>
       </c>
       <c r="C55" t="n">
-        <v>7.08919085325704</v>
+        <v>16.0824001900727</v>
       </c>
       <c r="D55" t="n">
-        <v>11.5377635531034</v>
+        <v>25.2434305597103</v>
       </c>
       <c r="E55" t="n">
-        <v>0.78736554579365</v>
+        <v>0.872643747910618</v>
       </c>
       <c r="F55" t="n">
-        <v>1.73622426230133</v>
+        <v>2.15124266649782</v>
       </c>
       <c r="G55" t="n">
-        <v>3.8285580377603</v>
+        <v>5.30324662411342</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2014</v>
+        <v>2004</v>
       </c>
       <c r="B56" t="n">
-        <v>7.40013130542942</v>
+        <v>5.62185825449413</v>
       </c>
       <c r="C56" t="n">
-        <v>12.0438237637143</v>
+        <v>8.87669628518746</v>
       </c>
       <c r="D56" t="n">
-        <v>19.6015023064502</v>
+        <v>14.0159593807744</v>
       </c>
       <c r="E56" t="n">
-        <v>1.15132197727119</v>
+        <v>0.309665242981578</v>
       </c>
       <c r="F56" t="n">
-        <v>2.52953991024376</v>
+        <v>0.73880232087638</v>
       </c>
       <c r="G56" t="n">
-        <v>5.55758709017404</v>
+        <v>1.76264169681063</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2015</v>
+        <v>2005</v>
       </c>
       <c r="B57" t="n">
-        <v>4.73219538912035</v>
+        <v>5.71751330290813</v>
       </c>
       <c r="C57" t="n">
-        <v>7.63988497794517</v>
+        <v>9.02786508508399</v>
       </c>
       <c r="D57" t="n">
-        <v>12.3341996001315</v>
+        <v>14.2548593552067</v>
       </c>
       <c r="E57" t="n">
-        <v>0.395451984170109</v>
+        <v>0.507415126378699</v>
       </c>
       <c r="F57" t="n">
-        <v>0.869113713297548</v>
+        <v>1.22868102721014</v>
       </c>
       <c r="G57" t="n">
-        <v>1.91011469629376</v>
+        <v>2.97519129435545</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="B58" t="n">
-        <v>6.99253347779649</v>
+        <v>4.67674445519123</v>
       </c>
       <c r="C58" t="n">
-        <v>11.4760302018363</v>
+        <v>7.30465126646779</v>
       </c>
       <c r="D58" t="n">
-        <v>18.8342708135251</v>
+        <v>11.4092036962767</v>
       </c>
       <c r="E58" t="n">
-        <v>0.775551556181402</v>
+        <v>0.219482760467522</v>
       </c>
       <c r="F58" t="n">
-        <v>1.71936139859508</v>
+        <v>0.511541111681994</v>
       </c>
       <c r="G58" t="n">
-        <v>3.81174352035905</v>
+        <v>1.1922317196278</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="B59" t="n">
-        <v>6.50977155876342</v>
+        <v>4.99882289472989</v>
       </c>
       <c r="C59" t="n">
-        <v>10.5947500334572</v>
+        <v>7.85525916976466</v>
       </c>
       <c r="D59" t="n">
-        <v>17.2431132579965</v>
+        <v>12.3439253447498</v>
       </c>
       <c r="E59" t="n">
-        <v>0.525214255861756</v>
+        <v>0.640102213702273</v>
       </c>
       <c r="F59" t="n">
-        <v>1.14976886900202</v>
+        <v>1.47789201039627</v>
       </c>
       <c r="G59" t="n">
-        <v>2.51700793984948</v>
+        <v>3.41221253049599</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2018</v>
+        <v>2008</v>
       </c>
       <c r="B60" t="n">
-        <v>6.15863638603538</v>
+        <v>4.46286214832733</v>
       </c>
       <c r="C60" t="n">
-        <v>10.4232105824238</v>
+        <v>7.0090318717342</v>
       </c>
       <c r="D60" t="n">
-        <v>17.6408074832766</v>
+        <v>11.0078523929757</v>
       </c>
       <c r="E60" t="n">
-        <v>0.802955009598603</v>
+        <v>0.581931524652832</v>
       </c>
       <c r="F60" t="n">
-        <v>1.75778296750706</v>
+        <v>1.31818081050975</v>
       </c>
       <c r="G60" t="n">
-        <v>3.84803746651074</v>
+        <v>2.98591943482138</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="B61" t="n">
-        <v>3.74343047679283</v>
+        <v>3.16223398820948</v>
       </c>
       <c r="C61" t="n">
-        <v>6.20021668817847</v>
+        <v>5.25742538845667</v>
       </c>
       <c r="D61" t="n">
-        <v>10.2693738320212</v>
+        <v>8.74082114677398</v>
       </c>
       <c r="E61" t="n">
-        <v>0.625926784058276</v>
+        <v>0.412719066028284</v>
       </c>
       <c r="F61" t="n">
-        <v>1.37520764166998</v>
+        <v>0.927894726590771</v>
       </c>
       <c r="G61" t="n">
-        <v>3.02143334631841</v>
+        <v>2.08613726504207</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2020</v>
+        <v>2010</v>
       </c>
       <c r="B62" t="n">
-        <v>4.28600672629676</v>
+        <v>3.60212964107282</v>
       </c>
       <c r="C62" t="n">
-        <v>7.09888178631213</v>
+        <v>5.84033224418566</v>
       </c>
       <c r="D62" t="n">
-        <v>11.7578263017744</v>
+        <v>9.46925405836195</v>
       </c>
       <c r="E62" t="n">
-        <v>0.385351439940468</v>
+        <v>0.349711182240499</v>
       </c>
       <c r="F62" t="n">
-        <v>0.853582705751228</v>
+        <v>0.802591409185687</v>
       </c>
       <c r="G62" t="n">
-        <v>1.8907505202787</v>
+        <v>1.84195702857359</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2.77566757294989</v>
+      </c>
+      <c r="C63" t="n">
+        <v>4.50034353028221</v>
+      </c>
+      <c r="D63" t="n">
+        <v>7.29665615865828</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.238056074270219</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.528703518857071</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.17420826882391</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3.68536734791047</v>
+      </c>
+      <c r="C64" t="n">
+        <v>6.03826919465875</v>
+      </c>
+      <c r="D64" t="n">
+        <v>9.89336785865792</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.265743152344414</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.582564089899812</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1.27710127559917</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B65" t="n">
+        <v>5.32844618625654</v>
+      </c>
+      <c r="C65" t="n">
+        <v>8.65520113104003</v>
+      </c>
+      <c r="D65" t="n">
+        <v>14.0589777958114</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.896170315968027</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1.96996028287764</v>
+      </c>
+      <c r="G65" t="n">
+        <v>4.33036382367053</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B66" t="n">
+        <v>9.05433357891421</v>
+      </c>
+      <c r="C66" t="n">
+        <v>14.7073040608276</v>
+      </c>
+      <c r="D66" t="n">
+        <v>23.8896425509843</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1.30218305688674</v>
+      </c>
+      <c r="F66" t="n">
+        <v>2.85207167974925</v>
+      </c>
+      <c r="G66" t="n">
+        <v>6.24667386310125</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B67" t="n">
+        <v>5.78986817393362</v>
+      </c>
+      <c r="C67" t="n">
+        <v>9.32952278254661</v>
+      </c>
+      <c r="D67" t="n">
+        <v>15.0331566687332</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.446093803917266</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.977354490697671</v>
+      </c>
+      <c r="G67" t="n">
+        <v>2.14130255138909</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B68" t="n">
+        <v>8.55980782999704</v>
+      </c>
+      <c r="C68" t="n">
+        <v>14.0203121542916</v>
+      </c>
+      <c r="D68" t="n">
+        <v>22.9642016278588</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.876411482381655</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1.93683751063396</v>
+      </c>
+      <c r="G68" t="n">
+        <v>4.28034047706046</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B69" t="n">
+        <v>7.95672145026708</v>
+      </c>
+      <c r="C69" t="n">
+        <v>12.9244102480284</v>
+      </c>
+      <c r="D69" t="n">
+        <v>20.9936192065308</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.593755667219603</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1.29578033754856</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2.82784110683101</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B70" t="n">
+        <v>7.53998654818503</v>
+      </c>
+      <c r="C70" t="n">
+        <v>12.7343155708572</v>
+      </c>
+      <c r="D70" t="n">
+        <v>21.5070401017107</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.90693250650158</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1.9792405770398</v>
+      </c>
+      <c r="G70" t="n">
+        <v>4.31938786372525</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4.57650072434409</v>
+      </c>
+      <c r="C71" t="n">
+        <v>7.56467941342443</v>
+      </c>
+      <c r="D71" t="n">
+        <v>12.5039583897562</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.706597626981423</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1.54760659051258</v>
+      </c>
+      <c r="G71" t="n">
+        <v>3.38960402291437</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5.24554358911691</v>
+      </c>
+      <c r="C72" t="n">
+        <v>8.67056687869317</v>
+      </c>
+      <c r="D72" t="n">
+        <v>14.3319236072819</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.436316267014617</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.963429746437362</v>
+      </c>
+      <c r="G72" t="n">
+        <v>2.12734877539934</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
         <v>2021</v>
       </c>
-      <c r="B63" t="n">
-        <v>3.19600351350295</v>
-      </c>
-      <c r="C63" t="n">
-        <v>5.40042664380569</v>
-      </c>
-      <c r="D63" t="n">
-        <v>9.12533663117311</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.353458128608874</v>
-      </c>
-      <c r="F63" t="n">
-        <v>0.597253628522114</v>
-      </c>
-      <c r="G63" t="n">
-        <v>1.00920552651247</v>
+      <c r="B73" t="n">
+        <v>3.90974589263941</v>
+      </c>
+      <c r="C73" t="n">
+        <v>6.5925564062528</v>
+      </c>
+      <c r="D73" t="n">
+        <v>11.1162723008283</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.400023427008181</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.674513658634132</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.13735507714327</v>
       </c>
     </row>
   </sheetData>
@@ -1853,982 +2083,1416 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1950</v>
+        <v>1920</v>
       </c>
       <c r="B2" t="n">
-        <v>45.949685720769</v>
+        <v>5.34710350504984</v>
       </c>
       <c r="C2" t="n">
-        <v>183.402943905541</v>
+        <v>55.0247867283179</v>
       </c>
       <c r="D2" t="n">
-        <v>732.031989024369</v>
+        <v>566.236870417314</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1951</v>
+        <v>1921</v>
       </c>
       <c r="B3" t="n">
-        <v>71.4897429701158</v>
+        <v>10.39343243794</v>
       </c>
       <c r="C3" t="n">
-        <v>261.050566175582</v>
+        <v>106.954429203162</v>
       </c>
       <c r="D3" t="n">
-        <v>953.247210989122</v>
+        <v>1100.62291687361</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1952</v>
+        <v>1922</v>
       </c>
       <c r="B4" t="n">
-        <v>68.9164255762009</v>
+        <v>3.04116511849652</v>
       </c>
       <c r="C4" t="n">
-        <v>251.653890027067</v>
+        <v>31.2953474517256</v>
       </c>
       <c r="D4" t="n">
-        <v>918.934489655613</v>
+        <v>322.047220049802</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1953</v>
+        <v>1923</v>
       </c>
       <c r="B5" t="n">
-        <v>109.604416579066</v>
+        <v>11.576479088432</v>
       </c>
       <c r="C5" t="n">
-        <v>400.229372978305</v>
+        <v>119.128663266798</v>
       </c>
       <c r="D5" t="n">
-        <v>1461.4698567284</v>
+        <v>1225.90282445336</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1954</v>
+        <v>1924</v>
       </c>
       <c r="B6" t="n">
-        <v>53.8101527852875</v>
+        <v>30.4183350643504</v>
       </c>
       <c r="C6" t="n">
-        <v>196.492115749611</v>
+        <v>313.02225550071</v>
       </c>
       <c r="D6" t="n">
-        <v>717.506818942075</v>
+        <v>3221.17999658651</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1955</v>
+        <v>1925</v>
       </c>
       <c r="B7" t="n">
-        <v>83.040481904345</v>
+        <v>42.2756141947147</v>
       </c>
       <c r="C7" t="n">
-        <v>303.229021619007</v>
+        <v>241.775373318648</v>
       </c>
       <c r="D7" t="n">
-        <v>1107.26524513593</v>
+        <v>1382.71985533163</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1956</v>
+        <v>1926</v>
       </c>
       <c r="B8" t="n">
-        <v>37.2876468871551</v>
+        <v>33.58721005114</v>
       </c>
       <c r="C8" t="n">
-        <v>136.15885198127</v>
+        <v>192.086156606602</v>
       </c>
       <c r="D8" t="n">
-        <v>497.195036977348</v>
+        <v>1098.54589004911</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1957</v>
+        <v>1927</v>
       </c>
       <c r="B9" t="n">
-        <v>42.9772706156106</v>
+        <v>45.3678019150813</v>
       </c>
       <c r="C9" t="n">
-        <v>156.934972217991</v>
+        <v>259.459677963398</v>
       </c>
       <c r="D9" t="n">
-        <v>573.060716799353</v>
+        <v>1483.85686868579</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1958</v>
+        <v>1928</v>
       </c>
       <c r="B10" t="n">
-        <v>42.2815601153787</v>
+        <v>6.30842765393031</v>
       </c>
       <c r="C10" t="n">
-        <v>154.394529177708</v>
+        <v>36.0780672294389</v>
       </c>
       <c r="D10" t="n">
-        <v>563.784084006303</v>
+        <v>206.331435726455</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1959</v>
+        <v>1929</v>
       </c>
       <c r="B11" t="n">
-        <v>91.7210643040833</v>
+        <v>4.67455023873657</v>
       </c>
       <c r="C11" t="n">
-        <v>334.926868835112</v>
+        <v>26.7338783976467</v>
       </c>
       <c r="D11" t="n">
-        <v>1223.01249248259</v>
+        <v>152.891768764759</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1960</v>
+        <v>1930</v>
       </c>
       <c r="B12" t="n">
-        <v>48.7000362880608</v>
+        <v>42.2196215393509</v>
       </c>
       <c r="C12" t="n">
-        <v>167.044904775601</v>
+        <v>241.455149818382</v>
       </c>
       <c r="D12" t="n">
-        <v>572.976990128663</v>
+        <v>1380.88848853081</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1961</v>
+        <v>1931</v>
       </c>
       <c r="B13" t="n">
-        <v>52.8150709375938</v>
+        <v>21.6334887698141</v>
       </c>
       <c r="C13" t="n">
-        <v>181.159793050294</v>
+        <v>123.72250346065</v>
       </c>
       <c r="D13" t="n">
-        <v>621.392152569556</v>
+        <v>707.572321110281</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1962</v>
+        <v>1932</v>
       </c>
       <c r="B14" t="n">
-        <v>51.8705631182221</v>
+        <v>55.1315717221996</v>
       </c>
       <c r="C14" t="n">
-        <v>177.920057913066</v>
+        <v>315.298939795068</v>
       </c>
       <c r="D14" t="n">
-        <v>610.279609566611</v>
+        <v>1803.2031072291</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1963</v>
+        <v>1933</v>
       </c>
       <c r="B15" t="n">
-        <v>43.7940874149666</v>
+        <v>46.7172501167505</v>
       </c>
       <c r="C15" t="n">
-        <v>150.217119319907</v>
+        <v>267.177208481813</v>
       </c>
       <c r="D15" t="n">
-        <v>515.256379770104</v>
+        <v>1527.99363305289</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1964</v>
+        <v>1934</v>
       </c>
       <c r="B16" t="n">
-        <v>17.6846232478129</v>
+        <v>44.827832548226</v>
       </c>
       <c r="C16" t="n">
-        <v>60.6596304969799</v>
+        <v>256.371578648017</v>
       </c>
       <c r="D16" t="n">
-        <v>208.067241267648</v>
+        <v>1466.19594573901</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1965</v>
+        <v>1935</v>
       </c>
       <c r="B17" t="n">
-        <v>33.2465521453063</v>
+        <v>9.55607631786142</v>
       </c>
       <c r="C17" t="n">
-        <v>114.038254599643</v>
+        <v>54.6514571869012</v>
       </c>
       <c r="D17" t="n">
-        <v>391.160065419568</v>
+        <v>312.553151869355</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1966</v>
+        <v>1936</v>
       </c>
       <c r="B18" t="n">
-        <v>45.450122924304</v>
+        <v>15.9542222326378</v>
       </c>
       <c r="C18" t="n">
-        <v>155.897449665578</v>
+        <v>91.2426255604103</v>
       </c>
       <c r="D18" t="n">
-        <v>534.74035378758</v>
+        <v>521.819026823269</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1967</v>
+        <v>1937</v>
       </c>
       <c r="B19" t="n">
-        <v>33.8182388055713</v>
+        <v>52.4021770951887</v>
       </c>
       <c r="C19" t="n">
-        <v>110.643790886553</v>
+        <v>299.689458597701</v>
       </c>
       <c r="D19" t="n">
-        <v>361.995446662071</v>
+        <v>1713.93206491089</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1968</v>
+        <v>1938</v>
       </c>
       <c r="B20" t="n">
-        <v>53.0836774416527</v>
+        <v>26.3568328393708</v>
       </c>
       <c r="C20" t="n">
-        <v>173.674901880932</v>
+        <v>150.735435087606</v>
       </c>
       <c r="D20" t="n">
-        <v>568.215560734373</v>
+        <v>862.060002790238</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1969</v>
+        <v>1939</v>
       </c>
       <c r="B21" t="n">
-        <v>35.4038736113248</v>
+        <v>29.7405792284619</v>
       </c>
       <c r="C21" t="n">
-        <v>115.831543178412</v>
+        <v>170.087171591545</v>
       </c>
       <c r="D21" t="n">
-        <v>378.968316924527</v>
+        <v>972.733103742845</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1970</v>
+        <v>1940</v>
       </c>
       <c r="B22" t="n">
-        <v>18.1180828032665</v>
+        <v>30.8413252061192</v>
       </c>
       <c r="C22" t="n">
-        <v>59.2772845586393</v>
+        <v>176.382367409431</v>
       </c>
       <c r="D22" t="n">
-        <v>193.938646974966</v>
+        <v>1008.73549774647</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1971</v>
+        <v>1941</v>
       </c>
       <c r="B23" t="n">
-        <v>18.9315428256403</v>
+        <v>26.2440753558531</v>
       </c>
       <c r="C23" t="n">
-        <v>61.9386975650219</v>
+        <v>150.090572010124</v>
       </c>
       <c r="D23" t="n">
-        <v>202.64604376857</v>
+        <v>858.372013525794</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1972</v>
+        <v>1942</v>
       </c>
       <c r="B24" t="n">
-        <v>31.7162634683966</v>
+        <v>13.4796748081919</v>
       </c>
       <c r="C24" t="n">
-        <v>108.789245650214</v>
+        <v>60.2414004135257</v>
       </c>
       <c r="D24" t="n">
-        <v>373.155557272236</v>
+        <v>269.222097374136</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1973</v>
+        <v>1943</v>
       </c>
       <c r="B25" t="n">
-        <v>41.3166102790225</v>
+        <v>45.3113720882695</v>
       </c>
       <c r="C25" t="n">
-        <v>135.176358950433</v>
+        <v>202.498988150425</v>
       </c>
       <c r="D25" t="n">
-        <v>442.259127641305</v>
+        <v>904.979000019332</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1974</v>
+        <v>1944</v>
       </c>
       <c r="B26" t="n">
-        <v>19.8824210473321</v>
+        <v>53.627609084235</v>
       </c>
       <c r="C26" t="n">
-        <v>65.0497043718613</v>
+        <v>239.664703936338</v>
       </c>
       <c r="D26" t="n">
-        <v>212.824385359968</v>
+        <v>1071.07460678828</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1975</v>
+        <v>1945</v>
       </c>
       <c r="B27" t="n">
-        <v>37.4252179091348</v>
+        <v>49.2205504337717</v>
       </c>
       <c r="C27" t="n">
-        <v>122.444814705722</v>
+        <v>219.969318952185</v>
       </c>
       <c r="D27" t="n">
-        <v>400.60508624745</v>
+        <v>983.054859278629</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1976</v>
+        <v>1946</v>
       </c>
       <c r="B28" t="n">
-        <v>11.4630501976646</v>
+        <v>34.0351281420357</v>
       </c>
       <c r="C28" t="n">
-        <v>37.5038847021069</v>
+        <v>132.299661224792</v>
       </c>
       <c r="D28" t="n">
-        <v>122.702190385198</v>
+        <v>514.268678147772</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1977</v>
+        <v>1947</v>
       </c>
       <c r="B29" t="n">
-        <v>23.8504836048459</v>
+        <v>17.2895978499411</v>
       </c>
       <c r="C29" t="n">
-        <v>78.0320919634353</v>
+        <v>67.2072668189825</v>
       </c>
       <c r="D29" t="n">
-        <v>255.299115819725</v>
+        <v>261.244752624093</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1978</v>
+        <v>1948</v>
       </c>
       <c r="B30" t="n">
-        <v>21.3254116807165</v>
+        <v>20.3966848553259</v>
       </c>
       <c r="C30" t="n">
-        <v>69.7707649453983</v>
+        <v>79.2849812466428</v>
       </c>
       <c r="D30" t="n">
-        <v>228.270371233577</v>
+        <v>308.192644827725</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1979</v>
+        <v>1949</v>
       </c>
       <c r="B31" t="n">
-        <v>17.9290992321082</v>
+        <v>24.12816103155</v>
       </c>
       <c r="C31" t="n">
-        <v>58.6589833263245</v>
+        <v>93.7897902757935</v>
       </c>
       <c r="D31" t="n">
-        <v>191.915738784911</v>
+        <v>364.575018729151</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1980</v>
+        <v>1950</v>
       </c>
       <c r="B32" t="n">
-        <v>31.4842632112583</v>
+        <v>34.5778538683551</v>
       </c>
       <c r="C32" t="n">
-        <v>99.3366603538739</v>
+        <v>134.40931773704</v>
       </c>
       <c r="D32" t="n">
-        <v>313.41918418254</v>
+        <v>522.469230256945</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1981</v>
+        <v>1951</v>
       </c>
       <c r="B33" t="n">
-        <v>13.103632391329</v>
+        <v>58.0433829638391</v>
       </c>
       <c r="C33" t="n">
-        <v>41.3435458700528</v>
+        <v>205.863780604785</v>
       </c>
       <c r="D33" t="n">
-        <v>130.443890217818</v>
+        <v>730.141731940359</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1982</v>
+        <v>1952</v>
       </c>
       <c r="B34" t="n">
-        <v>16.5278969723812</v>
+        <v>53.6401497855716</v>
       </c>
       <c r="C34" t="n">
-        <v>52.1475149947977</v>
+        <v>190.246733791245</v>
       </c>
       <c r="D34" t="n">
-        <v>164.531720198693</v>
+        <v>674.752398397895</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1983</v>
+        <v>1953</v>
       </c>
       <c r="B35" t="n">
-        <v>14.8728199202888</v>
+        <v>86.0637803975618</v>
       </c>
       <c r="C35" t="n">
-        <v>46.925546613959</v>
+        <v>305.244358634644</v>
       </c>
       <c r="D35" t="n">
-        <v>148.055778044819</v>
+        <v>1082.61707826298</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1984</v>
+        <v>1954</v>
       </c>
       <c r="B36" t="n">
-        <v>11.1350730593408</v>
+        <v>42.8736144599239</v>
       </c>
       <c r="C36" t="n">
-        <v>35.1325029615363</v>
+        <v>152.06081917056</v>
       </c>
       <c r="D36" t="n">
-        <v>110.847298240845</v>
+        <v>539.317550388373</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1985</v>
+        <v>1955</v>
       </c>
       <c r="B37" t="n">
-        <v>20.9836890686514</v>
+        <v>65.8568691079792</v>
       </c>
       <c r="C37" t="n">
-        <v>66.1679494204035</v>
+        <v>233.576048829018</v>
       </c>
       <c r="D37" t="n">
-        <v>208.647655623238</v>
+        <v>828.429461126109</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1986</v>
+        <v>1956</v>
       </c>
       <c r="B38" t="n">
-        <v>16.1748715521491</v>
+        <v>28.7908779446503</v>
       </c>
       <c r="C38" t="n">
-        <v>49.5360172643258</v>
+        <v>102.113258703566</v>
       </c>
       <c r="D38" t="n">
-        <v>151.705501864437</v>
+        <v>362.167406742763</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1987</v>
+        <v>1957</v>
       </c>
       <c r="B39" t="n">
-        <v>15.5494706411879</v>
+        <v>33.63762831728</v>
       </c>
       <c r="C39" t="n">
-        <v>47.6207086807231</v>
+        <v>119.303337992686</v>
       </c>
       <c r="D39" t="n">
-        <v>145.839813301905</v>
+        <v>423.135850183743</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1988</v>
+        <v>1958</v>
       </c>
       <c r="B40" t="n">
-        <v>20.1619958471869</v>
+        <v>32.6739085662951</v>
       </c>
       <c r="C40" t="n">
-        <v>61.7467020464102</v>
+        <v>115.88529133085</v>
       </c>
       <c r="D40" t="n">
-        <v>189.101081187859</v>
+        <v>411.012986695114</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1989</v>
+        <v>1959</v>
       </c>
       <c r="B41" t="n">
-        <v>11.2024261390007</v>
+        <v>73.319948094675</v>
       </c>
       <c r="C41" t="n">
-        <v>36.6435889188277</v>
+        <v>260.04552005385</v>
       </c>
       <c r="D41" t="n">
-        <v>119.862661194194</v>
+        <v>922.309334054053</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="B42" t="n">
-        <v>10.2423028507553</v>
+        <v>38.5204808975231</v>
       </c>
       <c r="C42" t="n">
-        <v>32.3000869094026</v>
+        <v>128.083473291341</v>
       </c>
       <c r="D42" t="n">
-        <v>101.861429949615</v>
+        <v>425.887105979215</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1991</v>
+        <v>1961</v>
       </c>
       <c r="B43" t="n">
-        <v>11.6032021899982</v>
+        <v>42.5791763519538</v>
       </c>
       <c r="C43" t="n">
-        <v>37.9545435887394</v>
+        <v>141.578938527567</v>
       </c>
       <c r="D43" t="n">
-        <v>124.150846933552</v>
+        <v>470.760534889324</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1992</v>
+        <v>1962</v>
       </c>
       <c r="B44" t="n">
-        <v>5.84793576217515</v>
+        <v>41.576539578142</v>
       </c>
       <c r="C44" t="n">
-        <v>17.8973141008762</v>
+        <v>138.245096440262</v>
       </c>
       <c r="D44" t="n">
-        <v>54.7738321780541</v>
+        <v>459.675261185637</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1993</v>
+        <v>1963</v>
       </c>
       <c r="B45" t="n">
-        <v>4.68768478315816</v>
+        <v>34.4336016336896</v>
       </c>
       <c r="C45" t="n">
-        <v>14.3464241711973</v>
+        <v>114.494294785841</v>
       </c>
       <c r="D45" t="n">
-        <v>43.9065116407528</v>
+        <v>380.7020734561</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1994</v>
+        <v>1964</v>
       </c>
       <c r="B46" t="n">
-        <v>18.0998588517666</v>
+        <v>13.9119720457474</v>
       </c>
       <c r="C46" t="n">
-        <v>55.3937102296588</v>
+        <v>46.2583451305237</v>
       </c>
       <c r="D46" t="n">
-        <v>169.529671923818</v>
+        <v>153.812449247176</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1995</v>
+        <v>1965</v>
       </c>
       <c r="B47" t="n">
-        <v>4.27657956400301</v>
+        <v>26.6064845863872</v>
       </c>
       <c r="C47" t="n">
-        <v>13.4746206729058</v>
+        <v>88.4685465626194</v>
       </c>
       <c r="D47" t="n">
-        <v>42.4557522107108</v>
+        <v>294.164518634181</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1996</v>
+        <v>1966</v>
       </c>
       <c r="B48" t="n">
-        <v>3.3123886256195</v>
+        <v>36.6253273028604</v>
       </c>
       <c r="C48" t="n">
-        <v>10.1373992580984</v>
+        <v>121.781946177214</v>
       </c>
       <c r="D48" t="n">
-        <v>31.0250019950103</v>
+        <v>404.934058119712</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1997</v>
+        <v>1967</v>
       </c>
       <c r="B49" t="n">
-        <v>7.42022989125379</v>
+        <v>26.7296970888476</v>
       </c>
       <c r="C49" t="n">
-        <v>21.7167658911868</v>
+        <v>84.642854648737</v>
       </c>
       <c r="D49" t="n">
-        <v>63.5583974734408</v>
+        <v>268.031950353691</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1998</v>
+        <v>1968</v>
       </c>
       <c r="B50" t="n">
-        <v>5.93650949016516</v>
+        <v>42.7786021650593</v>
       </c>
       <c r="C50" t="n">
-        <v>17.722507370216</v>
+        <v>135.463675218525</v>
       </c>
       <c r="D50" t="n">
-        <v>52.9077344199818</v>
+        <v>428.962293646387</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1999</v>
+        <v>1969</v>
       </c>
       <c r="B51" t="n">
-        <v>7.2603036306169</v>
+        <v>27.5560062809416</v>
       </c>
       <c r="C51" t="n">
-        <v>21.6744847821399</v>
+        <v>87.2594637561591</v>
       </c>
       <c r="D51" t="n">
-        <v>64.7057360783267</v>
+        <v>276.317763081605</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2000</v>
+        <v>1970</v>
       </c>
       <c r="B52" t="n">
-        <v>5.82767150719242</v>
+        <v>13.8782784227835</v>
       </c>
       <c r="C52" t="n">
-        <v>17.8201070736219</v>
+        <v>43.9472658223458</v>
       </c>
       <c r="D52" t="n">
-        <v>54.4910974689334</v>
+        <v>139.16439160705</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2001</v>
+        <v>1971</v>
       </c>
       <c r="B53" t="n">
-        <v>6.05486023884928</v>
+        <v>14.7308126990506</v>
       </c>
       <c r="C53" t="n">
-        <v>18.0758247563499</v>
+        <v>46.6469198659092</v>
       </c>
       <c r="D53" t="n">
-        <v>53.9625074292994</v>
+        <v>147.713176280952</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2002</v>
+        <v>1972</v>
       </c>
       <c r="B54" t="n">
-        <v>12.9128046477819</v>
+        <v>25.3707661750682</v>
       </c>
       <c r="C54" t="n">
-        <v>37.7918689372473</v>
+        <v>84.3596906386017</v>
       </c>
       <c r="D54" t="n">
-        <v>110.60535621248</v>
+        <v>280.502266093722</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2003</v>
+        <v>1973</v>
       </c>
       <c r="B55" t="n">
-        <v>8.27129124662997</v>
+        <v>32.849028074803</v>
       </c>
       <c r="C55" t="n">
-        <v>23.7813696999855</v>
+        <v>104.020464558421</v>
       </c>
       <c r="D55" t="n">
-        <v>68.3754843039548</v>
+        <v>329.393521851242</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2004</v>
+        <v>1974</v>
       </c>
       <c r="B56" t="n">
-        <v>9.09858248159211</v>
+        <v>15.7483588694231</v>
       </c>
       <c r="C56" t="n">
-        <v>26.1599727646771</v>
+        <v>49.8691042517229</v>
       </c>
       <c r="D56" t="n">
-        <v>75.214372835899</v>
+        <v>157.916617184651</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2005</v>
+        <v>1975</v>
       </c>
       <c r="B57" t="n">
-        <v>4.60699720557514</v>
+        <v>29.6883907282474</v>
       </c>
       <c r="C57" t="n">
-        <v>12.8658850366898</v>
+        <v>94.0119198812171</v>
       </c>
       <c r="D57" t="n">
-        <v>35.9303447323567</v>
+        <v>297.700241170132</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2006</v>
+        <v>1976</v>
       </c>
       <c r="B58" t="n">
-        <v>6.17727997865887</v>
+        <v>8.70883236541928</v>
       </c>
       <c r="C58" t="n">
-        <v>17.2511878124633</v>
+        <v>27.5775827019735</v>
       </c>
       <c r="D58" t="n">
-        <v>48.1771073950084</v>
+        <v>87.3277881319712</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2007</v>
+        <v>1977</v>
       </c>
       <c r="B59" t="n">
-        <v>7.24606380332688</v>
+        <v>19.0901282415316</v>
       </c>
       <c r="C59" t="n">
-        <v>20.4917741339295</v>
+        <v>60.4512256387624</v>
       </c>
       <c r="D59" t="n">
-        <v>57.9504705662664</v>
+        <v>191.426198661062</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2008</v>
+        <v>1978</v>
       </c>
       <c r="B60" t="n">
-        <v>4.95748754930798</v>
+        <v>16.599021398818</v>
       </c>
       <c r="C60" t="n">
-        <v>13.6812044346299</v>
+        <v>52.5628311799172</v>
       </c>
       <c r="D60" t="n">
-        <v>37.7560917542327</v>
+        <v>166.446632922903</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2009</v>
+        <v>1979</v>
       </c>
       <c r="B61" t="n">
-        <v>2.90465096057709</v>
+        <v>14.2493625189755</v>
       </c>
       <c r="C61" t="n">
-        <v>8.10981640531362</v>
+        <v>45.122348993398</v>
       </c>
       <c r="D61" t="n">
-        <v>22.6426937420484</v>
+        <v>142.885436170964</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2010</v>
+        <v>1980</v>
       </c>
       <c r="B62" t="n">
-        <v>4.41305296041032</v>
+        <v>24.822841414061</v>
       </c>
       <c r="C62" t="n">
-        <v>12.313809571158</v>
+        <v>75.7037018024581</v>
       </c>
       <c r="D62" t="n">
-        <v>34.3594122968884</v>
+        <v>230.878100173864</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2011</v>
+        <v>1981</v>
       </c>
       <c r="B63" t="n">
-        <v>9.01920599063467</v>
+        <v>10.436851648221</v>
       </c>
       <c r="C63" t="n">
-        <v>25.1604910645626</v>
+        <v>31.8298897275254</v>
       </c>
       <c r="D63" t="n">
-        <v>70.1891398497027</v>
+        <v>97.073515482911</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2012</v>
+        <v>1982</v>
       </c>
       <c r="B64" t="n">
-        <v>5.42482253017743</v>
+        <v>12.7270661736823</v>
       </c>
       <c r="C64" t="n">
-        <v>13.9611212962292</v>
+        <v>38.8144937302317</v>
       </c>
       <c r="D64" t="n">
-        <v>35.9298219921031</v>
+        <v>118.374879408543</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2013</v>
+        <v>1983</v>
       </c>
       <c r="B65" t="n">
-        <v>5.27391027209802</v>
+        <v>11.7933984214012</v>
       </c>
       <c r="C65" t="n">
-        <v>13.4984245569164</v>
+        <v>35.9670314303989</v>
       </c>
       <c r="D65" t="n">
-        <v>34.5488368436497</v>
+        <v>109.690803591252</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2014</v>
+        <v>1984</v>
       </c>
       <c r="B66" t="n">
-        <v>10.7541743427589</v>
+        <v>8.65734223204555</v>
       </c>
       <c r="C66" t="n">
-        <v>28.5765714760995</v>
+        <v>26.4028135943115</v>
       </c>
       <c r="D66" t="n">
-        <v>75.9352053724588</v>
+        <v>80.5222373115365</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2015</v>
+        <v>1985</v>
       </c>
       <c r="B67" t="n">
-        <v>4.52623128177489</v>
+        <v>16.4280021216909</v>
       </c>
       <c r="C67" t="n">
-        <v>11.5259743665346</v>
+        <v>50.0629252293213</v>
       </c>
       <c r="D67" t="n">
-        <v>29.3507063222625</v>
+        <v>152.562464014257</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2016</v>
+        <v>1986</v>
       </c>
       <c r="B68" t="n">
-        <v>6.1005840606509</v>
+        <v>12.659149097954</v>
       </c>
       <c r="C68" t="n">
-        <v>15.6971604369401</v>
+        <v>37.4268286050215</v>
       </c>
       <c r="D68" t="n">
-        <v>40.3897140557959</v>
+        <v>110.652579299824</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2017</v>
+        <v>1987</v>
       </c>
       <c r="B69" t="n">
-        <v>7.16272867962695</v>
+        <v>12.5210937241605</v>
       </c>
       <c r="C69" t="n">
-        <v>18.4210175781221</v>
+        <v>37.0186673002614</v>
       </c>
       <c r="D69" t="n">
-        <v>47.3749465868582</v>
+        <v>109.445848651638</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2018</v>
+        <v>1988</v>
       </c>
       <c r="B70" t="n">
-        <v>7.13184704294509</v>
+        <v>15.7717973615232</v>
       </c>
       <c r="C70" t="n">
-        <v>18.4509539343163</v>
+        <v>46.6293865468621</v>
       </c>
       <c r="D70" t="n">
-        <v>47.7348573288638</v>
+        <v>137.859981325977</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
+        <v>1989</v>
+      </c>
+      <c r="B71" t="n">
+        <v>8.50482424880265</v>
+      </c>
+      <c r="C71" t="n">
+        <v>26.9237567116777</v>
+      </c>
+      <c r="D71" t="n">
+        <v>85.2326461151341</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>1990</v>
+      </c>
+      <c r="B72" t="n">
+        <v>8.04707581708866</v>
+      </c>
+      <c r="C72" t="n">
+        <v>24.5285116760912</v>
+      </c>
+      <c r="D72" t="n">
+        <v>74.7660266561045</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B73" t="n">
+        <v>8.94937236733877</v>
+      </c>
+      <c r="C73" t="n">
+        <v>28.3310644984066</v>
+      </c>
+      <c r="D73" t="n">
+        <v>89.6877660987925</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>1992</v>
+      </c>
+      <c r="B74" t="n">
+        <v>4.49967480585589</v>
+      </c>
+      <c r="C74" t="n">
+        <v>13.2917464166519</v>
+      </c>
+      <c r="D74" t="n">
+        <v>39.2629535304773</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1993</v>
+      </c>
+      <c r="B75" t="n">
+        <v>3.69992796324199</v>
+      </c>
+      <c r="C75" t="n">
+        <v>10.9293463126026</v>
+      </c>
+      <c r="D75" t="n">
+        <v>32.2845774316463</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>1994</v>
+      </c>
+      <c r="B76" t="n">
+        <v>14.6105220419339</v>
+      </c>
+      <c r="C76" t="n">
+        <v>43.1585308661768</v>
+      </c>
+      <c r="D76" t="n">
+        <v>127.487490260832</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>1995</v>
+      </c>
+      <c r="B77" t="n">
+        <v>3.35374901397433</v>
+      </c>
+      <c r="C77" t="n">
+        <v>10.2101649209451</v>
+      </c>
+      <c r="D77" t="n">
+        <v>31.0838608609416</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>1996</v>
+      </c>
+      <c r="B78" t="n">
+        <v>2.50618822898446</v>
+      </c>
+      <c r="C78" t="n">
+        <v>7.40311685829102</v>
+      </c>
+      <c r="D78" t="n">
+        <v>21.8683252054539</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>1997</v>
+      </c>
+      <c r="B79" t="n">
+        <v>5.78249593859973</v>
+      </c>
+      <c r="C79" t="n">
+        <v>16.3039767657935</v>
+      </c>
+      <c r="D79" t="n">
+        <v>45.9697094822178</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>1998</v>
+      </c>
+      <c r="B80" t="n">
+        <v>4.72417000310393</v>
+      </c>
+      <c r="C80" t="n">
+        <v>13.597587157718</v>
+      </c>
+      <c r="D80" t="n">
+        <v>39.137959978209</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>1999</v>
+      </c>
+      <c r="B81" t="n">
+        <v>5.75948747562664</v>
+      </c>
+      <c r="C81" t="n">
+        <v>16.5775433318789</v>
+      </c>
+      <c r="D81" t="n">
+        <v>47.7151732829185</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B82" t="n">
+        <v>4.77850801588795</v>
+      </c>
+      <c r="C82" t="n">
+        <v>14.1008024295769</v>
+      </c>
+      <c r="D82" t="n">
+        <v>41.60977202442</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>2001</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4.89074376240665</v>
+      </c>
+      <c r="C83" t="n">
+        <v>14.0770367136863</v>
+      </c>
+      <c r="D83" t="n">
+        <v>40.5179605117892</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>2002</v>
+      </c>
+      <c r="B84" t="n">
+        <v>10.2088431200926</v>
+      </c>
+      <c r="C84" t="n">
+        <v>28.7842382948437</v>
+      </c>
+      <c r="D84" t="n">
+        <v>81.1583021178635</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>2003</v>
+      </c>
+      <c r="B85" t="n">
+        <v>6.51856403431133</v>
+      </c>
+      <c r="C85" t="n">
+        <v>18.0396499708061</v>
+      </c>
+      <c r="D85" t="n">
+        <v>49.9234140151518</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B86" t="n">
+        <v>7.11573787063407</v>
+      </c>
+      <c r="C86" t="n">
+        <v>19.6922849564074</v>
+      </c>
+      <c r="D86" t="n">
+        <v>54.4969606602155</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>2005</v>
+      </c>
+      <c r="B87" t="n">
+        <v>3.63745502142446</v>
+      </c>
+      <c r="C87" t="n">
+        <v>9.76592648859136</v>
+      </c>
+      <c r="D87" t="n">
+        <v>26.2197936795989</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>2006</v>
+      </c>
+      <c r="B88" t="n">
+        <v>4.88551488703515</v>
+      </c>
+      <c r="C88" t="n">
+        <v>13.1167475514294</v>
+      </c>
+      <c r="D88" t="n">
+        <v>35.2161584410481</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>2007</v>
+      </c>
+      <c r="B89" t="n">
+        <v>5.74359771506721</v>
+      </c>
+      <c r="C89" t="n">
+        <v>15.6239292341141</v>
+      </c>
+      <c r="D89" t="n">
+        <v>42.5007420126652</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>2008</v>
+      </c>
+      <c r="B90" t="n">
+        <v>3.96123640482387</v>
+      </c>
+      <c r="C90" t="n">
+        <v>10.5027626927186</v>
+      </c>
+      <c r="D90" t="n">
+        <v>27.8468672168195</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>2009</v>
+      </c>
+      <c r="B91" t="n">
+        <v>2.3603098616807</v>
+      </c>
+      <c r="C91" t="n">
+        <v>6.33537146901125</v>
+      </c>
+      <c r="D91" t="n">
+        <v>17.0049417248045</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>2010</v>
+      </c>
+      <c r="B92" t="n">
+        <v>3.5601608634664</v>
+      </c>
+      <c r="C92" t="n">
+        <v>9.54859636706964</v>
+      </c>
+      <c r="D92" t="n">
+        <v>25.6099923789514</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B93" t="n">
+        <v>7.93759393943339</v>
+      </c>
+      <c r="C93" t="n">
+        <v>21.283018882489</v>
+      </c>
+      <c r="D93" t="n">
+        <v>57.0660197798826</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>2012</v>
+      </c>
+      <c r="B94" t="n">
+        <v>4.103653287442</v>
+      </c>
+      <c r="C94" t="n">
+        <v>10.1651269690462</v>
+      </c>
+      <c r="D94" t="n">
+        <v>25.1799552883865</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>2013</v>
+      </c>
+      <c r="B95" t="n">
+        <v>4.32038542730264</v>
+      </c>
+      <c r="C95" t="n">
+        <v>10.6379227516443</v>
+      </c>
+      <c r="D95" t="n">
+        <v>26.1933576006447</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B96" t="n">
+        <v>8.44821962376436</v>
+      </c>
+      <c r="C96" t="n">
+        <v>21.5325883829236</v>
+      </c>
+      <c r="D96" t="n">
+        <v>54.8816653823948</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B97" t="n">
+        <v>3.58235232903482</v>
+      </c>
+      <c r="C97" t="n">
+        <v>8.77113080505473</v>
+      </c>
+      <c r="D97" t="n">
+        <v>21.4754799453541</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B98" t="n">
+        <v>4.73564794298946</v>
+      </c>
+      <c r="C98" t="n">
+        <v>11.7282536135544</v>
+      </c>
+      <c r="D98" t="n">
+        <v>29.0460639134884</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B99" t="n">
+        <v>5.58282671908113</v>
+      </c>
+      <c r="C99" t="n">
+        <v>13.8179618827328</v>
+      </c>
+      <c r="D99" t="n">
+        <v>34.2006084373118</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B100" t="n">
+        <v>5.5875460063328</v>
+      </c>
+      <c r="C100" t="n">
+        <v>13.9194959591387</v>
+      </c>
+      <c r="D100" t="n">
+        <v>34.6757534590111</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
         <v>2019</v>
       </c>
-      <c r="B71" t="n">
-        <v>5.90846055709454</v>
-      </c>
-      <c r="C71" t="n">
-        <v>15.2884659618587</v>
-      </c>
-      <c r="D71" t="n">
-        <v>39.5597447437056</v>
+      <c r="B101" t="n">
+        <v>4.66393679271465</v>
+      </c>
+      <c r="C101" t="n">
+        <v>11.6205530354848</v>
+      </c>
+      <c r="D101" t="n">
+        <v>28.9534911925589</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B102" t="n">
+        <v>4.94704657208832</v>
+      </c>
+      <c r="C102" t="n">
+        <v>12.7843755866328</v>
+      </c>
+      <c r="D102" t="n">
+        <v>33.0379463298847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes pb in the map
</commit_message>
<xml_diff>
--- a/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
+++ b/R/recruitment/2021/data/glm_results_glass_and_yellow.xlsx
@@ -402,13 +402,13 @@
         <v>1960</v>
       </c>
       <c r="B2" t="n">
-        <v>61.493762969138</v>
+        <v>61.4937629691388</v>
       </c>
       <c r="C2" t="n">
-        <v>152.048111818896</v>
+        <v>152.048111818898</v>
       </c>
       <c r="D2" t="n">
-        <v>375.95078250934</v>
+        <v>375.950782509347</v>
       </c>
       <c r="E2" t="n">
         <v>50.8345557658664</v>
@@ -417,7 +417,7 @@
         <v>208.076635205517</v>
       </c>
       <c r="G2" t="n">
-        <v>851.701868269726</v>
+        <v>851.701868269725</v>
       </c>
     </row>
     <row r="3">
@@ -425,22 +425,22 @@
         <v>1961</v>
       </c>
       <c r="B3" t="n">
-        <v>61.1403408017282</v>
+        <v>61.1403408017287</v>
       </c>
       <c r="C3" t="n">
-        <v>130.372135710347</v>
+        <v>130.372135710348</v>
       </c>
       <c r="D3" t="n">
-        <v>277.99802138487</v>
+        <v>277.998021384873</v>
       </c>
       <c r="E3" t="n">
-        <v>28.6896982592744</v>
+        <v>28.6896982592743</v>
       </c>
       <c r="F3" t="n">
         <v>117.433029342214</v>
       </c>
       <c r="G3" t="n">
-        <v>480.678334636417</v>
+        <v>480.678334636414</v>
       </c>
     </row>
     <row r="4">
@@ -448,22 +448,22 @@
         <v>1962</v>
       </c>
       <c r="B4" t="n">
-        <v>73.9868111169839</v>
+        <v>73.9868111169847</v>
       </c>
       <c r="C4" t="n">
-        <v>150.558796341544</v>
+        <v>150.558796341545</v>
       </c>
       <c r="D4" t="n">
-        <v>306.378269499588</v>
+        <v>306.378269499592</v>
       </c>
       <c r="E4" t="n">
-        <v>43.8548505490427</v>
+        <v>43.8548505490428</v>
       </c>
       <c r="F4" t="n">
-        <v>179.507219099431</v>
+        <v>179.507219099432</v>
       </c>
       <c r="G4" t="n">
-        <v>734.76117933127</v>
+        <v>734.761179331272</v>
       </c>
     </row>
     <row r="5">
@@ -471,22 +471,22 @@
         <v>1963</v>
       </c>
       <c r="B5" t="n">
-        <v>95.6318096561446</v>
+        <v>95.6318096561455</v>
       </c>
       <c r="C5" t="n">
-        <v>194.605091588919</v>
+        <v>194.605091588921</v>
       </c>
       <c r="D5" t="n">
-        <v>396.009882156385</v>
+        <v>396.009882156389</v>
       </c>
       <c r="E5" t="n">
-        <v>54.8839835478431</v>
+        <v>54.883983547845</v>
       </c>
       <c r="F5" t="n">
-        <v>224.651803310895</v>
+        <v>224.651803310904</v>
       </c>
       <c r="G5" t="n">
-        <v>919.547552280768</v>
+        <v>919.547552280805</v>
       </c>
     </row>
     <row r="6">
@@ -494,22 +494,22 @@
         <v>1964</v>
       </c>
       <c r="B6" t="n">
-        <v>48.5223266316684</v>
+        <v>48.5223266316689</v>
       </c>
       <c r="C6" t="n">
-        <v>119.975226578793</v>
+        <v>119.975226578794</v>
       </c>
       <c r="D6" t="n">
-        <v>296.648079180075</v>
+        <v>296.648079180078</v>
       </c>
       <c r="E6" t="n">
-        <v>34.3683156028316</v>
+        <v>34.3683156028325</v>
       </c>
       <c r="F6" t="n">
-        <v>116.378709121198</v>
+        <v>116.378709121202</v>
       </c>
       <c r="G6" t="n">
-        <v>394.084018932853</v>
+        <v>394.084018932863</v>
       </c>
     </row>
     <row r="7">
@@ -517,22 +517,22 @@
         <v>1965</v>
       </c>
       <c r="B7" t="n">
-        <v>66.4211309922307</v>
+        <v>66.4211309922311</v>
       </c>
       <c r="C7" t="n">
-        <v>135.163083566642</v>
+        <v>135.163083566643</v>
       </c>
       <c r="D7" t="n">
-        <v>275.048902154044</v>
+        <v>275.048902154046</v>
       </c>
       <c r="E7" t="n">
-        <v>23.282747825619</v>
+        <v>23.2827478256188</v>
       </c>
       <c r="F7" t="n">
-        <v>78.8405276549747</v>
+        <v>78.8405276549737</v>
       </c>
       <c r="G7" t="n">
-        <v>266.97144372604</v>
+        <v>266.971443726036</v>
       </c>
     </row>
     <row r="8">
@@ -540,22 +540,22 @@
         <v>1966</v>
       </c>
       <c r="B8" t="n">
-        <v>40.4174143964253</v>
+        <v>40.4174143964237</v>
       </c>
       <c r="C8" t="n">
-        <v>75.6222310982888</v>
+        <v>75.6222310982863</v>
       </c>
       <c r="D8" t="n">
-        <v>141.491530858263</v>
+        <v>141.491530858259</v>
       </c>
       <c r="E8" t="n">
-        <v>26.0687162261693</v>
+        <v>26.0687162261691</v>
       </c>
       <c r="F8" t="n">
-        <v>88.2744321225472</v>
+        <v>88.2744321225465</v>
       </c>
       <c r="G8" t="n">
-        <v>298.916728347971</v>
+        <v>298.916728347968</v>
       </c>
     </row>
     <row r="9">
@@ -563,22 +563,22 @@
         <v>1967</v>
       </c>
       <c r="B9" t="n">
-        <v>43.1856351433704</v>
+        <v>43.1856351433659</v>
       </c>
       <c r="C9" t="n">
-        <v>80.8016576445626</v>
+        <v>80.8016576445535</v>
       </c>
       <c r="D9" t="n">
-        <v>151.182397953255</v>
+        <v>151.182397953237</v>
       </c>
       <c r="E9" t="n">
-        <v>28.8813838175803</v>
+        <v>28.8813838175798</v>
       </c>
       <c r="F9" t="n">
-        <v>97.7987459486361</v>
+        <v>97.7987459486341</v>
       </c>
       <c r="G9" t="n">
-        <v>331.168159030657</v>
+        <v>331.168159030649</v>
       </c>
     </row>
     <row r="10">
@@ -586,13 +586,13 @@
         <v>1968</v>
       </c>
       <c r="B10" t="n">
-        <v>68.7353075349682</v>
+        <v>68.7353075349748</v>
       </c>
       <c r="C10" t="n">
-        <v>128.605884088445</v>
+        <v>128.605884088458</v>
       </c>
       <c r="D10" t="n">
-        <v>240.625582620057</v>
+        <v>240.625582620085</v>
       </c>
       <c r="E10" t="n">
         <v>36.6677596715368</v>
@@ -601,7 +601,7 @@
         <v>124.165134720429</v>
       </c>
       <c r="G10" t="n">
-        <v>420.450576153134</v>
+        <v>420.450576153132</v>
       </c>
     </row>
     <row r="11">
@@ -609,19 +609,19 @@
         <v>1969</v>
       </c>
       <c r="B11" t="n">
-        <v>35.9771450278742</v>
+        <v>35.9771450278757</v>
       </c>
       <c r="C11" t="n">
-        <v>67.3143499202962</v>
+        <v>67.3143499202989</v>
       </c>
       <c r="D11" t="n">
-        <v>125.947228488569</v>
+        <v>125.947228488575</v>
       </c>
       <c r="E11" t="n">
-        <v>29.3888258045362</v>
+        <v>29.3888258045363</v>
       </c>
       <c r="F11" t="n">
-        <v>89.5741510337175</v>
+        <v>89.5741510337179</v>
       </c>
       <c r="G11" t="n">
         <v>273.012899078561</v>
@@ -632,22 +632,22 @@
         <v>1970</v>
       </c>
       <c r="B12" t="n">
-        <v>54.1880288468947</v>
+        <v>54.1880288468922</v>
       </c>
       <c r="C12" t="n">
-        <v>101.387476200929</v>
+        <v>101.387476200924</v>
       </c>
       <c r="D12" t="n">
-        <v>189.699100504981</v>
+        <v>189.699100504971</v>
       </c>
       <c r="E12" t="n">
-        <v>32.3361808987327</v>
+        <v>32.3361808987329</v>
       </c>
       <c r="F12" t="n">
-        <v>98.557389496984</v>
+        <v>98.5573894969848</v>
       </c>
       <c r="G12" t="n">
-        <v>300.392895960108</v>
+        <v>300.39289596011</v>
       </c>
     </row>
     <row r="13">
@@ -655,22 +655,22 @@
         <v>1971</v>
       </c>
       <c r="B13" t="n">
-        <v>30.4267900149791</v>
+        <v>30.426790014979</v>
       </c>
       <c r="C13" t="n">
-        <v>55.4957607589901</v>
+        <v>55.49576075899</v>
       </c>
       <c r="D13" t="n">
         <v>101.219335352263</v>
       </c>
       <c r="E13" t="n">
-        <v>27.7503135098608</v>
+        <v>27.7503135098606</v>
       </c>
       <c r="F13" t="n">
-        <v>84.8783838350535</v>
+        <v>84.8783838350529</v>
       </c>
       <c r="G13" t="n">
-        <v>259.612924368969</v>
+        <v>259.612924368967</v>
       </c>
     </row>
     <row r="14">
@@ -678,22 +678,22 @@
         <v>1972</v>
       </c>
       <c r="B14" t="n">
-        <v>28.1050423646579</v>
+        <v>28.1050423646568</v>
       </c>
       <c r="C14" t="n">
-        <v>50.1621954024902</v>
+        <v>50.1621954024883</v>
       </c>
       <c r="D14" t="n">
-        <v>89.5300499799918</v>
+        <v>89.5300499799887</v>
       </c>
       <c r="E14" t="n">
-        <v>38.1999156648299</v>
+        <v>38.1999156648305</v>
       </c>
       <c r="F14" t="n">
-        <v>108.940385006265</v>
+        <v>108.940385006266</v>
       </c>
       <c r="G14" t="n">
-        <v>310.681510122807</v>
+        <v>310.681510122811</v>
       </c>
     </row>
     <row r="15">
@@ -701,22 +701,22 @@
         <v>1973</v>
       </c>
       <c r="B15" t="n">
-        <v>31.1073177013833</v>
+        <v>31.1073177013829</v>
       </c>
       <c r="C15" t="n">
-        <v>55.5206901572357</v>
+        <v>55.5206901572343</v>
       </c>
       <c r="D15" t="n">
-        <v>99.093951626652</v>
+        <v>99.0939516266482</v>
       </c>
       <c r="E15" t="n">
-        <v>17.3976509095919</v>
+        <v>17.3976509095918</v>
       </c>
       <c r="F15" t="n">
-        <v>47.2551422983527</v>
+        <v>47.2551422983522</v>
       </c>
       <c r="G15" t="n">
-        <v>128.3534475569</v>
+        <v>128.353447556898</v>
       </c>
     </row>
     <row r="16">
@@ -724,22 +724,22 @@
         <v>1974</v>
       </c>
       <c r="B16" t="n">
-        <v>47.3528068562281</v>
+        <v>47.3528068562271</v>
       </c>
       <c r="C16" t="n">
-        <v>82.952392022457</v>
+        <v>82.952392022455</v>
       </c>
       <c r="D16" t="n">
-        <v>145.315553587767</v>
+        <v>145.315553587763</v>
       </c>
       <c r="E16" t="n">
-        <v>45.9690206521592</v>
+        <v>45.9690206521596</v>
       </c>
       <c r="F16" t="n">
-        <v>131.096698017526</v>
+        <v>131.096698017527</v>
       </c>
       <c r="G16" t="n">
-        <v>373.867965583711</v>
+        <v>373.867965583713</v>
       </c>
     </row>
     <row r="17">
@@ -747,22 +747,22 @@
         <v>1975</v>
       </c>
       <c r="B17" t="n">
-        <v>42.043294402403</v>
+        <v>42.0432944024063</v>
       </c>
       <c r="C17" t="n">
-        <v>71.4364542614649</v>
+        <v>71.4364542614705</v>
       </c>
       <c r="D17" t="n">
-        <v>121.378856485583</v>
+        <v>121.378856485592</v>
       </c>
       <c r="E17" t="n">
         <v>20.6687817599012</v>
       </c>
       <c r="F17" t="n">
-        <v>54.2019441566602</v>
+        <v>54.20194415666</v>
       </c>
       <c r="G17" t="n">
-        <v>142.139521549419</v>
+        <v>142.139521549418</v>
       </c>
     </row>
     <row r="18">
@@ -770,22 +770,22 @@
         <v>1976</v>
       </c>
       <c r="B18" t="n">
-        <v>68.3853680212471</v>
+        <v>68.385368021244</v>
       </c>
       <c r="C18" t="n">
-        <v>116.194705582445</v>
+        <v>116.194705582439</v>
       </c>
       <c r="D18" t="n">
-        <v>197.428338781422</v>
+        <v>197.428338781412</v>
       </c>
       <c r="E18" t="n">
-        <v>38.3968649093513</v>
+        <v>38.3968649093507</v>
       </c>
       <c r="F18" t="n">
-        <v>97.7610289729989</v>
+        <v>97.7610289729972</v>
       </c>
       <c r="G18" t="n">
-        <v>248.906227329303</v>
+        <v>248.906227329298</v>
       </c>
     </row>
     <row r="19">
@@ -793,16 +793,16 @@
         <v>1977</v>
       </c>
       <c r="B19" t="n">
-        <v>65.7047744199338</v>
+        <v>65.7047744199357</v>
       </c>
       <c r="C19" t="n">
-        <v>114.54653526893</v>
+        <v>114.546535268934</v>
       </c>
       <c r="D19" t="n">
-        <v>199.694905856576</v>
+        <v>199.694905856583</v>
       </c>
       <c r="E19" t="n">
-        <v>29.137930626554</v>
+        <v>29.1379306265541</v>
       </c>
       <c r="F19" t="n">
         <v>74.1890875258781</v>
@@ -816,22 +816,22 @@
         <v>1978</v>
       </c>
       <c r="B20" t="n">
-        <v>63.1711594810196</v>
+        <v>63.1711594810186</v>
       </c>
       <c r="C20" t="n">
-        <v>110.12731373505</v>
+        <v>110.127313735048</v>
       </c>
       <c r="D20" t="n">
-        <v>191.986744111323</v>
+        <v>191.986744111319</v>
       </c>
       <c r="E20" t="n">
-        <v>21.5546674934246</v>
+        <v>21.5546674934244</v>
       </c>
       <c r="F20" t="n">
-        <v>54.8810803950355</v>
+        <v>54.8810803950348</v>
       </c>
       <c r="G20" t="n">
-        <v>139.734606727066</v>
+        <v>139.734606727064</v>
       </c>
     </row>
     <row r="21">
@@ -839,22 +839,22 @@
         <v>1979</v>
       </c>
       <c r="B21" t="n">
-        <v>86.7791024231333</v>
+        <v>86.779102423135</v>
       </c>
       <c r="C21" t="n">
-        <v>147.468163972069</v>
+        <v>147.468163972073</v>
       </c>
       <c r="D21" t="n">
-        <v>250.600188041308</v>
+        <v>250.600188041317</v>
       </c>
       <c r="E21" t="n">
-        <v>38.7333137017975</v>
+        <v>38.7333137017973</v>
       </c>
       <c r="F21" t="n">
-        <v>94.5717907249417</v>
+        <v>94.5717907249412</v>
       </c>
       <c r="G21" t="n">
-        <v>230.907783149654</v>
+        <v>230.907783149652</v>
       </c>
     </row>
     <row r="22">
@@ -862,22 +862,22 @@
         <v>1980</v>
       </c>
       <c r="B22" t="n">
-        <v>68.380598478324</v>
+        <v>68.3805984783242</v>
       </c>
       <c r="C22" t="n">
-        <v>114.736724518895</v>
+        <v>114.736724518896</v>
       </c>
       <c r="D22" t="n">
-        <v>192.518290952044</v>
+        <v>192.518290952047</v>
       </c>
       <c r="E22" t="n">
-        <v>32.6946909308633</v>
+        <v>32.6946909308632</v>
       </c>
       <c r="F22" t="n">
-        <v>81.3861581734682</v>
+        <v>81.3861581734678</v>
       </c>
       <c r="G22" t="n">
-        <v>202.592731530737</v>
+        <v>202.592731530735</v>
       </c>
     </row>
     <row r="23">
@@ -885,22 +885,22 @@
         <v>1981</v>
       </c>
       <c r="B23" t="n">
-        <v>52.0057953726676</v>
+        <v>52.0057953726687</v>
       </c>
       <c r="C23" t="n">
-        <v>89.3314090811445</v>
+        <v>89.3314090811465</v>
       </c>
       <c r="D23" t="n">
-        <v>153.446372490571</v>
+        <v>153.446372490575</v>
       </c>
       <c r="E23" t="n">
-        <v>24.1103673945081</v>
+        <v>24.1103673945079</v>
       </c>
       <c r="F23" t="n">
-        <v>57.9241143470729</v>
+        <v>57.9241143470721</v>
       </c>
       <c r="G23" t="n">
-        <v>139.160178191935</v>
+        <v>139.160178191933</v>
       </c>
     </row>
     <row r="24">
@@ -908,22 +908,22 @@
         <v>1982</v>
       </c>
       <c r="B24" t="n">
-        <v>54.948559535706</v>
+        <v>54.9485595357049</v>
       </c>
       <c r="C24" t="n">
-        <v>92.0559830811496</v>
+        <v>92.0559830811476</v>
       </c>
       <c r="D24" t="n">
-        <v>154.222496324589</v>
+        <v>154.222496324586</v>
       </c>
       <c r="E24" t="n">
         <v>11.9438581285676</v>
       </c>
       <c r="F24" t="n">
-        <v>29.1342958443738</v>
+        <v>29.1342958443737</v>
       </c>
       <c r="G24" t="n">
-        <v>71.0664163296867</v>
+        <v>71.0664163296861</v>
       </c>
     </row>
     <row r="25">
@@ -931,22 +931,22 @@
         <v>1983</v>
       </c>
       <c r="B25" t="n">
-        <v>28.8749373964071</v>
+        <v>28.8749373964082</v>
       </c>
       <c r="C25" t="n">
-        <v>48.9435421681937</v>
+        <v>48.9435421681957</v>
       </c>
       <c r="D25" t="n">
-        <v>82.9601909463473</v>
+        <v>82.9601909463509</v>
       </c>
       <c r="E25" t="n">
-        <v>9.57547277466898</v>
+        <v>9.57547277466889</v>
       </c>
       <c r="F25" t="n">
-        <v>23.3571642985021</v>
+        <v>23.3571642985018</v>
       </c>
       <c r="G25" t="n">
-        <v>56.9744321669882</v>
+        <v>56.9744321669874</v>
       </c>
     </row>
     <row r="26">
@@ -954,22 +954,22 @@
         <v>1984</v>
       </c>
       <c r="B26" t="n">
-        <v>31.7513717042807</v>
+        <v>31.7513717042816</v>
       </c>
       <c r="C26" t="n">
-        <v>53.82209307889</v>
+        <v>53.8220930788916</v>
       </c>
       <c r="D26" t="n">
-        <v>91.2344112365433</v>
+        <v>91.2344112365462</v>
       </c>
       <c r="E26" t="n">
-        <v>4.02920169478405</v>
+        <v>4.02920169478403</v>
       </c>
       <c r="F26" t="n">
-        <v>9.67998271769398</v>
+        <v>9.67998271769389</v>
       </c>
       <c r="G26" t="n">
-        <v>23.2557396012602</v>
+        <v>23.2557396012599</v>
       </c>
     </row>
     <row r="27">
@@ -977,22 +977,22 @@
         <v>1985</v>
       </c>
       <c r="B27" t="n">
-        <v>31.8037610957742</v>
+        <v>31.8037610957715</v>
       </c>
       <c r="C27" t="n">
-        <v>52.2396834951238</v>
+        <v>52.2396834951194</v>
       </c>
       <c r="D27" t="n">
-        <v>85.806974950309</v>
+        <v>85.8069749503018</v>
       </c>
       <c r="E27" t="n">
         <v>3.25998294081414</v>
       </c>
       <c r="F27" t="n">
-        <v>7.83196794737511</v>
+        <v>7.83196794737507</v>
       </c>
       <c r="G27" t="n">
-        <v>18.8159640839692</v>
+        <v>18.815964083969</v>
       </c>
     </row>
     <row r="28">
@@ -1000,22 +1000,22 @@
         <v>1986</v>
       </c>
       <c r="B28" t="n">
-        <v>20.5379954028191</v>
+        <v>20.5379954028206</v>
       </c>
       <c r="C28" t="n">
-        <v>34.0669623675595</v>
+        <v>34.066962367562</v>
       </c>
       <c r="D28" t="n">
-        <v>56.5078481219942</v>
+        <v>56.5078481219985</v>
       </c>
       <c r="E28" t="n">
-        <v>3.309622439834</v>
+        <v>3.30962243983398</v>
       </c>
       <c r="F28" t="n">
-        <v>8.08001721451591</v>
+        <v>8.08001721451583</v>
       </c>
       <c r="G28" t="n">
-        <v>19.7263220726011</v>
+        <v>19.7263220726008</v>
       </c>
     </row>
     <row r="29">
@@ -1023,22 +1023,22 @@
         <v>1987</v>
       </c>
       <c r="B29" t="n">
-        <v>36.2272379452304</v>
+        <v>36.2272379452312</v>
       </c>
       <c r="C29" t="n">
-        <v>58.9683853842759</v>
+        <v>58.9683853842773</v>
       </c>
       <c r="D29" t="n">
-        <v>95.9849735186972</v>
+        <v>95.9849735186997</v>
       </c>
       <c r="E29" t="n">
-        <v>3.80009070915391</v>
+        <v>3.80009070915389</v>
       </c>
       <c r="F29" t="n">
-        <v>9.27754006609873</v>
+        <v>9.27754006609865</v>
       </c>
       <c r="G29" t="n">
-        <v>22.6501829208259</v>
+        <v>22.6501829208257</v>
       </c>
     </row>
     <row r="30">
@@ -1046,22 +1046,22 @@
         <v>1988</v>
       </c>
       <c r="B30" t="n">
-        <v>42.4449019816901</v>
+        <v>42.4449019816911</v>
       </c>
       <c r="C30" t="n">
-        <v>69.7467425529649</v>
+        <v>69.7467425529665</v>
       </c>
       <c r="D30" t="n">
-        <v>114.609950067692</v>
+        <v>114.609950067694</v>
       </c>
       <c r="E30" t="n">
-        <v>3.89249091842567</v>
+        <v>3.89249091842565</v>
       </c>
       <c r="F30" t="n">
-        <v>9.34867074954462</v>
+        <v>9.34867074954453</v>
       </c>
       <c r="G30" t="n">
-        <v>22.4528834144947</v>
+        <v>22.4528834144945</v>
       </c>
     </row>
     <row r="31">
@@ -1069,22 +1069,22 @@
         <v>1989</v>
       </c>
       <c r="B31" t="n">
-        <v>27.1686358174029</v>
+        <v>27.1686358174015</v>
       </c>
       <c r="C31" t="n">
-        <v>45.0778110655666</v>
+        <v>45.0778110655641</v>
       </c>
       <c r="D31" t="n">
-        <v>74.7924578959283</v>
+        <v>74.7924578959241</v>
       </c>
       <c r="E31" t="n">
-        <v>1.66982794410142</v>
+        <v>1.66982794410141</v>
       </c>
       <c r="F31" t="n">
-        <v>3.95641574358921</v>
+        <v>3.95641574358917</v>
       </c>
       <c r="G31" t="n">
-        <v>9.37415473936388</v>
+        <v>9.37415473936375</v>
       </c>
     </row>
     <row r="32">
@@ -1092,22 +1092,22 @@
         <v>1990</v>
       </c>
       <c r="B32" t="n">
-        <v>21.5648558935236</v>
+        <v>21.5648558935234</v>
       </c>
       <c r="C32" t="n">
-        <v>35.4097935883272</v>
+        <v>35.409793588327</v>
       </c>
       <c r="D32" t="n">
-        <v>58.1433740229397</v>
+        <v>58.1433740229396</v>
       </c>
       <c r="E32" t="n">
-        <v>5.98930679909997</v>
+        <v>5.98930679909995</v>
       </c>
       <c r="F32" t="n">
-        <v>14.5863980930769</v>
+        <v>14.5863980930768</v>
       </c>
       <c r="G32" t="n">
-        <v>35.523812098203</v>
+        <v>35.5238120982027</v>
       </c>
     </row>
     <row r="33">
@@ -1115,22 +1115,22 @@
         <v>1991</v>
       </c>
       <c r="B33" t="n">
-        <v>10.4338743491426</v>
+        <v>10.4338743491427</v>
       </c>
       <c r="C33" t="n">
-        <v>17.3069668109526</v>
+        <v>17.3069668109528</v>
       </c>
       <c r="D33" t="n">
-        <v>28.7075625191928</v>
+        <v>28.7075625191931</v>
       </c>
       <c r="E33" t="n">
-        <v>1.35497070199326</v>
+        <v>1.35497070199325</v>
       </c>
       <c r="F33" t="n">
-        <v>3.2943299364804</v>
+        <v>3.29432993648039</v>
       </c>
       <c r="G33" t="n">
-        <v>8.0094792562127</v>
+        <v>8.00947925621266</v>
       </c>
     </row>
     <row r="34">
@@ -1138,22 +1138,22 @@
         <v>1992</v>
       </c>
       <c r="B34" t="n">
-        <v>13.269479386536</v>
+        <v>13.2694793865352</v>
       </c>
       <c r="C34" t="n">
-        <v>22.0104662617745</v>
+        <v>22.0104662617732</v>
       </c>
       <c r="D34" t="n">
-        <v>36.5093920378124</v>
+        <v>36.5093920378104</v>
       </c>
       <c r="E34" t="n">
-        <v>3.2447771371577</v>
+        <v>3.24477713715767</v>
       </c>
       <c r="F34" t="n">
-        <v>7.77173752098619</v>
+        <v>7.77173752098609</v>
       </c>
       <c r="G34" t="n">
-        <v>18.6145000232628</v>
+        <v>18.6145000232625</v>
       </c>
     </row>
     <row r="35">
@@ -1164,19 +1164,19 @@
         <v>14.6871212852401</v>
       </c>
       <c r="C35" t="n">
-        <v>24.1164576144126</v>
+        <v>24.1164576144128</v>
       </c>
       <c r="D35" t="n">
-        <v>39.5995591356794</v>
+        <v>39.5995591356798</v>
       </c>
       <c r="E35" t="n">
-        <v>2.88773684672118</v>
+        <v>2.88773684672115</v>
       </c>
       <c r="F35" t="n">
-        <v>6.91657141730734</v>
+        <v>6.91657141730724</v>
       </c>
       <c r="G35" t="n">
-        <v>16.5662464102401</v>
+        <v>16.5662464102398</v>
       </c>
     </row>
     <row r="36">
@@ -1187,19 +1187,19 @@
         <v>14.7479492731129</v>
       </c>
       <c r="C36" t="n">
-        <v>23.6287857263192</v>
+        <v>23.6287857263191</v>
       </c>
       <c r="D36" t="n">
-        <v>37.85743390901</v>
+        <v>37.8574339090098</v>
       </c>
       <c r="E36" t="n">
         <v>2.82243195486673</v>
       </c>
       <c r="F36" t="n">
-        <v>6.76015621315751</v>
+        <v>6.76015621315749</v>
       </c>
       <c r="G36" t="n">
-        <v>16.1916080731342</v>
+        <v>16.1916080731341</v>
       </c>
     </row>
     <row r="37">
@@ -1207,22 +1207,22 @@
         <v>1995</v>
       </c>
       <c r="B37" t="n">
-        <v>19.2808203812939</v>
+        <v>19.2808203812948</v>
       </c>
       <c r="C37" t="n">
-        <v>31.1217346137179</v>
+        <v>31.1217346137196</v>
       </c>
       <c r="D37" t="n">
-        <v>50.2344996847945</v>
+        <v>50.2344996847975</v>
       </c>
       <c r="E37" t="n">
-        <v>2.04581268013523</v>
+        <v>2.04581268013522</v>
       </c>
       <c r="F37" t="n">
-        <v>4.90003426893092</v>
+        <v>4.90003426893087</v>
       </c>
       <c r="G37" t="n">
-        <v>11.7363315174634</v>
+        <v>11.7363315174632</v>
       </c>
     </row>
     <row r="38">
@@ -1230,22 +1230,22 @@
         <v>1996</v>
       </c>
       <c r="B38" t="n">
-        <v>15.6103758452899</v>
+        <v>15.61037584529</v>
       </c>
       <c r="C38" t="n">
-        <v>25.0113913128226</v>
+        <v>25.0113913128229</v>
       </c>
       <c r="D38" t="n">
-        <v>40.0739675715041</v>
+        <v>40.0739675715049</v>
       </c>
       <c r="E38" t="n">
-        <v>2.04891382587148</v>
+        <v>2.04891382587147</v>
       </c>
       <c r="F38" t="n">
-        <v>4.90746198727879</v>
+        <v>4.90746198727876</v>
       </c>
       <c r="G38" t="n">
-        <v>11.7541220389505</v>
+        <v>11.7541220389504</v>
       </c>
     </row>
     <row r="39">
@@ -1253,22 +1253,22 @@
         <v>1997</v>
       </c>
       <c r="B39" t="n">
-        <v>25.8501675375538</v>
+        <v>25.8501675375542</v>
       </c>
       <c r="C39" t="n">
-        <v>41.1358405365615</v>
+        <v>41.1358405365621</v>
       </c>
       <c r="D39" t="n">
-        <v>65.4602092690942</v>
+        <v>65.4602092690952</v>
       </c>
       <c r="E39" t="n">
-        <v>1.7806567604346</v>
+        <v>1.78065676043458</v>
       </c>
       <c r="F39" t="n">
-        <v>4.26494528656273</v>
+        <v>4.26494528656269</v>
       </c>
       <c r="G39" t="n">
-        <v>10.2151962700179</v>
+        <v>10.2151962700178</v>
       </c>
     </row>
     <row r="40">
@@ -1276,22 +1276,22 @@
         <v>1998</v>
       </c>
       <c r="B40" t="n">
-        <v>10.266540236628</v>
+        <v>10.2665402366284</v>
       </c>
       <c r="C40" t="n">
-        <v>16.3437769301607</v>
+        <v>16.3437769301611</v>
       </c>
       <c r="D40" t="n">
-        <v>26.0184091413629</v>
+        <v>26.0184091413634</v>
       </c>
       <c r="E40" t="n">
-        <v>1.29479875637914</v>
+        <v>1.29479875637913</v>
       </c>
       <c r="F40" t="n">
-        <v>3.10124105654068</v>
+        <v>3.10124105654067</v>
       </c>
       <c r="G40" t="n">
-        <v>7.427946654559</v>
+        <v>7.42794665455894</v>
       </c>
     </row>
     <row r="41">
@@ -1299,22 +1299,22 @@
         <v>1999</v>
       </c>
       <c r="B41" t="n">
-        <v>11.8389177440226</v>
+        <v>11.8389177440223</v>
       </c>
       <c r="C41" t="n">
-        <v>19.1201516308863</v>
+        <v>19.1201516308858</v>
       </c>
       <c r="D41" t="n">
-        <v>30.8795285424349</v>
+        <v>30.8795285424341</v>
       </c>
       <c r="E41" t="n">
-        <v>2.7152566990306</v>
+        <v>2.71525669903058</v>
       </c>
       <c r="F41" t="n">
-        <v>6.60479666028117</v>
+        <v>6.60479666028111</v>
       </c>
       <c r="G41" t="n">
-        <v>16.066009132483</v>
+        <v>16.0660091324828</v>
       </c>
     </row>
     <row r="42">
@@ -1322,22 +1322,22 @@
         <v>2000</v>
       </c>
       <c r="B42" t="n">
-        <v>12.080960266145</v>
+        <v>12.0809602661449</v>
       </c>
       <c r="C42" t="n">
-        <v>19.3664706601411</v>
+        <v>19.3664706601408</v>
       </c>
       <c r="D42" t="n">
-        <v>31.0455607474477</v>
+        <v>31.0455607474472</v>
       </c>
       <c r="E42" t="n">
-        <v>1.97428012729895</v>
+        <v>1.97428012729894</v>
       </c>
       <c r="F42" t="n">
-        <v>4.72870286423031</v>
+        <v>4.72870286423027</v>
       </c>
       <c r="G42" t="n">
-        <v>11.3259665986568</v>
+        <v>11.3259665986567</v>
       </c>
     </row>
     <row r="43">
@@ -1345,22 +1345,22 @@
         <v>2001</v>
       </c>
       <c r="B43" t="n">
-        <v>5.56957895433922</v>
+        <v>5.56957895433941</v>
       </c>
       <c r="C43" t="n">
-        <v>8.80843897289129</v>
+        <v>8.80843897289157</v>
       </c>
       <c r="D43" t="n">
-        <v>13.9307832378786</v>
+        <v>13.930783237879</v>
       </c>
       <c r="E43" t="n">
-        <v>0.420545141794988</v>
+        <v>0.420545141794986</v>
       </c>
       <c r="F43" t="n">
-        <v>1.00726993553077</v>
+        <v>1.00726993553076</v>
       </c>
       <c r="G43" t="n">
-        <v>2.41256555406547</v>
+        <v>2.41256555406544</v>
       </c>
     </row>
     <row r="44">
@@ -1368,22 +1368,22 @@
         <v>2002</v>
       </c>
       <c r="B44" t="n">
-        <v>7.73708835606294</v>
+        <v>7.73708835606315</v>
       </c>
       <c r="C44" t="n">
-        <v>12.3136897061217</v>
+        <v>12.313689706122</v>
       </c>
       <c r="D44" t="n">
-        <v>19.597417943383</v>
+        <v>19.5974179433834</v>
       </c>
       <c r="E44" t="n">
         <v>1.05274916457164</v>
       </c>
       <c r="F44" t="n">
-        <v>2.55864191368098</v>
+        <v>2.55864191368096</v>
       </c>
       <c r="G44" t="n">
-        <v>6.21862136087174</v>
+        <v>6.21862136087167</v>
       </c>
     </row>
     <row r="45">
@@ -1391,22 +1391,22 @@
         <v>2003</v>
       </c>
       <c r="B45" t="n">
-        <v>8.36145906684725</v>
+        <v>8.36145906684732</v>
       </c>
       <c r="C45" t="n">
-        <v>13.1477615669177</v>
+        <v>13.1477615669178</v>
       </c>
       <c r="D45" t="n">
-        <v>20.6738600091834</v>
+        <v>20.6738600091836</v>
       </c>
       <c r="E45" t="n">
-        <v>0.773797811831294</v>
+        <v>0.773797811831293</v>
       </c>
       <c r="F45" t="n">
         <v>1.91441845468173</v>
       </c>
       <c r="G45" t="n">
-        <v>4.73637682038968</v>
+        <v>4.73637682038966</v>
       </c>
     </row>
     <row r="46">
@@ -1414,22 +1414,22 @@
         <v>2004</v>
       </c>
       <c r="B46" t="n">
-        <v>4.58979645069198</v>
+        <v>4.58979645069207</v>
       </c>
       <c r="C46" t="n">
-        <v>7.26017765152278</v>
+        <v>7.26017765152291</v>
       </c>
       <c r="D46" t="n">
-        <v>11.4842085260064</v>
+        <v>11.4842085260066</v>
       </c>
       <c r="E46" t="n">
-        <v>0.270691826796919</v>
+        <v>0.270691826796917</v>
       </c>
       <c r="F46" t="n">
-        <v>0.64805628678546</v>
+        <v>0.648056286785454</v>
       </c>
       <c r="G46" t="n">
-        <v>1.55149475997012</v>
+        <v>1.5514947599701</v>
       </c>
     </row>
     <row r="47">
@@ -1437,22 +1437,22 @@
         <v>2005</v>
       </c>
       <c r="B47" t="n">
-        <v>4.66951791775726</v>
+        <v>4.66951791775744</v>
       </c>
       <c r="C47" t="n">
-        <v>7.38639114768742</v>
+        <v>7.38639114768769</v>
       </c>
       <c r="D47" t="n">
-        <v>11.6840271624526</v>
+        <v>11.684027162453</v>
       </c>
       <c r="E47" t="n">
-        <v>0.447670818874421</v>
+        <v>0.44767081887442</v>
       </c>
       <c r="F47" t="n">
-        <v>1.0878301270177</v>
+        <v>1.08783012701769</v>
       </c>
       <c r="G47" t="n">
-        <v>2.64340299915616</v>
+        <v>2.64340299915614</v>
       </c>
     </row>
     <row r="48">
@@ -1463,19 +1463,19 @@
         <v>3.82001976557222</v>
       </c>
       <c r="C48" t="n">
-        <v>5.977030953534</v>
+        <v>5.97703095353402</v>
       </c>
       <c r="D48" t="n">
-        <v>9.35201941662001</v>
+        <v>9.35201941662004</v>
       </c>
       <c r="E48" t="n">
-        <v>0.193652305624083</v>
+        <v>0.193652305624082</v>
       </c>
       <c r="F48" t="n">
-        <v>0.452860935666484</v>
+        <v>0.452860935666482</v>
       </c>
       <c r="G48" t="n">
-        <v>1.05902703503479</v>
+        <v>1.05902703503478</v>
       </c>
     </row>
     <row r="49">
@@ -1483,22 +1483,22 @@
         <v>2007</v>
       </c>
       <c r="B49" t="n">
-        <v>4.08335316136952</v>
+        <v>4.08335316136946</v>
       </c>
       <c r="C49" t="n">
-        <v>6.42812476085872</v>
+        <v>6.42812476085862</v>
       </c>
       <c r="D49" t="n">
-        <v>10.1193275007607</v>
+        <v>10.1193275007606</v>
       </c>
       <c r="E49" t="n">
-        <v>0.566512854970824</v>
+        <v>0.566512854970822</v>
       </c>
       <c r="F49" t="n">
-        <v>1.31234860382227</v>
+        <v>1.31234860382226</v>
       </c>
       <c r="G49" t="n">
-        <v>3.04010552071755</v>
+        <v>3.04010552071752</v>
       </c>
     </row>
     <row r="50">
@@ -1506,22 +1506,22 @@
         <v>2008</v>
       </c>
       <c r="B50" t="n">
-        <v>3.64090570299035</v>
+        <v>3.64090570299053</v>
       </c>
       <c r="C50" t="n">
-        <v>5.72832290424384</v>
+        <v>5.72832290424408</v>
       </c>
       <c r="D50" t="n">
-        <v>9.01250567086481</v>
+        <v>9.01250567086514</v>
       </c>
       <c r="E50" t="n">
-        <v>0.514946587265635</v>
+        <v>0.514946587265633</v>
       </c>
       <c r="F50" t="n">
-        <v>1.17025035149354</v>
+        <v>1.17025035149353</v>
       </c>
       <c r="G50" t="n">
-        <v>2.65947171811105</v>
+        <v>2.65947171811102</v>
       </c>
     </row>
     <row r="51">
@@ -1529,19 +1529,19 @@
         <v>2009</v>
       </c>
       <c r="B51" t="n">
-        <v>2.58543689796428</v>
+        <v>2.58543689796431</v>
       </c>
       <c r="C51" t="n">
-        <v>4.30725534599828</v>
+        <v>4.30725534599832</v>
       </c>
       <c r="D51" t="n">
-        <v>7.1757499207343</v>
+        <v>7.17574992073438</v>
       </c>
       <c r="E51" t="n">
-        <v>0.366032614803044</v>
+        <v>0.366032614803046</v>
       </c>
       <c r="F51" t="n">
-        <v>0.825590570449573</v>
+        <v>0.825590570449576</v>
       </c>
       <c r="G51" t="n">
         <v>1.86212857119853</v>
@@ -1552,22 +1552,22 @@
         <v>2010</v>
       </c>
       <c r="B52" t="n">
-        <v>2.94590518658554</v>
+        <v>2.94590518658556</v>
       </c>
       <c r="C52" t="n">
-        <v>4.78564238776219</v>
+        <v>4.78564238776223</v>
       </c>
       <c r="D52" t="n">
-        <v>7.77430759409174</v>
+        <v>7.77430759409179</v>
       </c>
       <c r="E52" t="n">
-        <v>0.305788603692498</v>
+        <v>0.305788603692497</v>
       </c>
       <c r="F52" t="n">
-        <v>0.704111869046719</v>
+        <v>0.704111869046715</v>
       </c>
       <c r="G52" t="n">
-        <v>1.62129496699954</v>
+        <v>1.62129496699953</v>
       </c>
     </row>
     <row r="53">
@@ -1581,16 +1581,16 @@
         <v>3.69005094342121</v>
       </c>
       <c r="D53" t="n">
-        <v>5.99451207331843</v>
+        <v>5.99451207331844</v>
       </c>
       <c r="E53" t="n">
-        <v>0.209231740812217</v>
+        <v>0.209231740812214</v>
       </c>
       <c r="F53" t="n">
-        <v>0.466165767554834</v>
+        <v>0.466165767554826</v>
       </c>
       <c r="G53" t="n">
-        <v>1.03861164657145</v>
+        <v>1.03861164657143</v>
       </c>
     </row>
     <row r="54">
@@ -1598,22 +1598,22 @@
         <v>2012</v>
       </c>
       <c r="B54" t="n">
-        <v>3.0141610460709</v>
+        <v>3.01416104607087</v>
       </c>
       <c r="C54" t="n">
-        <v>4.94837343175202</v>
+        <v>4.94837343175199</v>
       </c>
       <c r="D54" t="n">
-        <v>8.12378610359538</v>
+        <v>8.12378610359535</v>
       </c>
       <c r="E54" t="n">
         <v>0.234937016122346</v>
       </c>
       <c r="F54" t="n">
-        <v>0.516643710741354</v>
+        <v>0.516643710741352</v>
       </c>
       <c r="G54" t="n">
-        <v>1.13613737100327</v>
+        <v>1.13613737100326</v>
       </c>
     </row>
     <row r="55">
@@ -1621,19 +1621,19 @@
         <v>2013</v>
       </c>
       <c r="B55" t="n">
-        <v>4.35583782962734</v>
+        <v>4.35583782962737</v>
       </c>
       <c r="C55" t="n">
-        <v>7.08919085325704</v>
+        <v>7.08919085325709</v>
       </c>
       <c r="D55" t="n">
-        <v>11.5377635531034</v>
+        <v>11.5377635531035</v>
       </c>
       <c r="E55" t="n">
-        <v>0.78736554579365</v>
+        <v>0.787365545793656</v>
       </c>
       <c r="F55" t="n">
-        <v>1.73622426230133</v>
+        <v>1.73622426230134</v>
       </c>
       <c r="G55" t="n">
         <v>3.8285580377603</v>
@@ -1644,22 +1644,22 @@
         <v>2014</v>
       </c>
       <c r="B56" t="n">
-        <v>7.40013130542942</v>
+        <v>7.40013130542953</v>
       </c>
       <c r="C56" t="n">
-        <v>12.0438237637143</v>
+        <v>12.0438237637145</v>
       </c>
       <c r="D56" t="n">
-        <v>19.6015023064502</v>
+        <v>19.6015023064505</v>
       </c>
       <c r="E56" t="n">
-        <v>1.15132197727119</v>
+        <v>1.15132197727118</v>
       </c>
       <c r="F56" t="n">
-        <v>2.52953991024376</v>
+        <v>2.52953991024374</v>
       </c>
       <c r="G56" t="n">
-        <v>5.55758709017404</v>
+        <v>5.55758709017396</v>
       </c>
     </row>
     <row r="57">
@@ -1676,13 +1676,13 @@
         <v>12.3341996001315</v>
       </c>
       <c r="E57" t="n">
-        <v>0.395451984170109</v>
+        <v>0.395451984170108</v>
       </c>
       <c r="F57" t="n">
-        <v>0.869113713297548</v>
+        <v>0.869113713297545</v>
       </c>
       <c r="G57" t="n">
-        <v>1.91011469629376</v>
+        <v>1.91011469629375</v>
       </c>
     </row>
     <row r="58">
@@ -1690,22 +1690,22 @@
         <v>2016</v>
       </c>
       <c r="B58" t="n">
-        <v>6.99253347779649</v>
+        <v>6.99253347779652</v>
       </c>
       <c r="C58" t="n">
-        <v>11.4760302018363</v>
+        <v>11.4760302018364</v>
       </c>
       <c r="D58" t="n">
         <v>18.8342708135251</v>
       </c>
       <c r="E58" t="n">
-        <v>0.775551556181402</v>
+        <v>0.775551556181392</v>
       </c>
       <c r="F58" t="n">
-        <v>1.71936139859508</v>
+        <v>1.71936139859506</v>
       </c>
       <c r="G58" t="n">
-        <v>3.81174352035905</v>
+        <v>3.81174352035898</v>
       </c>
     </row>
     <row r="59">
@@ -1713,22 +1713,22 @@
         <v>2017</v>
       </c>
       <c r="B59" t="n">
-        <v>6.50977155876342</v>
+        <v>6.50977155876346</v>
       </c>
       <c r="C59" t="n">
-        <v>10.5947500334572</v>
+        <v>10.5947500334573</v>
       </c>
       <c r="D59" t="n">
-        <v>17.2431132579965</v>
+        <v>17.2431132579966</v>
       </c>
       <c r="E59" t="n">
         <v>0.525214255861756</v>
       </c>
       <c r="F59" t="n">
-        <v>1.14976886900202</v>
+        <v>1.14976886900201</v>
       </c>
       <c r="G59" t="n">
-        <v>2.51700793984948</v>
+        <v>2.51700793984946</v>
       </c>
     </row>
     <row r="60">
@@ -1736,22 +1736,22 @@
         <v>2018</v>
       </c>
       <c r="B60" t="n">
-        <v>6.15863638603538</v>
+        <v>6.15863638603549</v>
       </c>
       <c r="C60" t="n">
-        <v>10.4232105824238</v>
+        <v>10.423210582424</v>
       </c>
       <c r="D60" t="n">
-        <v>17.6408074832766</v>
+        <v>17.6408074832769</v>
       </c>
       <c r="E60" t="n">
-        <v>0.802955009598603</v>
+        <v>0.802955009598593</v>
       </c>
       <c r="F60" t="n">
-        <v>1.75778296750706</v>
+        <v>1.75778296750703</v>
       </c>
       <c r="G60" t="n">
-        <v>3.84803746651074</v>
+        <v>3.84803746651067</v>
       </c>
     </row>
     <row r="61">
@@ -1759,22 +1759,22 @@
         <v>2019</v>
       </c>
       <c r="B61" t="n">
-        <v>3.74343047679283</v>
+        <v>3.74343047679288</v>
       </c>
       <c r="C61" t="n">
-        <v>6.20021668817847</v>
+        <v>6.20021668817854</v>
       </c>
       <c r="D61" t="n">
-        <v>10.2693738320212</v>
+        <v>10.2693738320213</v>
       </c>
       <c r="E61" t="n">
-        <v>0.625926784058276</v>
+        <v>0.625926784058269</v>
       </c>
       <c r="F61" t="n">
-        <v>1.37520764166998</v>
+        <v>1.37520764166996</v>
       </c>
       <c r="G61" t="n">
-        <v>3.02143334631841</v>
+        <v>3.02143334631836</v>
       </c>
     </row>
     <row r="62">
@@ -1782,22 +1782,22 @@
         <v>2020</v>
       </c>
       <c r="B62" t="n">
-        <v>4.28600672629676</v>
+        <v>4.28600672629682</v>
       </c>
       <c r="C62" t="n">
-        <v>7.09888178631213</v>
+        <v>7.09888178631222</v>
       </c>
       <c r="D62" t="n">
-        <v>11.7578263017744</v>
+        <v>11.7578263017746</v>
       </c>
       <c r="E62" t="n">
-        <v>0.385351439940468</v>
+        <v>0.385351439940477</v>
       </c>
       <c r="F62" t="n">
-        <v>0.853582705751228</v>
+        <v>0.853582705751246</v>
       </c>
       <c r="G62" t="n">
-        <v>1.8907505202787</v>
+        <v>1.89075052027874</v>
       </c>
     </row>
     <row r="63">
@@ -1805,22 +1805,22 @@
         <v>2021</v>
       </c>
       <c r="B63" t="n">
-        <v>3.19600351350295</v>
+        <v>3.1960035135031</v>
       </c>
       <c r="C63" t="n">
-        <v>5.40042664380569</v>
+        <v>5.40042664380593</v>
       </c>
       <c r="D63" t="n">
-        <v>9.12533663117311</v>
+        <v>9.12533663117347</v>
       </c>
       <c r="E63" t="n">
-        <v>0.353458128608874</v>
+        <v>0.353458128608857</v>
       </c>
       <c r="F63" t="n">
-        <v>0.597253628522114</v>
+        <v>0.597253628522083</v>
       </c>
       <c r="G63" t="n">
-        <v>1.00920552651247</v>
+        <v>1.00920552651242</v>
       </c>
     </row>
   </sheetData>
@@ -1856,13 +1856,13 @@
         <v>1950</v>
       </c>
       <c r="B2" t="n">
-        <v>46.531732227211</v>
+        <v>45.7224901412603</v>
       </c>
       <c r="C2" t="n">
-        <v>182.258038385847</v>
+        <v>180.881097711606</v>
       </c>
       <c r="D2" t="n">
-        <v>713.87827115603</v>
+        <v>715.577200810214</v>
       </c>
     </row>
     <row r="3">
@@ -1870,13 +1870,13 @@
         <v>1951</v>
       </c>
       <c r="B3" t="n">
-        <v>73.4977296654705</v>
+        <v>73.3957637828496</v>
       </c>
       <c r="C3" t="n">
-        <v>262.532308509005</v>
+        <v>264.581218631341</v>
       </c>
       <c r="D3" t="n">
-        <v>937.759755638378</v>
+        <v>953.7774068209</v>
       </c>
     </row>
     <row r="4">
@@ -1884,13 +1884,13 @@
         <v>1952</v>
       </c>
       <c r="B4" t="n">
-        <v>70.6231974853068</v>
+        <v>70.0586099573685</v>
       </c>
       <c r="C4" t="n">
-        <v>252.264541428623</v>
+        <v>252.551256949656</v>
       </c>
       <c r="D4" t="n">
-        <v>901.083512615427</v>
+        <v>910.411117572317</v>
       </c>
     </row>
     <row r="5">
@@ -1898,13 +1898,13 @@
         <v>1953</v>
       </c>
       <c r="B5" t="n">
-        <v>112.110513279753</v>
+        <v>111.202207404916</v>
       </c>
       <c r="C5" t="n">
-        <v>400.456340534969</v>
+        <v>400.868034247001</v>
       </c>
       <c r="D5" t="n">
-        <v>1430.42142956294</v>
+        <v>1445.07186171154</v>
       </c>
     </row>
     <row r="6">
@@ -1912,13 +1912,13 @@
         <v>1954</v>
       </c>
       <c r="B6" t="n">
-        <v>55.1589601037605</v>
+        <v>54.5339845920588</v>
       </c>
       <c r="C6" t="n">
-        <v>197.026618331034</v>
+        <v>196.587205535169</v>
       </c>
       <c r="D6" t="n">
-        <v>703.77484016992</v>
+        <v>708.668725918747</v>
       </c>
     </row>
     <row r="7">
@@ -1926,13 +1926,13 @@
         <v>1955</v>
       </c>
       <c r="B7" t="n">
-        <v>85.1734368371371</v>
+        <v>84.4439627675028</v>
       </c>
       <c r="C7" t="n">
-        <v>304.237683235603</v>
+        <v>304.408393939301</v>
       </c>
       <c r="D7" t="n">
-        <v>1086.73045655719</v>
+        <v>1097.3486708083</v>
       </c>
     </row>
     <row r="8">
@@ -1940,13 +1940,13 @@
         <v>1956</v>
       </c>
       <c r="B8" t="n">
-        <v>38.000254565784</v>
+        <v>37.3958941248674</v>
       </c>
       <c r="C8" t="n">
-        <v>135.736091447897</v>
+        <v>134.806843466327</v>
       </c>
       <c r="D8" t="n">
-        <v>484.846397269701</v>
+        <v>485.959367214869</v>
       </c>
     </row>
     <row r="9">
@@ -1954,13 +1954,13 @@
         <v>1957</v>
       </c>
       <c r="B9" t="n">
-        <v>43.9354281582806</v>
+        <v>43.4663792569039</v>
       </c>
       <c r="C9" t="n">
-        <v>156.936403780426</v>
+        <v>156.690073112517</v>
       </c>
       <c r="D9" t="n">
-        <v>560.573456637434</v>
+        <v>564.845276550297</v>
       </c>
     </row>
     <row r="10">
@@ -1968,13 +1968,13 @@
         <v>1958</v>
       </c>
       <c r="B10" t="n">
-        <v>43.1034155482698</v>
+        <v>42.2949558874122</v>
       </c>
       <c r="C10" t="n">
-        <v>153.964472644471</v>
+        <v>152.467259605864</v>
       </c>
       <c r="D10" t="n">
-        <v>549.957782583231</v>
+        <v>549.622638538807</v>
       </c>
     </row>
     <row r="11">
@@ -1982,13 +1982,13 @@
         <v>1959</v>
       </c>
       <c r="B11" t="n">
-        <v>93.8598832088638</v>
+        <v>92.7859969699884</v>
       </c>
       <c r="C11" t="n">
-        <v>335.265482721232</v>
+        <v>334.480232713102</v>
       </c>
       <c r="D11" t="n">
-        <v>1197.56108852355</v>
+        <v>1205.7533434921</v>
       </c>
     </row>
     <row r="12">
@@ -1996,13 +1996,13 @@
         <v>1960</v>
       </c>
       <c r="B12" t="n">
-        <v>49.8400383065583</v>
+        <v>49.1864749783822</v>
       </c>
       <c r="C12" t="n">
-        <v>166.84123284993</v>
+        <v>166.070428984608</v>
       </c>
       <c r="D12" t="n">
-        <v>558.506733234626</v>
+        <v>560.710792860297</v>
       </c>
     </row>
     <row r="13">
@@ -2010,13 +2010,13 @@
         <v>1961</v>
       </c>
       <c r="B13" t="n">
-        <v>54.1250421093407</v>
+        <v>53.642066421168</v>
       </c>
       <c r="C13" t="n">
-        <v>181.18542963456</v>
+        <v>181.114035638852</v>
       </c>
       <c r="D13" t="n">
-        <v>606.524422568437</v>
+        <v>611.503174539281</v>
       </c>
     </row>
     <row r="14">
@@ -2024,13 +2024,13 @@
         <v>1962</v>
       </c>
       <c r="B14" t="n">
-        <v>53.2111249389923</v>
+        <v>52.7956852415999</v>
       </c>
       <c r="C14" t="n">
-        <v>178.126060649213</v>
+        <v>178.256362149604</v>
       </c>
       <c r="D14" t="n">
-        <v>596.283080254079</v>
+        <v>601.854687582949</v>
       </c>
     </row>
     <row r="15">
@@ -2038,13 +2038,13 @@
         <v>1963</v>
       </c>
       <c r="B15" t="n">
-        <v>44.9764341920806</v>
+        <v>44.4986252455557</v>
       </c>
       <c r="C15" t="n">
-        <v>150.56015173273</v>
+        <v>150.242638591252</v>
       </c>
       <c r="D15" t="n">
-        <v>504.005257352615</v>
+        <v>507.270737608146</v>
       </c>
     </row>
     <row r="16">
@@ -2052,13 +2052,13 @@
         <v>1964</v>
       </c>
       <c r="B16" t="n">
-        <v>18.1761809024229</v>
+        <v>18.0181899712968</v>
       </c>
       <c r="C16" t="n">
-        <v>60.8453872288565</v>
+        <v>60.8355963580341</v>
       </c>
       <c r="D16" t="n">
-        <v>203.68201477</v>
+        <v>205.40186279162</v>
       </c>
     </row>
     <row r="17">
@@ -2066,13 +2066,13 @@
         <v>1965</v>
       </c>
       <c r="B17" t="n">
-        <v>34.2017594933329</v>
+        <v>33.9463725752482</v>
       </c>
       <c r="C17" t="n">
-        <v>114.491559665466</v>
+        <v>114.614610185433</v>
       </c>
       <c r="D17" t="n">
-        <v>383.264411796888</v>
+        <v>386.978279898369</v>
       </c>
     </row>
     <row r="18">
@@ -2080,13 +2080,13 @@
         <v>1966</v>
       </c>
       <c r="B18" t="n">
-        <v>46.7201067170363</v>
+        <v>46.5354535832553</v>
       </c>
       <c r="C18" t="n">
-        <v>156.397155146745</v>
+        <v>157.119670457399</v>
       </c>
       <c r="D18" t="n">
-        <v>523.544825917015</v>
+        <v>530.489958596311</v>
       </c>
     </row>
     <row r="19">
@@ -2094,13 +2094,13 @@
         <v>1967</v>
       </c>
       <c r="B19" t="n">
-        <v>34.7956217496718</v>
+        <v>34.7461856971558</v>
       </c>
       <c r="C19" t="n">
-        <v>110.898254560505</v>
+        <v>111.645301750541</v>
       </c>
       <c r="D19" t="n">
-        <v>353.44742373177</v>
+        <v>358.735013725251</v>
       </c>
     </row>
     <row r="20">
@@ -2108,13 +2108,13 @@
         <v>1968</v>
       </c>
       <c r="B20" t="n">
-        <v>54.4378346552625</v>
+        <v>53.7849342606197</v>
       </c>
       <c r="C20" t="n">
-        <v>173.500588342814</v>
+        <v>172.81998281761</v>
       </c>
       <c r="D20" t="n">
-        <v>552.969352031207</v>
+        <v>555.299488075174</v>
       </c>
     </row>
     <row r="21">
@@ -2122,13 +2122,13 @@
         <v>1969</v>
       </c>
       <c r="B21" t="n">
-        <v>36.3670346151812</v>
+        <v>36.011954855364</v>
       </c>
       <c r="C21" t="n">
-        <v>115.906555467805</v>
+        <v>115.712429602973</v>
       </c>
       <c r="D21" t="n">
-        <v>369.409541981277</v>
+        <v>371.803375251336</v>
       </c>
     </row>
     <row r="22">
@@ -2136,13 +2136,13 @@
         <v>1970</v>
       </c>
       <c r="B22" t="n">
-        <v>18.5959764299131</v>
+        <v>18.4669657757319</v>
       </c>
       <c r="C22" t="n">
-        <v>59.2678395794181</v>
+        <v>59.3374474084295</v>
       </c>
       <c r="D22" t="n">
-        <v>188.894453681993</v>
+        <v>190.66113554914</v>
       </c>
     </row>
     <row r="23">
@@ -2150,13 +2150,13 @@
         <v>1971</v>
       </c>
       <c r="B23" t="n">
-        <v>19.472259867876</v>
+        <v>19.2422225806657</v>
       </c>
       <c r="C23" t="n">
-        <v>62.0606709439355</v>
+        <v>61.8284770908068</v>
       </c>
       <c r="D23" t="n">
-        <v>197.795577100192</v>
+        <v>198.665230242658</v>
       </c>
     </row>
     <row r="24">
@@ -2164,13 +2164,13 @@
         <v>1972</v>
       </c>
       <c r="B24" t="n">
-        <v>32.4010824784941</v>
+        <v>31.8743159426091</v>
       </c>
       <c r="C24" t="n">
-        <v>108.463731771908</v>
+        <v>107.618635499016</v>
       </c>
       <c r="D24" t="n">
-        <v>363.086051760677</v>
+        <v>363.357467106856</v>
       </c>
     </row>
     <row r="25">
@@ -2178,13 +2178,13 @@
         <v>1973</v>
       </c>
       <c r="B25" t="n">
-        <v>42.3126229891255</v>
+        <v>41.7831816727659</v>
       </c>
       <c r="C25" t="n">
-        <v>134.855933000106</v>
+        <v>134.256345908365</v>
       </c>
       <c r="D25" t="n">
-        <v>429.803717675523</v>
+        <v>431.388077572252</v>
       </c>
     </row>
     <row r="26">
@@ -2192,13 +2192,13 @@
         <v>1974</v>
       </c>
       <c r="B26" t="n">
-        <v>20.3565313295165</v>
+        <v>20.1709119967824</v>
       </c>
       <c r="C26" t="n">
-        <v>64.8789611977816</v>
+        <v>64.8125113959987</v>
       </c>
       <c r="D26" t="n">
-        <v>206.777841370248</v>
+        <v>208.253431184794</v>
       </c>
     </row>
     <row r="27">
@@ -2206,13 +2206,13 @@
         <v>1975</v>
       </c>
       <c r="B27" t="n">
-        <v>38.3650792781955</v>
+        <v>38.0074151778596</v>
       </c>
       <c r="C27" t="n">
-        <v>122.274588413338</v>
+        <v>122.124177119033</v>
       </c>
       <c r="D27" t="n">
-        <v>389.705306308295</v>
+        <v>392.405391611289</v>
       </c>
     </row>
     <row r="28">
@@ -2220,13 +2220,13 @@
         <v>1976</v>
       </c>
       <c r="B28" t="n">
-        <v>11.7448067079925</v>
+        <v>11.670140657017</v>
       </c>
       <c r="C28" t="n">
-        <v>37.4322543634146</v>
+        <v>37.4981123533968</v>
       </c>
       <c r="D28" t="n">
-        <v>119.301551874316</v>
+        <v>120.487702024612</v>
       </c>
     </row>
     <row r="29">
@@ -2234,13 +2234,13 @@
         <v>1977</v>
       </c>
       <c r="B29" t="n">
-        <v>24.5350972067765</v>
+        <v>24.5090169640009</v>
       </c>
       <c r="C29" t="n">
-        <v>78.1966040233066</v>
+        <v>78.751567680104</v>
       </c>
       <c r="D29" t="n">
-        <v>249.222932733641</v>
+        <v>253.041948650298</v>
       </c>
     </row>
     <row r="30">
@@ -2248,13 +2248,13 @@
         <v>1978</v>
       </c>
       <c r="B30" t="n">
-        <v>21.848540019739</v>
+        <v>21.8238828891053</v>
       </c>
       <c r="C30" t="n">
-        <v>69.6341904828084</v>
+        <v>70.1237831328949</v>
       </c>
       <c r="D30" t="n">
-        <v>221.933386844856</v>
+        <v>225.319434944552</v>
       </c>
     </row>
     <row r="31">
@@ -2262,13 +2262,13 @@
         <v>1979</v>
       </c>
       <c r="B31" t="n">
-        <v>18.309876391009</v>
+        <v>18.1805546856222</v>
       </c>
       <c r="C31" t="n">
-        <v>58.3560008667086</v>
+        <v>58.4171607082239</v>
       </c>
       <c r="D31" t="n">
-        <v>185.988302948212</v>
+        <v>187.704100574513</v>
       </c>
     </row>
     <row r="32">
@@ -2276,13 +2276,13 @@
         <v>1980</v>
       </c>
       <c r="B32" t="n">
-        <v>32.1988759647938</v>
+        <v>31.9159464048355</v>
       </c>
       <c r="C32" t="n">
-        <v>98.8138091455523</v>
+        <v>98.7089338540855</v>
       </c>
       <c r="D32" t="n">
-        <v>303.245643994833</v>
+        <v>305.284809637793</v>
       </c>
     </row>
     <row r="33">
@@ -2290,13 +2290,13 @@
         <v>1981</v>
       </c>
       <c r="B33" t="n">
-        <v>13.396744670465</v>
+        <v>13.3689335539022</v>
       </c>
       <c r="C33" t="n">
-        <v>41.1127199746487</v>
+        <v>41.3471423072653</v>
       </c>
       <c r="D33" t="n">
-        <v>126.169139241736</v>
+        <v>127.877528157677</v>
       </c>
     </row>
     <row r="34">
@@ -2304,13 +2304,13 @@
         <v>1982</v>
       </c>
       <c r="B34" t="n">
-        <v>16.8981370490142</v>
+        <v>16.8348986723715</v>
       </c>
       <c r="C34" t="n">
-        <v>51.8579993631578</v>
+        <v>52.0666026447386</v>
       </c>
       <c r="D34" t="n">
-        <v>159.144886217274</v>
+        <v>161.030438241611</v>
       </c>
     </row>
     <row r="35">
@@ -2318,13 +2318,13 @@
         <v>1983</v>
       </c>
       <c r="B35" t="n">
-        <v>15.2557672660441</v>
+        <v>15.1705952454379</v>
       </c>
       <c r="C35" t="n">
-        <v>46.8177981319636</v>
+        <v>46.9192817789087</v>
       </c>
       <c r="D35" t="n">
-        <v>143.677219486953</v>
+        <v>145.110917998464</v>
       </c>
     </row>
     <row r="36">
@@ -2332,13 +2332,13 @@
         <v>1984</v>
       </c>
       <c r="B36" t="n">
-        <v>11.4046275170595</v>
+        <v>11.3893766708656</v>
       </c>
       <c r="C36" t="n">
-        <v>34.9991933904467</v>
+        <v>35.2248125179642</v>
       </c>
       <c r="D36" t="n">
-        <v>107.407588380205</v>
+        <v>108.942521858962</v>
       </c>
     </row>
     <row r="37">
@@ -2346,13 +2346,13 @@
         <v>1985</v>
       </c>
       <c r="B37" t="n">
-        <v>21.3753006431456</v>
+        <v>21.3505031347332</v>
       </c>
       <c r="C37" t="n">
-        <v>65.5482706719883</v>
+        <v>65.9818665513102</v>
       </c>
       <c r="D37" t="n">
-        <v>201.006566401957</v>
+        <v>203.911199943219</v>
       </c>
     </row>
     <row r="38">
@@ -2360,13 +2360,13 @@
         <v>1986</v>
       </c>
       <c r="B38" t="n">
-        <v>16.4991496730305</v>
+        <v>16.6157503164053</v>
       </c>
       <c r="C38" t="n">
-        <v>49.0766402084606</v>
+        <v>49.7950416385881</v>
       </c>
       <c r="D38" t="n">
-        <v>145.978226871149</v>
+        <v>149.228661033777</v>
       </c>
     </row>
     <row r="39">
@@ -2374,13 +2374,13 @@
         <v>1987</v>
       </c>
       <c r="B39" t="n">
-        <v>15.9299872994742</v>
+        <v>15.8429163143624</v>
       </c>
       <c r="C39" t="n">
-        <v>47.383669505075</v>
+        <v>47.4789679989015</v>
       </c>
       <c r="D39" t="n">
-        <v>140.942493773381</v>
+        <v>142.287717583733</v>
       </c>
     </row>
     <row r="40">
@@ -2388,13 +2388,13 @@
         <v>1988</v>
       </c>
       <c r="B40" t="n">
-        <v>20.5970786084154</v>
+        <v>20.5622735005735</v>
       </c>
       <c r="C40" t="n">
-        <v>61.2659098343043</v>
+        <v>61.6222105922093</v>
       </c>
       <c r="D40" t="n">
-        <v>182.23514990575</v>
+        <v>184.67300506263</v>
       </c>
     </row>
     <row r="41">
@@ -2402,13 +2402,13 @@
         <v>1989</v>
       </c>
       <c r="B41" t="n">
-        <v>11.3987502262883</v>
+        <v>11.4207793349117</v>
       </c>
       <c r="C41" t="n">
-        <v>36.3195452104713</v>
+        <v>36.685262063555</v>
       </c>
       <c r="D41" t="n">
-        <v>115.724034486981</v>
+        <v>117.838582920323</v>
       </c>
     </row>
     <row r="42">
@@ -2416,13 +2416,13 @@
         <v>1990</v>
       </c>
       <c r="B42" t="n">
-        <v>10.4166065366395</v>
+        <v>10.4359081186199</v>
       </c>
       <c r="C42" t="n">
-        <v>31.9498185649232</v>
+        <v>32.2583807644469</v>
       </c>
       <c r="D42" t="n">
-        <v>97.9964926908751</v>
+        <v>99.7137113240184</v>
       </c>
     </row>
     <row r="43">
@@ -2430,13 +2430,13 @@
         <v>1991</v>
       </c>
       <c r="B43" t="n">
-        <v>11.7765347142923</v>
+        <v>11.7329788031554</v>
       </c>
       <c r="C43" t="n">
-        <v>37.5232702258887</v>
+        <v>37.6880937419168</v>
       </c>
       <c r="D43" t="n">
-        <v>119.559432600855</v>
+        <v>121.05982919849</v>
       </c>
     </row>
     <row r="44">
@@ -2444,13 +2444,13 @@
         <v>1992</v>
       </c>
       <c r="B44" t="n">
-        <v>5.97309835744899</v>
+        <v>8.05714639567</v>
       </c>
       <c r="C44" t="n">
-        <v>17.7516880582373</v>
+        <v>23.5094960525035</v>
       </c>
       <c r="D44" t="n">
-        <v>52.7569462377892</v>
+        <v>68.5970413718315</v>
       </c>
     </row>
     <row r="45">
@@ -2458,13 +2458,13 @@
         <v>1993</v>
       </c>
       <c r="B45" t="n">
-        <v>4.77183652506027</v>
+        <v>4.76472293595244</v>
       </c>
       <c r="C45" t="n">
-        <v>14.1816103450119</v>
+        <v>14.2667989470708</v>
       </c>
       <c r="D45" t="n">
-        <v>42.1468905989418</v>
+        <v>42.7184444787564</v>
       </c>
     </row>
     <row r="46">
@@ -2472,13 +2472,13 @@
         <v>1994</v>
       </c>
       <c r="B46" t="n">
-        <v>18.6875481885444</v>
+        <v>18.7486801671194</v>
       </c>
       <c r="C46" t="n">
-        <v>55.5382660998057</v>
+        <v>56.1383429976415</v>
       </c>
       <c r="D46" t="n">
-        <v>165.056377126222</v>
+        <v>168.092555125444</v>
       </c>
     </row>
     <row r="47">
@@ -2486,13 +2486,13 @@
         <v>1995</v>
       </c>
       <c r="B47" t="n">
-        <v>4.33067255431814</v>
+        <v>6.08563038612497</v>
       </c>
       <c r="C47" t="n">
-        <v>13.2670965200305</v>
+        <v>18.2092400675214</v>
       </c>
       <c r="D47" t="n">
-        <v>40.6439987932818</v>
+        <v>54.4851400427815</v>
       </c>
     </row>
     <row r="48">
@@ -2500,13 +2500,13 @@
         <v>1996</v>
       </c>
       <c r="B48" t="n">
-        <v>3.39444651202076</v>
+        <v>3.37010856066951</v>
       </c>
       <c r="C48" t="n">
-        <v>10.0880903018477</v>
+        <v>10.0909668644277</v>
       </c>
       <c r="D48" t="n">
-        <v>29.9811959262978</v>
+        <v>30.2149353428391</v>
       </c>
     </row>
     <row r="49">
@@ -2514,13 +2514,13 @@
         <v>1997</v>
       </c>
       <c r="B49" t="n">
-        <v>7.56231793328809</v>
+        <v>8.13427446199931</v>
       </c>
       <c r="C49" t="n">
-        <v>21.4462174211501</v>
+        <v>22.8080675852127</v>
       </c>
       <c r="D49" t="n">
-        <v>60.8200085916331</v>
+        <v>63.9525933630432</v>
       </c>
     </row>
     <row r="50">
@@ -2528,13 +2528,13 @@
         <v>1998</v>
       </c>
       <c r="B50" t="n">
-        <v>6.04240535633368</v>
+        <v>6.85251656427667</v>
       </c>
       <c r="C50" t="n">
-        <v>17.495215016052</v>
+        <v>19.5588853350915</v>
       </c>
       <c r="D50" t="n">
-        <v>50.6557455859951</v>
+        <v>55.8262051558626</v>
       </c>
     </row>
     <row r="51">
@@ -2542,13 +2542,13 @@
         <v>1999</v>
       </c>
       <c r="B51" t="n">
-        <v>7.40366257955159</v>
+        <v>8.85756489777383</v>
       </c>
       <c r="C51" t="n">
-        <v>21.4366069631162</v>
+        <v>25.28182085496</v>
       </c>
       <c r="D51" t="n">
-        <v>62.0676743643486</v>
+        <v>72.1609689704825</v>
       </c>
     </row>
     <row r="52">
@@ -2556,13 +2556,13 @@
         <v>2000</v>
       </c>
       <c r="B52" t="n">
-        <v>5.99084489839571</v>
+        <v>7.09849366121194</v>
       </c>
       <c r="C52" t="n">
-        <v>17.7860091573974</v>
+        <v>20.694087322464</v>
       </c>
       <c r="D52" t="n">
-        <v>52.8042583495589</v>
+        <v>60.3290318409117</v>
       </c>
     </row>
     <row r="53">
@@ -2570,13 +2570,13 @@
         <v>2001</v>
       </c>
       <c r="B53" t="n">
-        <v>6.21143303938536</v>
+        <v>6.99844302439806</v>
       </c>
       <c r="C53" t="n">
-        <v>17.9846187359721</v>
+        <v>19.9753978490121</v>
       </c>
       <c r="D53" t="n">
-        <v>52.072767914807</v>
+        <v>57.0150414649746</v>
       </c>
     </row>
     <row r="54">
@@ -2584,13 +2584,13 @@
         <v>2002</v>
       </c>
       <c r="B54" t="n">
-        <v>13.271823334022</v>
+        <v>13.0468211094684</v>
       </c>
       <c r="C54" t="n">
-        <v>37.6379849812493</v>
+        <v>36.5825838588429</v>
       </c>
       <c r="D54" t="n">
-        <v>106.738756069581</v>
+        <v>102.575595277999</v>
       </c>
     </row>
     <row r="55">
@@ -2598,13 +2598,13 @@
         <v>2003</v>
       </c>
       <c r="B55" t="n">
-        <v>8.55198221406132</v>
+        <v>8.58228130437359</v>
       </c>
       <c r="C55" t="n">
-        <v>23.8020644130431</v>
+        <v>23.6754086700139</v>
       </c>
       <c r="D55" t="n">
-        <v>66.2464275698727</v>
+        <v>65.3118857111481</v>
       </c>
     </row>
     <row r="56">
@@ -2612,13 +2612,13 @@
         <v>2004</v>
       </c>
       <c r="B56" t="n">
-        <v>9.25524512321405</v>
+        <v>8.59471511644231</v>
       </c>
       <c r="C56" t="n">
-        <v>25.7594011618771</v>
+        <v>23.7097090584087</v>
       </c>
       <c r="D56" t="n">
-        <v>71.6941301267326</v>
+        <v>65.4065080713327</v>
       </c>
     </row>
     <row r="57">
@@ -2626,13 +2626,13 @@
         <v>2005</v>
       </c>
       <c r="B57" t="n">
-        <v>4.75367878457447</v>
+        <v>4.61524331634036</v>
       </c>
       <c r="C57" t="n">
-        <v>12.8334360670918</v>
+        <v>12.3944511632854</v>
       </c>
       <c r="D57" t="n">
-        <v>34.6462368939545</v>
+        <v>33.2858766286849</v>
       </c>
     </row>
     <row r="58">
@@ -2640,13 +2640,13 @@
         <v>2006</v>
       </c>
       <c r="B58" t="n">
-        <v>6.32970850448039</v>
+        <v>5.97326549794511</v>
       </c>
       <c r="C58" t="n">
-        <v>17.088220112636</v>
+        <v>16.0414830649329</v>
       </c>
       <c r="D58" t="n">
-        <v>46.1328142380021</v>
+        <v>43.0801508841441</v>
       </c>
     </row>
     <row r="59">
@@ -2654,13 +2654,13 @@
         <v>2007</v>
       </c>
       <c r="B59" t="n">
-        <v>7.4116434440377</v>
+        <v>7.095623840711</v>
       </c>
       <c r="C59" t="n">
-        <v>20.2746217685521</v>
+        <v>19.2794429487923</v>
       </c>
       <c r="D59" t="n">
-        <v>55.4614224175242</v>
+        <v>52.383966337552</v>
       </c>
     </row>
     <row r="60">
@@ -2668,13 +2668,13 @@
         <v>2008</v>
       </c>
       <c r="B60" t="n">
-        <v>5.12750830009762</v>
+        <v>5.62312242993416</v>
       </c>
       <c r="C60" t="n">
-        <v>13.6692803116259</v>
+        <v>14.9320397692631</v>
       </c>
       <c r="D60" t="n">
-        <v>36.4405503223168</v>
+        <v>39.6516018367156</v>
       </c>
     </row>
     <row r="61">
@@ -2682,13 +2682,13 @@
         <v>2009</v>
       </c>
       <c r="B61" t="n">
-        <v>3.04705917319055</v>
+        <v>3.02744034055668</v>
       </c>
       <c r="C61" t="n">
-        <v>8.22395170390206</v>
+        <v>8.12841818974935</v>
       </c>
       <c r="D61" t="n">
-        <v>22.1962809988017</v>
+        <v>21.8241071119832</v>
       </c>
     </row>
     <row r="62">
@@ -2696,13 +2696,13 @@
         <v>2010</v>
       </c>
       <c r="B62" t="n">
-        <v>4.56799002603962</v>
+        <v>4.34062337378182</v>
       </c>
       <c r="C62" t="n">
-        <v>12.3194702886673</v>
+        <v>11.6461754900028</v>
       </c>
       <c r="D62" t="n">
-        <v>33.2245358085729</v>
+        <v>31.2474480884918</v>
       </c>
     </row>
     <row r="63">
@@ -2710,13 +2710,13 @@
         <v>2011</v>
       </c>
       <c r="B63" t="n">
-        <v>10.1901213058427</v>
+        <v>9.02913628662229</v>
       </c>
       <c r="C63" t="n">
-        <v>27.4738887284908</v>
+        <v>24.2192673207318</v>
       </c>
       <c r="D63" t="n">
-        <v>74.0731674541211</v>
+        <v>64.9644540665693</v>
       </c>
     </row>
     <row r="64">
@@ -2724,13 +2724,13 @@
         <v>2012</v>
       </c>
       <c r="B64" t="n">
-        <v>5.46927262308776</v>
+        <v>5.10663784109984</v>
       </c>
       <c r="C64" t="n">
-        <v>13.6167217836676</v>
+        <v>12.7205076602804</v>
       </c>
       <c r="D64" t="n">
-        <v>33.9012378631674</v>
+        <v>31.6864677249959</v>
       </c>
     </row>
     <row r="65">
@@ -2738,13 +2738,13 @@
         <v>2013</v>
       </c>
       <c r="B65" t="n">
-        <v>5.68249530510507</v>
+        <v>5.18983514979478</v>
       </c>
       <c r="C65" t="n">
-        <v>14.0624043931155</v>
+        <v>12.8565670392418</v>
       </c>
       <c r="D65" t="n">
-        <v>34.800066994839</v>
+        <v>31.8490493943831</v>
       </c>
     </row>
     <row r="66">
@@ -2752,13 +2752,13 @@
         <v>2014</v>
       </c>
       <c r="B66" t="n">
-        <v>11.1561288483486</v>
+        <v>10.4641425996353</v>
       </c>
       <c r="C66" t="n">
-        <v>28.5834317113192</v>
+        <v>26.804667354926</v>
       </c>
       <c r="D66" t="n">
-        <v>73.2344148675361</v>
+        <v>68.6621178149158</v>
       </c>
     </row>
     <row r="67">
@@ -2766,13 +2766,13 @@
         <v>2015</v>
       </c>
       <c r="B67" t="n">
-        <v>4.60684262132756</v>
+        <v>4.25342750758008</v>
       </c>
       <c r="C67" t="n">
-        <v>11.3360824976711</v>
+        <v>10.4821388511505</v>
       </c>
       <c r="D67" t="n">
-        <v>27.894759373606</v>
+        <v>25.8321635196528</v>
       </c>
     </row>
     <row r="68">
@@ -2780,13 +2780,13 @@
         <v>2016</v>
       </c>
       <c r="B68" t="n">
-        <v>6.17868661975696</v>
+        <v>5.60935732822623</v>
       </c>
       <c r="C68" t="n">
-        <v>15.3797907590597</v>
+        <v>13.9701062483553</v>
       </c>
       <c r="D68" t="n">
-        <v>38.2828873430972</v>
+        <v>34.7925541502364</v>
       </c>
     </row>
     <row r="69">
@@ -2794,13 +2794,13 @@
         <v>2017</v>
       </c>
       <c r="B69" t="n">
-        <v>7.25065187107438</v>
+        <v>6.50532517202073</v>
       </c>
       <c r="C69" t="n">
-        <v>18.037045371303</v>
+        <v>16.1922688427523</v>
       </c>
       <c r="D69" t="n">
-        <v>44.869759507325</v>
+        <v>40.3038377548963</v>
       </c>
     </row>
     <row r="70">
@@ -2808,13 +2808,13 @@
         <v>2018</v>
       </c>
       <c r="B70" t="n">
-        <v>7.20123525782998</v>
+        <v>6.643186805687</v>
       </c>
       <c r="C70" t="n">
-        <v>18.03127974589</v>
+        <v>16.633545353766</v>
       </c>
       <c r="D70" t="n">
-        <v>45.1487887332982</v>
+        <v>41.6479077178648</v>
       </c>
     </row>
     <row r="71">
@@ -2822,13 +2822,13 @@
         <v>2019</v>
       </c>
       <c r="B71" t="n">
-        <v>6.03333823700205</v>
+        <v>5.54100415005655</v>
       </c>
       <c r="C71" t="n">
-        <v>15.1094910633054</v>
+        <v>13.8759878357393</v>
       </c>
       <c r="D71" t="n">
-        <v>37.83920463666</v>
+        <v>34.7487627158012</v>
       </c>
     </row>
     <row r="72">
@@ -2836,13 +2836,13 @@
         <v>2020</v>
       </c>
       <c r="B72" t="n">
-        <v>6.41228906478957</v>
+        <v>6.15771804483593</v>
       </c>
       <c r="C72" t="n">
-        <v>16.6593578482956</v>
+        <v>16.1117107358708</v>
       </c>
       <c r="D72" t="n">
-        <v>43.2816114671954</v>
+        <v>42.1563996510158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>